<commit_message>
Removed random number generation for nameNumber to keep test data consistent
</commit_message>
<xml_diff>
--- a/models/mock-data/FakeUsers.xlsx
+++ b/models/mock-data/FakeUsers.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1012" uniqueCount="691">
   <si>
     <t>Spot</t>
   </si>
@@ -1422,6 +1422,681 @@
   </si>
   <si>
     <t>Noella Krebsbach</t>
+  </si>
+  <si>
+    <t>Name.Number</t>
+  </si>
+  <si>
+    <t>Koop.960</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mcbain.358</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Huot.633</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bezanson.660</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cavalieri.839</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bass.111</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Isaacs.442</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Wolanski.136</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Clendening.100</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ashbaugh.213</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Pinder.964</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Depalma.763</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Imel.715</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Shambaugh.40</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Albritton.668</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Slocum.139</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Maysonet.58</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Maag.400</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Laguardia.605</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Rosso.903</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Jeanbaptiste.831</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Siegrist.361</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Balas.71</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Costello.760</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Poulter.816</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Whitmire.337</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Politte.833</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Hartshorn.948</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Iser.962</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tinajero.70</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Caplan.540</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Seppala.173</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Statler.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Dartez.850</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Backman.359</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Norgard.983</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ingwersen.694</t>
+  </si>
+  <si>
+    <t>Torgersen.942</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Landey.624</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Herbst.123</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mings.349</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gandara.979</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Caffrey.986</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Branning.888</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Beland.117</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mariscal.729</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Medel.318</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Normandin.386</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Breuer.491</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Liberto.857</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Godfrey.949</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mikkelson.973</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Fleagle.381</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Darlington.481</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Hosein.882</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Juarbe.11</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Deslauriers.767</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Horney.105</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Nivens.576</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Enfinger.107</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mccraw.316</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Eggleton.598</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Wymore.153</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Dayton.843</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Petti.427</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Guercio.396</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Vasconcellos.50</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Heal.856</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Hornick.940</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Franson.807</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mahar.143</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Denney.753</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Saffell.584</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Maze.620</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Pawlowicz.398</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lahr.942</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lerman.315</t>
+  </si>
+  <si>
+    <t>Provencal.801</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Delagarza.200</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thompkins.432</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mccroskey.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Wynter.419</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cliff.333</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Storck.591</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Meikle.556</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lightfoot.559</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ester.921</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mungo.80</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Michalski.556</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lunceford.641</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Siebert.643</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Call.939</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Robin.11</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Roddy.883</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Pangle.362</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Hastings.286</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Seller.821</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mumaw.240</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Popham.241</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Grieve.693</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Camacho.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ehrenberg.441</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Champine.202</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Wells.55</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Spicer.41</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Shirley.671</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Eddington.306</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Morrisette.605</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Whiting.851</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Nordahl.9</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mullet.321</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Rand.840</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mathisen.218</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Garten.560</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tyree.611</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Peppler.143</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Paulson.371</t>
+  </si>
+  <si>
+    <t>Mercer.633</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lickteig.332</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Haddon.17</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mauger.736</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Berge.171</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Willcutt.973</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gaver.489</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ruyle.883</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Heeter.44</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Fitzwater.145</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Aquilino.382</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Palomino.241</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Dunson.706</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Hager.952</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bussell.732</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Reese.274</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Borjas.930</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cady.595</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Okada.299</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Debow.528</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Calderone.593</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Berrier.471</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Parry.560</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tignor.161</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cutsforth.174</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cripe.236</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Belmont.982</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Girard.502</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Vining.935</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Clever.468</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Dias.832</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Drake.377</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lane.218</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gerry.184</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Younts.552</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mcmurtrie.820</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Dowless.286</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Scheffer.323</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Rempel.454</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lis.287</t>
+  </si>
+  <si>
+    <t>Marsch.502</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lesperance.914</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gunning.855</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cripps.973</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Younkin.677</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Braz.539</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Zielinski.230</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Junior.195</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Veneziano.661</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Down.797</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ogle.891</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Resnick.437</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tindell.641</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Woltz.563</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Borjas.78</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Esquer.919</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Zdenek.728</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Astorga.32</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Dollins.210</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Standifer.77</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Stoke.982</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Grief.860</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Denis.806</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gamblin.788</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Faddis.634</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Binns.159</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Hepfer.154</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Slade.484</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Papp.563</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Encinas.262</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mcdonald.342</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Benigno.116</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Brinkley.866</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Certain.335</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cypher.353</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lautenschlage.917</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Rushford.890</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Delossantos.38</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Slee.951</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Moretti.365</t>
+  </si>
+  <si>
+    <t>Alphin.603</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Rainer.108</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Breitenstein.677</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Coletta.344</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Hieber.798</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Closson.956</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tully.114</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Caywood.170</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Silsby.242</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tait.159</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Aleman.73</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Brindley.439</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Dicarlo.674</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Florez.613</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sawyers.890</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Byrne.461</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Hagar.119</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Goldie.250</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Monfort.301</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Toll.679</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gammage.15</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Darnell.242</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Paro.334</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Barwick.128</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Dugger.786</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Leibowitz.835</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Krebsbach.938</t>
   </si>
 </sst>
 </file>
@@ -1556,7 +2231,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1853,7 +2538,7 @@
   <dimension ref="A1:E225"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1878,7 +2563,9 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1"/>
+      <c r="E1" s="1" t="s">
+        <v>466</v>
+      </c>
     </row>
     <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -1893,7 +2580,9 @@
       <c r="D2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="4"/>
+      <c r="E2" s="4" t="s">
+        <v>467</v>
+      </c>
     </row>
     <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
@@ -1908,7 +2597,9 @@
       <c r="D3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="4"/>
+      <c r="E3" s="4" t="s">
+        <v>468</v>
+      </c>
     </row>
     <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
@@ -1923,7 +2614,9 @@
       <c r="D4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="4"/>
+      <c r="E4" s="4" t="s">
+        <v>469</v>
+      </c>
     </row>
     <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -1938,7 +2631,9 @@
       <c r="D5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="4"/>
+      <c r="E5" s="4" t="s">
+        <v>470</v>
+      </c>
     </row>
     <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
@@ -1953,7 +2648,9 @@
       <c r="D6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="4"/>
+      <c r="E6" s="4" t="s">
+        <v>471</v>
+      </c>
     </row>
     <row r="7" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
@@ -1968,7 +2665,9 @@
       <c r="D7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="4"/>
+      <c r="E7" s="4" t="s">
+        <v>472</v>
+      </c>
     </row>
     <row r="8" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
@@ -1983,7 +2682,9 @@
       <c r="D8" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="4"/>
+      <c r="E8" s="4" t="s">
+        <v>473</v>
+      </c>
     </row>
     <row r="9" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
@@ -1998,7 +2699,9 @@
       <c r="D9" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="4"/>
+      <c r="E9" s="4" t="s">
+        <v>474</v>
+      </c>
     </row>
     <row r="10" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
@@ -2013,7 +2716,9 @@
       <c r="D10" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="4"/>
+      <c r="E10" s="4" t="s">
+        <v>475</v>
+      </c>
     </row>
     <row r="11" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
@@ -2028,7 +2733,9 @@
       <c r="D11" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="4"/>
+      <c r="E11" s="4" t="s">
+        <v>476</v>
+      </c>
     </row>
     <row r="12" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
@@ -2043,7 +2750,9 @@
       <c r="D12" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="4"/>
+      <c r="E12" s="4" t="s">
+        <v>477</v>
+      </c>
     </row>
     <row r="13" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
@@ -2058,7 +2767,9 @@
       <c r="D13" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="4"/>
+      <c r="E13" s="4" t="s">
+        <v>478</v>
+      </c>
     </row>
     <row r="14" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
@@ -2073,7 +2784,9 @@
       <c r="D14" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="4"/>
+      <c r="E14" s="4" t="s">
+        <v>479</v>
+      </c>
     </row>
     <row r="15" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
@@ -2088,7 +2801,9 @@
       <c r="D15" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E15" s="4"/>
+      <c r="E15" s="4" t="s">
+        <v>480</v>
+      </c>
     </row>
     <row r="16" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
@@ -2103,7 +2818,9 @@
       <c r="D16" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="4"/>
+      <c r="E16" s="4" t="s">
+        <v>481</v>
+      </c>
     </row>
     <row r="17" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
@@ -2118,7 +2835,9 @@
       <c r="D17" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E17" s="4"/>
+      <c r="E17" s="4" t="s">
+        <v>482</v>
+      </c>
     </row>
     <row r="18" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
@@ -2133,7 +2852,9 @@
       <c r="D18" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E18" s="4"/>
+      <c r="E18" s="4" t="s">
+        <v>483</v>
+      </c>
     </row>
     <row r="19" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
@@ -2148,7 +2869,9 @@
       <c r="D19" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E19" s="4"/>
+      <c r="E19" s="4" t="s">
+        <v>484</v>
+      </c>
     </row>
     <row r="20" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
@@ -2163,7 +2886,9 @@
       <c r="D20" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E20" s="4"/>
+      <c r="E20" s="4" t="s">
+        <v>485</v>
+      </c>
     </row>
     <row r="21" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
@@ -2178,7 +2903,9 @@
       <c r="D21" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E21" s="4"/>
+      <c r="E21" s="4" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="22" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
@@ -2193,7 +2920,9 @@
       <c r="D22" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E22" s="4"/>
+      <c r="E22" s="4" t="s">
+        <v>487</v>
+      </c>
     </row>
     <row r="23" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
@@ -2208,7 +2937,9 @@
       <c r="D23" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E23" s="4"/>
+      <c r="E23" s="4" t="s">
+        <v>488</v>
+      </c>
     </row>
     <row r="24" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
@@ -2223,7 +2954,9 @@
       <c r="D24" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E24" s="4"/>
+      <c r="E24" s="4" t="s">
+        <v>489</v>
+      </c>
     </row>
     <row r="25" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
@@ -2238,7 +2971,9 @@
       <c r="D25" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E25" s="4"/>
+      <c r="E25" s="4" t="s">
+        <v>490</v>
+      </c>
     </row>
     <row r="26" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
@@ -2253,7 +2988,9 @@
       <c r="D26" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E26" s="4"/>
+      <c r="E26" s="4" t="s">
+        <v>491</v>
+      </c>
     </row>
     <row r="27" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
@@ -2268,7 +3005,9 @@
       <c r="D27" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E27" s="4"/>
+      <c r="E27" s="4" t="s">
+        <v>492</v>
+      </c>
     </row>
     <row r="28" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
@@ -2283,7 +3022,9 @@
       <c r="D28" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E28" s="4"/>
+      <c r="E28" s="4" t="s">
+        <v>493</v>
+      </c>
     </row>
     <row r="29" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
@@ -2298,7 +3039,9 @@
       <c r="D29" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E29" s="4"/>
+      <c r="E29" s="4" t="s">
+        <v>494</v>
+      </c>
     </row>
     <row r="30" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
@@ -2313,7 +3056,9 @@
       <c r="D30" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E30" s="4"/>
+      <c r="E30" s="4" t="s">
+        <v>495</v>
+      </c>
     </row>
     <row r="31" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
@@ -2328,7 +3073,9 @@
       <c r="D31" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E31" s="4"/>
+      <c r="E31" s="4" t="s">
+        <v>496</v>
+      </c>
     </row>
     <row r="32" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
@@ -2343,7 +3090,9 @@
       <c r="D32" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E32" s="4"/>
+      <c r="E32" s="4" t="s">
+        <v>497</v>
+      </c>
     </row>
     <row r="33" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
@@ -2358,7 +3107,9 @@
       <c r="D33" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E33" s="4"/>
+      <c r="E33" s="4" t="s">
+        <v>498</v>
+      </c>
     </row>
     <row r="34" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
@@ -2373,7 +3124,9 @@
       <c r="D34" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E34" s="4"/>
+      <c r="E34" s="4" t="s">
+        <v>499</v>
+      </c>
     </row>
     <row r="35" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
@@ -2388,7 +3141,9 @@
       <c r="D35" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E35" s="4"/>
+      <c r="E35" s="4" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="36" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
@@ -2403,7 +3158,9 @@
       <c r="D36" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E36" s="4"/>
+      <c r="E36" s="4" t="s">
+        <v>501</v>
+      </c>
     </row>
     <row r="37" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
@@ -2418,7 +3175,9 @@
       <c r="D37" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E37" s="4"/>
+      <c r="E37" s="4" t="s">
+        <v>502</v>
+      </c>
     </row>
     <row r="38" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
@@ -2433,7 +3192,9 @@
       <c r="D38" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E38" s="4"/>
+      <c r="E38" s="4" t="s">
+        <v>503</v>
+      </c>
     </row>
     <row r="39" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
@@ -2448,7 +3209,9 @@
       <c r="D39" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E39" s="4"/>
+      <c r="E39" s="4" t="s">
+        <v>504</v>
+      </c>
     </row>
     <row r="40" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
@@ -2463,7 +3226,9 @@
       <c r="D40" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E40" s="4"/>
+      <c r="E40" s="4" t="s">
+        <v>505</v>
+      </c>
     </row>
     <row r="41" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
@@ -2478,7 +3243,9 @@
       <c r="D41" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E41" s="4"/>
+      <c r="E41" s="4" t="s">
+        <v>506</v>
+      </c>
     </row>
     <row r="42" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
@@ -2493,7 +3260,9 @@
       <c r="D42" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E42" s="4"/>
+      <c r="E42" s="4" t="s">
+        <v>507</v>
+      </c>
     </row>
     <row r="43" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
@@ -2506,7 +3275,9 @@
         <v>52</v>
       </c>
       <c r="D43" s="6"/>
-      <c r="E43" s="4"/>
+      <c r="E43" s="4" t="s">
+        <v>508</v>
+      </c>
     </row>
     <row r="44" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
@@ -2519,7 +3290,9 @@
         <v>52</v>
       </c>
       <c r="D44" s="6"/>
-      <c r="E44" s="4"/>
+      <c r="E44" s="4" t="s">
+        <v>509</v>
+      </c>
     </row>
     <row r="45" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
@@ -2532,7 +3305,9 @@
         <v>52</v>
       </c>
       <c r="D45" s="6"/>
-      <c r="E45" s="4"/>
+      <c r="E45" s="4" t="s">
+        <v>510</v>
+      </c>
     </row>
     <row r="46" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
@@ -2545,7 +3320,9 @@
         <v>52</v>
       </c>
       <c r="D46" s="6"/>
-      <c r="E46" s="4"/>
+      <c r="E46" s="4" t="s">
+        <v>511</v>
+      </c>
     </row>
     <row r="47" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
@@ -2558,7 +3335,9 @@
         <v>52</v>
       </c>
       <c r="D47" s="6"/>
-      <c r="E47" s="4"/>
+      <c r="E47" s="4" t="s">
+        <v>512</v>
+      </c>
     </row>
     <row r="48" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
@@ -2571,7 +3350,9 @@
         <v>52</v>
       </c>
       <c r="D48" s="6"/>
-      <c r="E48" s="4"/>
+      <c r="E48" s="4" t="s">
+        <v>513</v>
+      </c>
     </row>
     <row r="49" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
@@ -2584,7 +3365,9 @@
         <v>52</v>
       </c>
       <c r="D49" s="6"/>
-      <c r="E49" s="4"/>
+      <c r="E49" s="4" t="s">
+        <v>514</v>
+      </c>
     </row>
     <row r="50" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
@@ -2597,7 +3380,9 @@
         <v>52</v>
       </c>
       <c r="D50" s="6"/>
-      <c r="E50" s="4"/>
+      <c r="E50" s="4" t="s">
+        <v>515</v>
+      </c>
     </row>
     <row r="51" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
@@ -2610,7 +3395,9 @@
         <v>52</v>
       </c>
       <c r="D51" s="6"/>
-      <c r="E51" s="4"/>
+      <c r="E51" s="4" t="s">
+        <v>516</v>
+      </c>
     </row>
     <row r="52" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
@@ -2623,7 +3410,9 @@
         <v>52</v>
       </c>
       <c r="D52" s="6"/>
-      <c r="E52" s="4"/>
+      <c r="E52" s="4" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="53" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
@@ -2636,7 +3425,9 @@
         <v>52</v>
       </c>
       <c r="D53" s="6"/>
-      <c r="E53" s="4"/>
+      <c r="E53" s="4" t="s">
+        <v>518</v>
+      </c>
     </row>
     <row r="54" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
@@ -2649,7 +3440,9 @@
         <v>52</v>
       </c>
       <c r="D54" s="6"/>
-      <c r="E54" s="4"/>
+      <c r="E54" s="4" t="s">
+        <v>519</v>
+      </c>
     </row>
     <row r="55" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
@@ -2662,7 +3455,9 @@
         <v>52</v>
       </c>
       <c r="D55" s="6"/>
-      <c r="E55" s="4"/>
+      <c r="E55" s="4" t="s">
+        <v>520</v>
+      </c>
     </row>
     <row r="56" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
@@ -2675,7 +3470,9 @@
         <v>52</v>
       </c>
       <c r="D56" s="8"/>
-      <c r="E56" s="4"/>
+      <c r="E56" s="4" t="s">
+        <v>521</v>
+      </c>
     </row>
     <row r="57" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
@@ -2690,7 +3487,9 @@
       <c r="D57" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="E57" s="4"/>
+      <c r="E57" s="4" t="s">
+        <v>522</v>
+      </c>
     </row>
     <row r="58" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
@@ -2705,7 +3504,9 @@
       <c r="D58" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E58" s="4"/>
+      <c r="E58" s="4" t="s">
+        <v>523</v>
+      </c>
     </row>
     <row r="59" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
@@ -2720,7 +3521,9 @@
       <c r="D59" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E59" s="4"/>
+      <c r="E59" s="4" t="s">
+        <v>524</v>
+      </c>
     </row>
     <row r="60" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
@@ -2735,7 +3538,9 @@
       <c r="D60" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E60" s="4"/>
+      <c r="E60" s="4" t="s">
+        <v>525</v>
+      </c>
     </row>
     <row r="61" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
@@ -2750,7 +3555,9 @@
       <c r="D61" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E61" s="4"/>
+      <c r="E61" s="4" t="s">
+        <v>526</v>
+      </c>
     </row>
     <row r="62" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
@@ -2765,7 +3572,9 @@
       <c r="D62" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="E62" s="4"/>
+      <c r="E62" s="4" t="s">
+        <v>527</v>
+      </c>
     </row>
     <row r="63" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
@@ -2780,7 +3589,9 @@
       <c r="D63" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E63" s="4"/>
+      <c r="E63" s="4" t="s">
+        <v>528</v>
+      </c>
     </row>
     <row r="64" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
@@ -2795,7 +3606,9 @@
       <c r="D64" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E64" s="4"/>
+      <c r="E64" s="4" t="s">
+        <v>529</v>
+      </c>
     </row>
     <row r="65" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
@@ -2810,7 +3623,9 @@
       <c r="D65" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E65" s="4"/>
+      <c r="E65" s="4" t="s">
+        <v>530</v>
+      </c>
     </row>
     <row r="66" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
@@ -2825,7 +3640,9 @@
       <c r="D66" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E66" s="4"/>
+      <c r="E66" s="4" t="s">
+        <v>531</v>
+      </c>
     </row>
     <row r="67" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
@@ -2840,7 +3657,9 @@
       <c r="D67" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="E67" s="4"/>
+      <c r="E67" s="4" t="s">
+        <v>532</v>
+      </c>
     </row>
     <row r="68" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
@@ -2855,7 +3674,9 @@
       <c r="D68" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E68" s="4"/>
+      <c r="E68" s="4" t="s">
+        <v>533</v>
+      </c>
     </row>
     <row r="69" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
@@ -2870,7 +3691,9 @@
       <c r="D69" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E69" s="4"/>
+      <c r="E69" s="4" t="s">
+        <v>534</v>
+      </c>
     </row>
     <row r="70" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
@@ -2885,7 +3708,9 @@
       <c r="D70" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E70" s="4"/>
+      <c r="E70" s="4" t="s">
+        <v>535</v>
+      </c>
     </row>
     <row r="71" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
@@ -2898,7 +3723,9 @@
         <v>82</v>
       </c>
       <c r="D71" s="6"/>
-      <c r="E71" s="4"/>
+      <c r="E71" s="4" t="s">
+        <v>536</v>
+      </c>
     </row>
     <row r="72" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
@@ -2911,7 +3738,9 @@
         <v>82</v>
       </c>
       <c r="D72" s="6"/>
-      <c r="E72" s="4"/>
+      <c r="E72" s="4" t="s">
+        <v>537</v>
+      </c>
     </row>
     <row r="73" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
@@ -2924,7 +3753,9 @@
         <v>82</v>
       </c>
       <c r="D73" s="6"/>
-      <c r="E73" s="4"/>
+      <c r="E73" s="4" t="s">
+        <v>538</v>
+      </c>
     </row>
     <row r="74" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
@@ -2937,7 +3768,9 @@
         <v>82</v>
       </c>
       <c r="D74" s="6"/>
-      <c r="E74" s="4"/>
+      <c r="E74" s="4" t="s">
+        <v>539</v>
+      </c>
     </row>
     <row r="75" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
@@ -2950,7 +3783,9 @@
         <v>82</v>
       </c>
       <c r="D75" s="6"/>
-      <c r="E75" s="4"/>
+      <c r="E75" s="4" t="s">
+        <v>540</v>
+      </c>
     </row>
     <row r="76" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
@@ -2963,7 +3798,9 @@
         <v>82</v>
       </c>
       <c r="D76" s="6"/>
-      <c r="E76" s="4"/>
+      <c r="E76" s="4" t="s">
+        <v>541</v>
+      </c>
     </row>
     <row r="77" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
@@ -2976,7 +3813,9 @@
         <v>82</v>
       </c>
       <c r="D77" s="6"/>
-      <c r="E77" s="4"/>
+      <c r="E77" s="4" t="s">
+        <v>542</v>
+      </c>
     </row>
     <row r="78" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
@@ -2989,7 +3828,9 @@
         <v>82</v>
       </c>
       <c r="D78" s="6"/>
-      <c r="E78" s="4"/>
+      <c r="E78" s="4" t="s">
+        <v>543</v>
+      </c>
     </row>
     <row r="79" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
@@ -3002,7 +3843,9 @@
         <v>82</v>
       </c>
       <c r="D79" s="6"/>
-      <c r="E79" s="4"/>
+      <c r="E79" s="4" t="s">
+        <v>544</v>
+      </c>
     </row>
     <row r="80" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
@@ -3015,7 +3858,9 @@
         <v>82</v>
       </c>
       <c r="D80" s="6"/>
-      <c r="E80" s="4"/>
+      <c r="E80" s="4" t="s">
+        <v>545</v>
+      </c>
     </row>
     <row r="81" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
@@ -3028,7 +3873,9 @@
         <v>82</v>
       </c>
       <c r="D81" s="6"/>
-      <c r="E81" s="4"/>
+      <c r="E81" s="4" t="s">
+        <v>546</v>
+      </c>
     </row>
     <row r="82" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
@@ -3041,7 +3888,9 @@
         <v>82</v>
       </c>
       <c r="D82" s="6"/>
-      <c r="E82" s="4"/>
+      <c r="E82" s="4" t="s">
+        <v>547</v>
+      </c>
     </row>
     <row r="83" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
@@ -3054,7 +3903,9 @@
         <v>82</v>
       </c>
       <c r="D83" s="6"/>
-      <c r="E83" s="4"/>
+      <c r="E83" s="4" t="s">
+        <v>548</v>
+      </c>
     </row>
     <row r="84" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A84" s="7" t="s">
@@ -3067,7 +3918,9 @@
         <v>82</v>
       </c>
       <c r="D84" s="8"/>
-      <c r="E84" s="4"/>
+      <c r="E84" s="4" t="s">
+        <v>549</v>
+      </c>
     </row>
     <row r="85" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
@@ -3080,7 +3933,9 @@
         <v>96</v>
       </c>
       <c r="D85" s="6"/>
-      <c r="E85" s="4"/>
+      <c r="E85" s="4" t="s">
+        <v>550</v>
+      </c>
     </row>
     <row r="86" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
@@ -3093,7 +3948,9 @@
         <v>96</v>
       </c>
       <c r="D86" s="6"/>
-      <c r="E86" s="4"/>
+      <c r="E86" s="4" t="s">
+        <v>551</v>
+      </c>
     </row>
     <row r="87" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
@@ -3106,7 +3963,9 @@
         <v>96</v>
       </c>
       <c r="D87" s="6"/>
-      <c r="E87" s="4"/>
+      <c r="E87" s="4" t="s">
+        <v>552</v>
+      </c>
     </row>
     <row r="88" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
@@ -3119,7 +3978,9 @@
         <v>96</v>
       </c>
       <c r="D88" s="6"/>
-      <c r="E88" s="4"/>
+      <c r="E88" s="4" t="s">
+        <v>553</v>
+      </c>
     </row>
     <row r="89" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
@@ -3132,7 +3993,9 @@
         <v>96</v>
       </c>
       <c r="D89" s="6"/>
-      <c r="E89" s="4"/>
+      <c r="E89" s="4" t="s">
+        <v>554</v>
+      </c>
     </row>
     <row r="90" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
@@ -3145,7 +4008,9 @@
         <v>96</v>
       </c>
       <c r="D90" s="6"/>
-      <c r="E90" s="4"/>
+      <c r="E90" s="4" t="s">
+        <v>555</v>
+      </c>
     </row>
     <row r="91" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
@@ -3158,7 +4023,9 @@
         <v>96</v>
       </c>
       <c r="D91" s="6"/>
-      <c r="E91" s="4"/>
+      <c r="E91" s="4" t="s">
+        <v>556</v>
+      </c>
     </row>
     <row r="92" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
@@ -3171,7 +4038,9 @@
         <v>96</v>
       </c>
       <c r="D92" s="6"/>
-      <c r="E92" s="4"/>
+      <c r="E92" s="4" t="s">
+        <v>557</v>
+      </c>
     </row>
     <row r="93" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
@@ -3184,7 +4053,9 @@
         <v>96</v>
       </c>
       <c r="D93" s="6"/>
-      <c r="E93" s="4"/>
+      <c r="E93" s="4" t="s">
+        <v>558</v>
+      </c>
     </row>
     <row r="94" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
@@ -3197,7 +4068,9 @@
         <v>96</v>
       </c>
       <c r="D94" s="6"/>
-      <c r="E94" s="4"/>
+      <c r="E94" s="4" t="s">
+        <v>559</v>
+      </c>
     </row>
     <row r="95" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
@@ -3210,7 +4083,9 @@
         <v>96</v>
       </c>
       <c r="D95" s="6"/>
-      <c r="E95" s="4"/>
+      <c r="E95" s="4" t="s">
+        <v>560</v>
+      </c>
     </row>
     <row r="96" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
@@ -3223,7 +4098,9 @@
         <v>96</v>
       </c>
       <c r="D96" s="6"/>
-      <c r="E96" s="4"/>
+      <c r="E96" s="4" t="s">
+        <v>561</v>
+      </c>
     </row>
     <row r="97" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
@@ -3236,7 +4113,9 @@
         <v>96</v>
       </c>
       <c r="D97" s="6"/>
-      <c r="E97" s="4"/>
+      <c r="E97" s="4" t="s">
+        <v>562</v>
+      </c>
     </row>
     <row r="98" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A98" s="7" t="s">
@@ -3249,7 +4128,9 @@
         <v>96</v>
       </c>
       <c r="D98" s="8"/>
-      <c r="E98" s="4"/>
+      <c r="E98" s="4" t="s">
+        <v>563</v>
+      </c>
     </row>
     <row r="99" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
@@ -3262,7 +4143,9 @@
         <v>110</v>
       </c>
       <c r="D99" s="6"/>
-      <c r="E99" s="4"/>
+      <c r="E99" s="4" t="s">
+        <v>564</v>
+      </c>
     </row>
     <row r="100" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
@@ -3275,7 +4158,9 @@
         <v>68</v>
       </c>
       <c r="D100" s="6"/>
-      <c r="E100" s="4"/>
+      <c r="E100" s="4" t="s">
+        <v>565</v>
+      </c>
     </row>
     <row r="101" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
@@ -3288,7 +4173,9 @@
         <v>68</v>
       </c>
       <c r="D101" s="6"/>
-      <c r="E101" s="4"/>
+      <c r="E101" s="4" t="s">
+        <v>566</v>
+      </c>
     </row>
     <row r="102" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
@@ -3301,7 +4188,9 @@
         <v>113</v>
       </c>
       <c r="D102" s="6"/>
-      <c r="E102" s="4"/>
+      <c r="E102" s="4" t="s">
+        <v>567</v>
+      </c>
     </row>
     <row r="103" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
@@ -3314,7 +4203,9 @@
         <v>113</v>
       </c>
       <c r="D103" s="6"/>
-      <c r="E103" s="4"/>
+      <c r="E103" s="4" t="s">
+        <v>568</v>
+      </c>
     </row>
     <row r="104" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
@@ -3327,7 +4218,9 @@
         <v>68</v>
       </c>
       <c r="D104" s="6"/>
-      <c r="E104" s="4"/>
+      <c r="E104" s="4" t="s">
+        <v>569</v>
+      </c>
     </row>
     <row r="105" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
@@ -3340,7 +4233,9 @@
         <v>68</v>
       </c>
       <c r="D105" s="6"/>
-      <c r="E105" s="4"/>
+      <c r="E105" s="4" t="s">
+        <v>570</v>
+      </c>
     </row>
     <row r="106" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
@@ -3353,7 +4248,9 @@
         <v>113</v>
       </c>
       <c r="D106" s="6"/>
-      <c r="E106" s="4"/>
+      <c r="E106" s="4" t="s">
+        <v>571</v>
+      </c>
     </row>
     <row r="107" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
@@ -3366,7 +4263,9 @@
         <v>113</v>
       </c>
       <c r="D107" s="6"/>
-      <c r="E107" s="4"/>
+      <c r="E107" s="4" t="s">
+        <v>572</v>
+      </c>
     </row>
     <row r="108" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
@@ -3379,7 +4278,9 @@
         <v>68</v>
       </c>
       <c r="D108" s="6"/>
-      <c r="E108" s="4"/>
+      <c r="E108" s="4" t="s">
+        <v>573</v>
+      </c>
     </row>
     <row r="109" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
@@ -3392,7 +4293,9 @@
         <v>110</v>
       </c>
       <c r="D109" s="6"/>
-      <c r="E109" s="4"/>
+      <c r="E109" s="4" t="s">
+        <v>574</v>
+      </c>
     </row>
     <row r="110" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
@@ -3405,7 +4308,9 @@
         <v>110</v>
       </c>
       <c r="D110" s="6"/>
-      <c r="E110" s="4"/>
+      <c r="E110" s="4" t="s">
+        <v>575</v>
+      </c>
     </row>
     <row r="111" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
@@ -3418,7 +4323,9 @@
         <v>110</v>
       </c>
       <c r="D111" s="6"/>
-      <c r="E111" s="4"/>
+      <c r="E111" s="4" t="s">
+        <v>576</v>
+      </c>
     </row>
     <row r="112" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
@@ -3431,7 +4338,9 @@
         <v>68</v>
       </c>
       <c r="D112" s="6"/>
-      <c r="E112" s="4"/>
+      <c r="E112" s="4" t="s">
+        <v>577</v>
+      </c>
     </row>
     <row r="113" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A113" s="7" t="s">
@@ -3444,7 +4353,9 @@
         <v>113</v>
       </c>
       <c r="D113" s="8"/>
-      <c r="E113" s="4"/>
+      <c r="E113" s="4" t="s">
+        <v>578</v>
+      </c>
     </row>
     <row r="114" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
@@ -3457,7 +4368,9 @@
         <v>126</v>
       </c>
       <c r="D114" s="6"/>
-      <c r="E114" s="4"/>
+      <c r="E114" s="4" t="s">
+        <v>579</v>
+      </c>
     </row>
     <row r="115" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
@@ -3470,7 +4383,9 @@
         <v>126</v>
       </c>
       <c r="D115" s="6"/>
-      <c r="E115" s="4"/>
+      <c r="E115" s="4" t="s">
+        <v>580</v>
+      </c>
     </row>
     <row r="116" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
@@ -3483,7 +4398,9 @@
         <v>126</v>
       </c>
       <c r="D116" s="6"/>
-      <c r="E116" s="4"/>
+      <c r="E116" s="4" t="s">
+        <v>581</v>
+      </c>
     </row>
     <row r="117" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="s">
@@ -3496,7 +4413,9 @@
         <v>126</v>
       </c>
       <c r="D117" s="6"/>
-      <c r="E117" s="4"/>
+      <c r="E117" s="4" t="s">
+        <v>582</v>
+      </c>
     </row>
     <row r="118" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
@@ -3509,7 +4428,9 @@
         <v>126</v>
       </c>
       <c r="D118" s="6"/>
-      <c r="E118" s="4"/>
+      <c r="E118" s="4" t="s">
+        <v>583</v>
+      </c>
     </row>
     <row r="119" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A119" s="5" t="s">
@@ -3522,7 +4443,9 @@
         <v>126</v>
       </c>
       <c r="D119" s="6"/>
-      <c r="E119" s="4"/>
+      <c r="E119" s="4" t="s">
+        <v>584</v>
+      </c>
     </row>
     <row r="120" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A120" s="5" t="s">
@@ -3535,7 +4458,9 @@
         <v>126</v>
       </c>
       <c r="D120" s="6"/>
-      <c r="E120" s="4"/>
+      <c r="E120" s="4" t="s">
+        <v>585</v>
+      </c>
     </row>
     <row r="121" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="s">
@@ -3548,7 +4473,9 @@
         <v>126</v>
       </c>
       <c r="D121" s="6"/>
-      <c r="E121" s="4"/>
+      <c r="E121" s="4" t="s">
+        <v>586</v>
+      </c>
     </row>
     <row r="122" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A122" s="5" t="s">
@@ -3561,7 +4488,9 @@
         <v>126</v>
       </c>
       <c r="D122" s="6"/>
-      <c r="E122" s="4"/>
+      <c r="E122" s="4" t="s">
+        <v>587</v>
+      </c>
     </row>
     <row r="123" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
@@ -3574,7 +4503,9 @@
         <v>126</v>
       </c>
       <c r="D123" s="6"/>
-      <c r="E123" s="4"/>
+      <c r="E123" s="4" t="s">
+        <v>588</v>
+      </c>
     </row>
     <row r="124" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
@@ -3587,7 +4518,9 @@
         <v>126</v>
       </c>
       <c r="D124" s="6"/>
-      <c r="E124" s="4"/>
+      <c r="E124" s="4" t="s">
+        <v>589</v>
+      </c>
     </row>
     <row r="125" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
@@ -3600,7 +4533,9 @@
         <v>126</v>
       </c>
       <c r="D125" s="6"/>
-      <c r="E125" s="4"/>
+      <c r="E125" s="4" t="s">
+        <v>590</v>
+      </c>
     </row>
     <row r="126" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
@@ -3613,7 +4548,9 @@
         <v>126</v>
       </c>
       <c r="D126" s="6"/>
-      <c r="E126" s="4"/>
+      <c r="E126" s="4" t="s">
+        <v>591</v>
+      </c>
     </row>
     <row r="127" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A127" s="7" t="s">
@@ -3626,7 +4563,9 @@
         <v>126</v>
       </c>
       <c r="D127" s="8"/>
-      <c r="E127" s="4"/>
+      <c r="E127" s="4" t="s">
+        <v>592</v>
+      </c>
     </row>
     <row r="128" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A128" s="5" t="s">
@@ -3639,7 +4578,9 @@
         <v>126</v>
       </c>
       <c r="D128" s="6"/>
-      <c r="E128" s="4"/>
+      <c r="E128" s="4" t="s">
+        <v>593</v>
+      </c>
     </row>
     <row r="129" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A129" s="5" t="s">
@@ -3652,7 +4593,9 @@
         <v>126</v>
       </c>
       <c r="D129" s="6"/>
-      <c r="E129" s="4"/>
+      <c r="E129" s="4" t="s">
+        <v>594</v>
+      </c>
     </row>
     <row r="130" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
@@ -3665,7 +4608,9 @@
         <v>126</v>
       </c>
       <c r="D130" s="6"/>
-      <c r="E130" s="4"/>
+      <c r="E130" s="4" t="s">
+        <v>595</v>
+      </c>
     </row>
     <row r="131" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A131" s="5" t="s">
@@ -3678,7 +4623,9 @@
         <v>126</v>
       </c>
       <c r="D131" s="6"/>
-      <c r="E131" s="4"/>
+      <c r="E131" s="4" t="s">
+        <v>596</v>
+      </c>
     </row>
     <row r="132" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A132" s="5" t="s">
@@ -3691,7 +4638,9 @@
         <v>126</v>
       </c>
       <c r="D132" s="6"/>
-      <c r="E132" s="4"/>
+      <c r="E132" s="4" t="s">
+        <v>597</v>
+      </c>
     </row>
     <row r="133" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A133" s="5" t="s">
@@ -3704,7 +4653,9 @@
         <v>126</v>
       </c>
       <c r="D133" s="6"/>
-      <c r="E133" s="4"/>
+      <c r="E133" s="4" t="s">
+        <v>598</v>
+      </c>
     </row>
     <row r="134" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A134" s="5" t="s">
@@ -3717,7 +4668,9 @@
         <v>126</v>
       </c>
       <c r="D134" s="6"/>
-      <c r="E134" s="4"/>
+      <c r="E134" s="4" t="s">
+        <v>599</v>
+      </c>
     </row>
     <row r="135" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A135" s="5" t="s">
@@ -3730,7 +4683,9 @@
         <v>126</v>
       </c>
       <c r="D135" s="6"/>
-      <c r="E135" s="4"/>
+      <c r="E135" s="4" t="s">
+        <v>600</v>
+      </c>
     </row>
     <row r="136" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A136" s="5" t="s">
@@ -3743,7 +4698,9 @@
         <v>126</v>
       </c>
       <c r="D136" s="6"/>
-      <c r="E136" s="4"/>
+      <c r="E136" s="4" t="s">
+        <v>601</v>
+      </c>
     </row>
     <row r="137" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A137" s="5" t="s">
@@ -3756,7 +4713,9 @@
         <v>126</v>
       </c>
       <c r="D137" s="6"/>
-      <c r="E137" s="4"/>
+      <c r="E137" s="4" t="s">
+        <v>602</v>
+      </c>
     </row>
     <row r="138" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A138" s="5" t="s">
@@ -3769,7 +4728,9 @@
         <v>126</v>
       </c>
       <c r="D138" s="6"/>
-      <c r="E138" s="4"/>
+      <c r="E138" s="4" t="s">
+        <v>603</v>
+      </c>
     </row>
     <row r="139" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A139" s="5" t="s">
@@ -3782,7 +4743,9 @@
         <v>126</v>
       </c>
       <c r="D139" s="6"/>
-      <c r="E139" s="4"/>
+      <c r="E139" s="4" t="s">
+        <v>604</v>
+      </c>
     </row>
     <row r="140" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A140" s="5" t="s">
@@ -3795,7 +4758,9 @@
         <v>126</v>
       </c>
       <c r="D140" s="6"/>
-      <c r="E140" s="4"/>
+      <c r="E140" s="4" t="s">
+        <v>605</v>
+      </c>
     </row>
     <row r="141" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A141" s="5" t="s">
@@ -3808,7 +4773,9 @@
         <v>126</v>
       </c>
       <c r="D141" s="6"/>
-      <c r="E141" s="4"/>
+      <c r="E141" s="4" t="s">
+        <v>606</v>
+      </c>
     </row>
     <row r="142" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A142" s="5" t="s">
@@ -3821,7 +4788,9 @@
         <v>82</v>
       </c>
       <c r="D142" s="6"/>
-      <c r="E142" s="4"/>
+      <c r="E142" s="4" t="s">
+        <v>607</v>
+      </c>
     </row>
     <row r="143" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A143" s="5" t="s">
@@ -3834,7 +4803,9 @@
         <v>82</v>
       </c>
       <c r="D143" s="6"/>
-      <c r="E143" s="4"/>
+      <c r="E143" s="4" t="s">
+        <v>608</v>
+      </c>
     </row>
     <row r="144" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A144" s="5" t="s">
@@ -3847,7 +4818,9 @@
         <v>82</v>
       </c>
       <c r="D144" s="6"/>
-      <c r="E144" s="4"/>
+      <c r="E144" s="4" t="s">
+        <v>609</v>
+      </c>
     </row>
     <row r="145" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A145" s="5" t="s">
@@ -3860,7 +4833,9 @@
         <v>82</v>
       </c>
       <c r="D145" s="6"/>
-      <c r="E145" s="4"/>
+      <c r="E145" s="4" t="s">
+        <v>610</v>
+      </c>
     </row>
     <row r="146" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A146" s="5" t="s">
@@ -3873,7 +4848,9 @@
         <v>82</v>
       </c>
       <c r="D146" s="6"/>
-      <c r="E146" s="4"/>
+      <c r="E146" s="4" t="s">
+        <v>611</v>
+      </c>
     </row>
     <row r="147" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A147" s="5" t="s">
@@ -3886,7 +4863,9 @@
         <v>82</v>
       </c>
       <c r="D147" s="6"/>
-      <c r="E147" s="4"/>
+      <c r="E147" s="4" t="s">
+        <v>612</v>
+      </c>
     </row>
     <row r="148" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A148" s="5" t="s">
@@ -3899,7 +4878,9 @@
         <v>82</v>
       </c>
       <c r="D148" s="6"/>
-      <c r="E148" s="4"/>
+      <c r="E148" s="4" t="s">
+        <v>613</v>
+      </c>
     </row>
     <row r="149" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A149" s="5" t="s">
@@ -3912,7 +4893,9 @@
         <v>82</v>
       </c>
       <c r="D149" s="6"/>
-      <c r="E149" s="4"/>
+      <c r="E149" s="4" t="s">
+        <v>614</v>
+      </c>
     </row>
     <row r="150" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A150" s="5" t="s">
@@ -3925,7 +4908,9 @@
         <v>82</v>
       </c>
       <c r="D150" s="6"/>
-      <c r="E150" s="4"/>
+      <c r="E150" s="4" t="s">
+        <v>615</v>
+      </c>
     </row>
     <row r="151" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A151" s="5" t="s">
@@ -3938,7 +4923,9 @@
         <v>82</v>
       </c>
       <c r="D151" s="6"/>
-      <c r="E151" s="4"/>
+      <c r="E151" s="4" t="s">
+        <v>616</v>
+      </c>
     </row>
     <row r="152" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A152" s="5" t="s">
@@ -3951,7 +4938,9 @@
         <v>82</v>
       </c>
       <c r="D152" s="6"/>
-      <c r="E152" s="4"/>
+      <c r="E152" s="4" t="s">
+        <v>617</v>
+      </c>
     </row>
     <row r="153" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A153" s="5" t="s">
@@ -3964,7 +4953,9 @@
         <v>82</v>
       </c>
       <c r="D153" s="6"/>
-      <c r="E153" s="4"/>
+      <c r="E153" s="4" t="s">
+        <v>618</v>
+      </c>
     </row>
     <row r="154" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A154" s="5" t="s">
@@ -3977,7 +4968,9 @@
         <v>82</v>
       </c>
       <c r="D154" s="6"/>
-      <c r="E154" s="4"/>
+      <c r="E154" s="4" t="s">
+        <v>619</v>
+      </c>
     </row>
     <row r="155" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A155" s="7" t="s">
@@ -3990,7 +4983,9 @@
         <v>82</v>
       </c>
       <c r="D155" s="8"/>
-      <c r="E155" s="4"/>
+      <c r="E155" s="4" t="s">
+        <v>620</v>
+      </c>
     </row>
     <row r="156" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A156" s="5" t="s">
@@ -4005,7 +5000,9 @@
       <c r="D156" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E156" s="4"/>
+      <c r="E156" s="4" t="s">
+        <v>621</v>
+      </c>
     </row>
     <row r="157" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A157" s="5" t="s">
@@ -4020,7 +5017,9 @@
       <c r="D157" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E157" s="4"/>
+      <c r="E157" s="4" t="s">
+        <v>622</v>
+      </c>
     </row>
     <row r="158" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A158" s="5" t="s">
@@ -4035,7 +5034,9 @@
       <c r="D158" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="E158" s="4"/>
+      <c r="E158" s="4" t="s">
+        <v>623</v>
+      </c>
     </row>
     <row r="159" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A159" s="5" t="s">
@@ -4050,7 +5051,9 @@
       <c r="D159" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E159" s="4"/>
+      <c r="E159" s="4" t="s">
+        <v>624</v>
+      </c>
     </row>
     <row r="160" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A160" s="5" t="s">
@@ -4065,7 +5068,9 @@
       <c r="D160" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E160" s="4"/>
+      <c r="E160" s="4" t="s">
+        <v>625</v>
+      </c>
     </row>
     <row r="161" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A161" s="5" t="s">
@@ -4080,7 +5085,9 @@
       <c r="D161" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E161" s="4"/>
+      <c r="E161" s="4" t="s">
+        <v>626</v>
+      </c>
     </row>
     <row r="162" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A162" s="5" t="s">
@@ -4095,7 +5102,9 @@
       <c r="D162" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="E162" s="4"/>
+      <c r="E162" s="4" t="s">
+        <v>627</v>
+      </c>
     </row>
     <row r="163" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A163" s="5" t="s">
@@ -4110,7 +5119,9 @@
       <c r="D163" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E163" s="4"/>
+      <c r="E163" s="4" t="s">
+        <v>628</v>
+      </c>
     </row>
     <row r="164" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A164" s="5" t="s">
@@ -4125,7 +5136,9 @@
       <c r="D164" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E164" s="4"/>
+      <c r="E164" s="4" t="s">
+        <v>629</v>
+      </c>
     </row>
     <row r="165" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A165" s="5" t="s">
@@ -4140,7 +5153,9 @@
       <c r="D165" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E165" s="4"/>
+      <c r="E165" s="4" t="s">
+        <v>630</v>
+      </c>
     </row>
     <row r="166" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A166" s="5" t="s">
@@ -4155,7 +5170,9 @@
       <c r="D166" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E166" s="4"/>
+      <c r="E166" s="4" t="s">
+        <v>631</v>
+      </c>
     </row>
     <row r="167" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A167" s="5" t="s">
@@ -4170,7 +5187,9 @@
       <c r="D167" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E167" s="4"/>
+      <c r="E167" s="4" t="s">
+        <v>632</v>
+      </c>
     </row>
     <row r="168" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A168" s="5" t="s">
@@ -4185,7 +5204,9 @@
       <c r="D168" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E168" s="4"/>
+      <c r="E168" s="4" t="s">
+        <v>633</v>
+      </c>
     </row>
     <row r="169" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A169" s="7" t="s">
@@ -4200,7 +5221,9 @@
       <c r="D169" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="E169" s="4"/>
+      <c r="E169" s="4" t="s">
+        <v>634</v>
+      </c>
     </row>
     <row r="170" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A170" s="5" t="s">
@@ -4213,7 +5236,9 @@
         <v>52</v>
       </c>
       <c r="D170" s="1"/>
-      <c r="E170" s="4"/>
+      <c r="E170" s="4" t="s">
+        <v>635</v>
+      </c>
     </row>
     <row r="171" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A171" s="5" t="s">
@@ -4226,7 +5251,9 @@
         <v>52</v>
       </c>
       <c r="D171" s="1"/>
-      <c r="E171" s="4"/>
+      <c r="E171" s="4" t="s">
+        <v>636</v>
+      </c>
     </row>
     <row r="172" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A172" s="5" t="s">
@@ -4239,7 +5266,9 @@
         <v>52</v>
       </c>
       <c r="D172" s="1"/>
-      <c r="E172" s="4"/>
+      <c r="E172" s="4" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="173" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A173" s="5" t="s">
@@ -4252,7 +5281,9 @@
         <v>52</v>
       </c>
       <c r="D173" s="1"/>
-      <c r="E173" s="4"/>
+      <c r="E173" s="4" t="s">
+        <v>638</v>
+      </c>
     </row>
     <row r="174" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A174" s="5" t="s">
@@ -4265,7 +5296,9 @@
         <v>52</v>
       </c>
       <c r="D174" s="1"/>
-      <c r="E174" s="4"/>
+      <c r="E174" s="4" t="s">
+        <v>639</v>
+      </c>
     </row>
     <row r="175" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A175" s="5" t="s">
@@ -4278,7 +5311,9 @@
         <v>52</v>
       </c>
       <c r="D175" s="1"/>
-      <c r="E175" s="4"/>
+      <c r="E175" s="4" t="s">
+        <v>640</v>
+      </c>
     </row>
     <row r="176" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A176" s="5" t="s">
@@ -4291,7 +5326,9 @@
         <v>52</v>
       </c>
       <c r="D176" s="1"/>
-      <c r="E176" s="4"/>
+      <c r="E176" s="4" t="s">
+        <v>641</v>
+      </c>
     </row>
     <row r="177" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A177" s="5" t="s">
@@ -4304,7 +5341,9 @@
         <v>52</v>
       </c>
       <c r="D177" s="1"/>
-      <c r="E177" s="4"/>
+      <c r="E177" s="4" t="s">
+        <v>642</v>
+      </c>
     </row>
     <row r="178" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A178" s="5" t="s">
@@ -4317,7 +5356,9 @@
         <v>52</v>
       </c>
       <c r="D178" s="1"/>
-      <c r="E178" s="4"/>
+      <c r="E178" s="4" t="s">
+        <v>643</v>
+      </c>
     </row>
     <row r="179" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A179" s="5" t="s">
@@ -4330,7 +5371,9 @@
         <v>52</v>
       </c>
       <c r="D179" s="1"/>
-      <c r="E179" s="4"/>
+      <c r="E179" s="4" t="s">
+        <v>644</v>
+      </c>
     </row>
     <row r="180" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A180" s="5" t="s">
@@ -4343,7 +5386,9 @@
         <v>52</v>
       </c>
       <c r="D180" s="1"/>
-      <c r="E180" s="4"/>
+      <c r="E180" s="4" t="s">
+        <v>645</v>
+      </c>
     </row>
     <row r="181" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A181" s="5" t="s">
@@ -4356,7 +5401,9 @@
         <v>52</v>
       </c>
       <c r="D181" s="1"/>
-      <c r="E181" s="4"/>
+      <c r="E181" s="4" t="s">
+        <v>646</v>
+      </c>
     </row>
     <row r="182" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A182" s="5" t="s">
@@ -4369,7 +5416,9 @@
         <v>52</v>
       </c>
       <c r="D182" s="1"/>
-      <c r="E182" s="4"/>
+      <c r="E182" s="4" t="s">
+        <v>647</v>
+      </c>
     </row>
     <row r="183" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A183" s="7" t="s">
@@ -4382,7 +5431,9 @@
         <v>52</v>
       </c>
       <c r="D183" s="1"/>
-      <c r="E183" s="4"/>
+      <c r="E183" s="4" t="s">
+        <v>648</v>
+      </c>
     </row>
     <row r="184" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A184" s="5" t="s">
@@ -4397,7 +5448,9 @@
       <c r="D184" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E184" s="4"/>
+      <c r="E184" s="4" t="s">
+        <v>649</v>
+      </c>
     </row>
     <row r="185" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A185" s="5" t="s">
@@ -4412,7 +5465,9 @@
       <c r="D185" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E185" s="4"/>
+      <c r="E185" s="4" t="s">
+        <v>650</v>
+      </c>
     </row>
     <row r="186" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A186" s="5" t="s">
@@ -4427,7 +5482,9 @@
       <c r="D186" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E186" s="4"/>
+      <c r="E186" s="4" t="s">
+        <v>651</v>
+      </c>
     </row>
     <row r="187" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A187" s="5" t="s">
@@ -4442,7 +5499,9 @@
       <c r="D187" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E187" s="4"/>
+      <c r="E187" s="4" t="s">
+        <v>652</v>
+      </c>
     </row>
     <row r="188" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A188" s="5" t="s">
@@ -4457,7 +5516,9 @@
       <c r="D188" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E188" s="4"/>
+      <c r="E188" s="4" t="s">
+        <v>653</v>
+      </c>
     </row>
     <row r="189" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A189" s="5" t="s">
@@ -4472,7 +5533,9 @@
       <c r="D189" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E189" s="4"/>
+      <c r="E189" s="4" t="s">
+        <v>654</v>
+      </c>
     </row>
     <row r="190" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A190" s="5" t="s">
@@ -4487,7 +5550,9 @@
       <c r="D190" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E190" s="4"/>
+      <c r="E190" s="4" t="s">
+        <v>655</v>
+      </c>
     </row>
     <row r="191" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A191" s="5" t="s">
@@ -4502,7 +5567,9 @@
       <c r="D191" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E191" s="4"/>
+      <c r="E191" s="4" t="s">
+        <v>656</v>
+      </c>
     </row>
     <row r="192" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A192" s="5" t="s">
@@ -4517,7 +5584,9 @@
       <c r="D192" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E192" s="4"/>
+      <c r="E192" s="4" t="s">
+        <v>657</v>
+      </c>
     </row>
     <row r="193" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A193" s="5" t="s">
@@ -4532,7 +5601,9 @@
       <c r="D193" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E193" s="4"/>
+      <c r="E193" s="4" t="s">
+        <v>658</v>
+      </c>
     </row>
     <row r="194" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A194" s="5" t="s">
@@ -4547,7 +5618,9 @@
       <c r="D194" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E194" s="4"/>
+      <c r="E194" s="4" t="s">
+        <v>659</v>
+      </c>
     </row>
     <row r="195" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A195" s="5" t="s">
@@ -4562,7 +5635,9 @@
       <c r="D195" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E195" s="4"/>
+      <c r="E195" s="4" t="s">
+        <v>660</v>
+      </c>
     </row>
     <row r="196" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A196" s="5" t="s">
@@ -4577,7 +5652,9 @@
       <c r="D196" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E196" s="4"/>
+      <c r="E196" s="4" t="s">
+        <v>661</v>
+      </c>
     </row>
     <row r="197" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A197" s="7" t="s">
@@ -4592,7 +5669,9 @@
       <c r="D197" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E197" s="4"/>
+      <c r="E197" s="4" t="s">
+        <v>662</v>
+      </c>
     </row>
     <row r="198" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A198" s="5" t="s">
@@ -4607,7 +5686,9 @@
       <c r="D198" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E198" s="4"/>
+      <c r="E198" s="4" t="s">
+        <v>663</v>
+      </c>
     </row>
     <row r="199" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A199" s="5" t="s">
@@ -4622,7 +5703,9 @@
       <c r="D199" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E199" s="4"/>
+      <c r="E199" s="4" t="s">
+        <v>664</v>
+      </c>
     </row>
     <row r="200" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A200" s="5" t="s">
@@ -4637,7 +5720,9 @@
       <c r="D200" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E200" s="4"/>
+      <c r="E200" s="4" t="s">
+        <v>665</v>
+      </c>
     </row>
     <row r="201" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A201" s="5" t="s">
@@ -4652,7 +5737,9 @@
       <c r="D201" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E201" s="4"/>
+      <c r="E201" s="4" t="s">
+        <v>666</v>
+      </c>
     </row>
     <row r="202" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A202" s="5" t="s">
@@ -4667,7 +5754,9 @@
       <c r="D202" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E202" s="4"/>
+      <c r="E202" s="4" t="s">
+        <v>667</v>
+      </c>
     </row>
     <row r="203" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A203" s="5" t="s">
@@ -4682,7 +5771,9 @@
       <c r="D203" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E203" s="4"/>
+      <c r="E203" s="4" t="s">
+        <v>668</v>
+      </c>
     </row>
     <row r="204" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A204" s="5" t="s">
@@ -4697,7 +5788,9 @@
       <c r="D204" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E204" s="4"/>
+      <c r="E204" s="4" t="s">
+        <v>669</v>
+      </c>
     </row>
     <row r="205" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A205" s="5" t="s">
@@ -4712,7 +5805,9 @@
       <c r="D205" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E205" s="4"/>
+      <c r="E205" s="4" t="s">
+        <v>670</v>
+      </c>
     </row>
     <row r="206" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A206" s="5" t="s">
@@ -4727,7 +5822,9 @@
       <c r="D206" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E206" s="4"/>
+      <c r="E206" s="4" t="s">
+        <v>671</v>
+      </c>
     </row>
     <row r="207" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A207" s="5" t="s">
@@ -4742,7 +5839,9 @@
       <c r="D207" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E207" s="4"/>
+      <c r="E207" s="4" t="s">
+        <v>672</v>
+      </c>
     </row>
     <row r="208" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A208" s="5" t="s">
@@ -4757,7 +5856,9 @@
       <c r="D208" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E208" s="4"/>
+      <c r="E208" s="4" t="s">
+        <v>673</v>
+      </c>
     </row>
     <row r="209" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A209" s="5" t="s">
@@ -4772,7 +5873,9 @@
       <c r="D209" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E209" s="4"/>
+      <c r="E209" s="4" t="s">
+        <v>674</v>
+      </c>
     </row>
     <row r="210" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A210" s="5" t="s">
@@ -4787,7 +5890,9 @@
       <c r="D210" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E210" s="4"/>
+      <c r="E210" s="4" t="s">
+        <v>675</v>
+      </c>
     </row>
     <row r="211" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A211" s="7" t="s">
@@ -4802,7 +5907,9 @@
       <c r="D211" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E211" s="4"/>
+      <c r="E211" s="4" t="s">
+        <v>676</v>
+      </c>
     </row>
     <row r="212" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A212" s="5" t="s">
@@ -4817,7 +5924,9 @@
       <c r="D212" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E212" s="4"/>
+      <c r="E212" s="4" t="s">
+        <v>677</v>
+      </c>
     </row>
     <row r="213" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A213" s="5" t="s">
@@ -4832,7 +5941,9 @@
       <c r="D213" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E213" s="4"/>
+      <c r="E213" s="4" t="s">
+        <v>678</v>
+      </c>
     </row>
     <row r="214" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A214" s="5" t="s">
@@ -4847,7 +5958,9 @@
       <c r="D214" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E214" s="4"/>
+      <c r="E214" s="4" t="s">
+        <v>679</v>
+      </c>
     </row>
     <row r="215" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A215" s="5" t="s">
@@ -4862,7 +5975,9 @@
       <c r="D215" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E215" s="4"/>
+      <c r="E215" s="4" t="s">
+        <v>680</v>
+      </c>
     </row>
     <row r="216" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A216" s="5" t="s">
@@ -4877,7 +5992,9 @@
       <c r="D216" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E216" s="4"/>
+      <c r="E216" s="4" t="s">
+        <v>681</v>
+      </c>
     </row>
     <row r="217" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A217" s="5" t="s">
@@ -4892,7 +6009,9 @@
       <c r="D217" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E217" s="4"/>
+      <c r="E217" s="4" t="s">
+        <v>682</v>
+      </c>
     </row>
     <row r="218" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A218" s="5" t="s">
@@ -4907,7 +6026,9 @@
       <c r="D218" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E218" s="4"/>
+      <c r="E218" s="4" t="s">
+        <v>683</v>
+      </c>
     </row>
     <row r="219" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A219" s="5" t="s">
@@ -4922,7 +6043,9 @@
       <c r="D219" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E219" s="4"/>
+      <c r="E219" s="4" t="s">
+        <v>684</v>
+      </c>
     </row>
     <row r="220" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A220" s="5" t="s">
@@ -4937,7 +6060,9 @@
       <c r="D220" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E220" s="11"/>
+      <c r="E220" s="11" t="s">
+        <v>685</v>
+      </c>
     </row>
     <row r="221" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A221" s="5" t="s">
@@ -4952,7 +6077,9 @@
       <c r="D221" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E221" s="4"/>
+      <c r="E221" s="4" t="s">
+        <v>686</v>
+      </c>
     </row>
     <row r="222" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A222" s="5" t="s">
@@ -4967,7 +6094,9 @@
       <c r="D222" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E222" s="4"/>
+      <c r="E222" s="4" t="s">
+        <v>687</v>
+      </c>
     </row>
     <row r="223" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A223" s="5" t="s">
@@ -4982,7 +6111,9 @@
       <c r="D223" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E223" s="4"/>
+      <c r="E223" s="4" t="s">
+        <v>688</v>
+      </c>
     </row>
     <row r="224" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A224" s="5" t="s">
@@ -4997,7 +6128,9 @@
       <c r="D224" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E224" s="4"/>
+      <c r="E224" s="4" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="225" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A225" s="7" t="s">
@@ -5012,7 +6145,9 @@
       <c r="D225" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E225" s="4"/>
+      <c r="E225" s="4" t="s">
+        <v>690</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2">

</xml_diff>

<commit_message>
Removed random number generation for nameNumber to keep test data consistent (#24)
</commit_message>
<xml_diff>
--- a/models/mock-data/FakeUsers.xlsx
+++ b/models/mock-data/FakeUsers.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1012" uniqueCount="691">
   <si>
     <t>Spot</t>
   </si>
@@ -1422,6 +1422,681 @@
   </si>
   <si>
     <t>Noella Krebsbach</t>
+  </si>
+  <si>
+    <t>Name.Number</t>
+  </si>
+  <si>
+    <t>Koop.960</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mcbain.358</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Huot.633</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bezanson.660</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cavalieri.839</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bass.111</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Isaacs.442</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Wolanski.136</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Clendening.100</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ashbaugh.213</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Pinder.964</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Depalma.763</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Imel.715</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Shambaugh.40</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Albritton.668</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Slocum.139</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Maysonet.58</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Maag.400</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Laguardia.605</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Rosso.903</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Jeanbaptiste.831</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Siegrist.361</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Balas.71</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Costello.760</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Poulter.816</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Whitmire.337</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Politte.833</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Hartshorn.948</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Iser.962</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tinajero.70</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Caplan.540</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Seppala.173</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Statler.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Dartez.850</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Backman.359</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Norgard.983</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ingwersen.694</t>
+  </si>
+  <si>
+    <t>Torgersen.942</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Landey.624</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Herbst.123</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mings.349</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gandara.979</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Caffrey.986</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Branning.888</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Beland.117</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mariscal.729</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Medel.318</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Normandin.386</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Breuer.491</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Liberto.857</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Godfrey.949</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mikkelson.973</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Fleagle.381</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Darlington.481</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Hosein.882</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Juarbe.11</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Deslauriers.767</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Horney.105</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Nivens.576</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Enfinger.107</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mccraw.316</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Eggleton.598</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Wymore.153</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Dayton.843</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Petti.427</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Guercio.396</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Vasconcellos.50</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Heal.856</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Hornick.940</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Franson.807</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mahar.143</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Denney.753</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Saffell.584</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Maze.620</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Pawlowicz.398</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lahr.942</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lerman.315</t>
+  </si>
+  <si>
+    <t>Provencal.801</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Delagarza.200</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thompkins.432</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mccroskey.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Wynter.419</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cliff.333</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Storck.591</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Meikle.556</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lightfoot.559</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ester.921</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mungo.80</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Michalski.556</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lunceford.641</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Siebert.643</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Call.939</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Robin.11</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Roddy.883</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Pangle.362</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Hastings.286</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Seller.821</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mumaw.240</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Popham.241</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Grieve.693</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Camacho.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ehrenberg.441</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Champine.202</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Wells.55</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Spicer.41</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Shirley.671</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Eddington.306</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Morrisette.605</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Whiting.851</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Nordahl.9</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mullet.321</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Rand.840</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mathisen.218</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Garten.560</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tyree.611</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Peppler.143</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Paulson.371</t>
+  </si>
+  <si>
+    <t>Mercer.633</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lickteig.332</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Haddon.17</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mauger.736</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Berge.171</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Willcutt.973</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gaver.489</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ruyle.883</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Heeter.44</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Fitzwater.145</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Aquilino.382</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Palomino.241</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Dunson.706</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Hager.952</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bussell.732</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Reese.274</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Borjas.930</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cady.595</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Okada.299</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Debow.528</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Calderone.593</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Berrier.471</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Parry.560</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tignor.161</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cutsforth.174</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cripe.236</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Belmont.982</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Girard.502</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Vining.935</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Clever.468</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Dias.832</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Drake.377</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lane.218</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gerry.184</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Younts.552</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mcmurtrie.820</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Dowless.286</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Scheffer.323</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Rempel.454</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lis.287</t>
+  </si>
+  <si>
+    <t>Marsch.502</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lesperance.914</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gunning.855</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cripps.973</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Younkin.677</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Braz.539</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Zielinski.230</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Junior.195</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Veneziano.661</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Down.797</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ogle.891</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Resnick.437</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tindell.641</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Woltz.563</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Borjas.78</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Esquer.919</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Zdenek.728</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Astorga.32</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Dollins.210</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Standifer.77</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Stoke.982</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Grief.860</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Denis.806</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gamblin.788</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Faddis.634</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Binns.159</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Hepfer.154</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Slade.484</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Papp.563</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Encinas.262</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mcdonald.342</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Benigno.116</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Brinkley.866</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Certain.335</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cypher.353</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lautenschlage.917</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Rushford.890</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Delossantos.38</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Slee.951</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Moretti.365</t>
+  </si>
+  <si>
+    <t>Alphin.603</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Rainer.108</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Breitenstein.677</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Coletta.344</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Hieber.798</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Closson.956</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tully.114</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Caywood.170</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Silsby.242</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tait.159</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Aleman.73</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Brindley.439</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Dicarlo.674</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Florez.613</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sawyers.890</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Byrne.461</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Hagar.119</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Goldie.250</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Monfort.301</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Toll.679</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gammage.15</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Darnell.242</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Paro.334</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Barwick.128</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Dugger.786</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Leibowitz.835</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Krebsbach.938</t>
   </si>
 </sst>
 </file>
@@ -1556,7 +2231,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1853,7 +2538,7 @@
   <dimension ref="A1:E225"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1878,7 +2563,9 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1"/>
+      <c r="E1" s="1" t="s">
+        <v>466</v>
+      </c>
     </row>
     <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -1893,7 +2580,9 @@
       <c r="D2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="4"/>
+      <c r="E2" s="4" t="s">
+        <v>467</v>
+      </c>
     </row>
     <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
@@ -1908,7 +2597,9 @@
       <c r="D3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="4"/>
+      <c r="E3" s="4" t="s">
+        <v>468</v>
+      </c>
     </row>
     <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
@@ -1923,7 +2614,9 @@
       <c r="D4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="4"/>
+      <c r="E4" s="4" t="s">
+        <v>469</v>
+      </c>
     </row>
     <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -1938,7 +2631,9 @@
       <c r="D5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="4"/>
+      <c r="E5" s="4" t="s">
+        <v>470</v>
+      </c>
     </row>
     <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
@@ -1953,7 +2648,9 @@
       <c r="D6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="4"/>
+      <c r="E6" s="4" t="s">
+        <v>471</v>
+      </c>
     </row>
     <row r="7" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
@@ -1968,7 +2665,9 @@
       <c r="D7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="4"/>
+      <c r="E7" s="4" t="s">
+        <v>472</v>
+      </c>
     </row>
     <row r="8" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
@@ -1983,7 +2682,9 @@
       <c r="D8" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="4"/>
+      <c r="E8" s="4" t="s">
+        <v>473</v>
+      </c>
     </row>
     <row r="9" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
@@ -1998,7 +2699,9 @@
       <c r="D9" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="4"/>
+      <c r="E9" s="4" t="s">
+        <v>474</v>
+      </c>
     </row>
     <row r="10" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
@@ -2013,7 +2716,9 @@
       <c r="D10" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="4"/>
+      <c r="E10" s="4" t="s">
+        <v>475</v>
+      </c>
     </row>
     <row r="11" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
@@ -2028,7 +2733,9 @@
       <c r="D11" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="4"/>
+      <c r="E11" s="4" t="s">
+        <v>476</v>
+      </c>
     </row>
     <row r="12" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
@@ -2043,7 +2750,9 @@
       <c r="D12" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="4"/>
+      <c r="E12" s="4" t="s">
+        <v>477</v>
+      </c>
     </row>
     <row r="13" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
@@ -2058,7 +2767,9 @@
       <c r="D13" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="4"/>
+      <c r="E13" s="4" t="s">
+        <v>478</v>
+      </c>
     </row>
     <row r="14" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
@@ -2073,7 +2784,9 @@
       <c r="D14" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="4"/>
+      <c r="E14" s="4" t="s">
+        <v>479</v>
+      </c>
     </row>
     <row r="15" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
@@ -2088,7 +2801,9 @@
       <c r="D15" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E15" s="4"/>
+      <c r="E15" s="4" t="s">
+        <v>480</v>
+      </c>
     </row>
     <row r="16" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
@@ -2103,7 +2818,9 @@
       <c r="D16" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="4"/>
+      <c r="E16" s="4" t="s">
+        <v>481</v>
+      </c>
     </row>
     <row r="17" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
@@ -2118,7 +2835,9 @@
       <c r="D17" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E17" s="4"/>
+      <c r="E17" s="4" t="s">
+        <v>482</v>
+      </c>
     </row>
     <row r="18" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
@@ -2133,7 +2852,9 @@
       <c r="D18" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E18" s="4"/>
+      <c r="E18" s="4" t="s">
+        <v>483</v>
+      </c>
     </row>
     <row r="19" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
@@ -2148,7 +2869,9 @@
       <c r="D19" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E19" s="4"/>
+      <c r="E19" s="4" t="s">
+        <v>484</v>
+      </c>
     </row>
     <row r="20" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
@@ -2163,7 +2886,9 @@
       <c r="D20" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E20" s="4"/>
+      <c r="E20" s="4" t="s">
+        <v>485</v>
+      </c>
     </row>
     <row r="21" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
@@ -2178,7 +2903,9 @@
       <c r="D21" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E21" s="4"/>
+      <c r="E21" s="4" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="22" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
@@ -2193,7 +2920,9 @@
       <c r="D22" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E22" s="4"/>
+      <c r="E22" s="4" t="s">
+        <v>487</v>
+      </c>
     </row>
     <row r="23" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
@@ -2208,7 +2937,9 @@
       <c r="D23" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E23" s="4"/>
+      <c r="E23" s="4" t="s">
+        <v>488</v>
+      </c>
     </row>
     <row r="24" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
@@ -2223,7 +2954,9 @@
       <c r="D24" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E24" s="4"/>
+      <c r="E24" s="4" t="s">
+        <v>489</v>
+      </c>
     </row>
     <row r="25" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
@@ -2238,7 +2971,9 @@
       <c r="D25" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E25" s="4"/>
+      <c r="E25" s="4" t="s">
+        <v>490</v>
+      </c>
     </row>
     <row r="26" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
@@ -2253,7 +2988,9 @@
       <c r="D26" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E26" s="4"/>
+      <c r="E26" s="4" t="s">
+        <v>491</v>
+      </c>
     </row>
     <row r="27" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
@@ -2268,7 +3005,9 @@
       <c r="D27" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E27" s="4"/>
+      <c r="E27" s="4" t="s">
+        <v>492</v>
+      </c>
     </row>
     <row r="28" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
@@ -2283,7 +3022,9 @@
       <c r="D28" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E28" s="4"/>
+      <c r="E28" s="4" t="s">
+        <v>493</v>
+      </c>
     </row>
     <row r="29" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
@@ -2298,7 +3039,9 @@
       <c r="D29" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E29" s="4"/>
+      <c r="E29" s="4" t="s">
+        <v>494</v>
+      </c>
     </row>
     <row r="30" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
@@ -2313,7 +3056,9 @@
       <c r="D30" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E30" s="4"/>
+      <c r="E30" s="4" t="s">
+        <v>495</v>
+      </c>
     </row>
     <row r="31" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
@@ -2328,7 +3073,9 @@
       <c r="D31" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E31" s="4"/>
+      <c r="E31" s="4" t="s">
+        <v>496</v>
+      </c>
     </row>
     <row r="32" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
@@ -2343,7 +3090,9 @@
       <c r="D32" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E32" s="4"/>
+      <c r="E32" s="4" t="s">
+        <v>497</v>
+      </c>
     </row>
     <row r="33" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
@@ -2358,7 +3107,9 @@
       <c r="D33" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E33" s="4"/>
+      <c r="E33" s="4" t="s">
+        <v>498</v>
+      </c>
     </row>
     <row r="34" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
@@ -2373,7 +3124,9 @@
       <c r="D34" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E34" s="4"/>
+      <c r="E34" s="4" t="s">
+        <v>499</v>
+      </c>
     </row>
     <row r="35" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
@@ -2388,7 +3141,9 @@
       <c r="D35" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E35" s="4"/>
+      <c r="E35" s="4" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="36" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
@@ -2403,7 +3158,9 @@
       <c r="D36" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E36" s="4"/>
+      <c r="E36" s="4" t="s">
+        <v>501</v>
+      </c>
     </row>
     <row r="37" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
@@ -2418,7 +3175,9 @@
       <c r="D37" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E37" s="4"/>
+      <c r="E37" s="4" t="s">
+        <v>502</v>
+      </c>
     </row>
     <row r="38" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
@@ -2433,7 +3192,9 @@
       <c r="D38" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E38" s="4"/>
+      <c r="E38" s="4" t="s">
+        <v>503</v>
+      </c>
     </row>
     <row r="39" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
@@ -2448,7 +3209,9 @@
       <c r="D39" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E39" s="4"/>
+      <c r="E39" s="4" t="s">
+        <v>504</v>
+      </c>
     </row>
     <row r="40" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
@@ -2463,7 +3226,9 @@
       <c r="D40" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E40" s="4"/>
+      <c r="E40" s="4" t="s">
+        <v>505</v>
+      </c>
     </row>
     <row r="41" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
@@ -2478,7 +3243,9 @@
       <c r="D41" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E41" s="4"/>
+      <c r="E41" s="4" t="s">
+        <v>506</v>
+      </c>
     </row>
     <row r="42" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
@@ -2493,7 +3260,9 @@
       <c r="D42" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E42" s="4"/>
+      <c r="E42" s="4" t="s">
+        <v>507</v>
+      </c>
     </row>
     <row r="43" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
@@ -2506,7 +3275,9 @@
         <v>52</v>
       </c>
       <c r="D43" s="6"/>
-      <c r="E43" s="4"/>
+      <c r="E43" s="4" t="s">
+        <v>508</v>
+      </c>
     </row>
     <row r="44" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
@@ -2519,7 +3290,9 @@
         <v>52</v>
       </c>
       <c r="D44" s="6"/>
-      <c r="E44" s="4"/>
+      <c r="E44" s="4" t="s">
+        <v>509</v>
+      </c>
     </row>
     <row r="45" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
@@ -2532,7 +3305,9 @@
         <v>52</v>
       </c>
       <c r="D45" s="6"/>
-      <c r="E45" s="4"/>
+      <c r="E45" s="4" t="s">
+        <v>510</v>
+      </c>
     </row>
     <row r="46" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
@@ -2545,7 +3320,9 @@
         <v>52</v>
       </c>
       <c r="D46" s="6"/>
-      <c r="E46" s="4"/>
+      <c r="E46" s="4" t="s">
+        <v>511</v>
+      </c>
     </row>
     <row r="47" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
@@ -2558,7 +3335,9 @@
         <v>52</v>
       </c>
       <c r="D47" s="6"/>
-      <c r="E47" s="4"/>
+      <c r="E47" s="4" t="s">
+        <v>512</v>
+      </c>
     </row>
     <row r="48" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
@@ -2571,7 +3350,9 @@
         <v>52</v>
       </c>
       <c r="D48" s="6"/>
-      <c r="E48" s="4"/>
+      <c r="E48" s="4" t="s">
+        <v>513</v>
+      </c>
     </row>
     <row r="49" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
@@ -2584,7 +3365,9 @@
         <v>52</v>
       </c>
       <c r="D49" s="6"/>
-      <c r="E49" s="4"/>
+      <c r="E49" s="4" t="s">
+        <v>514</v>
+      </c>
     </row>
     <row r="50" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
@@ -2597,7 +3380,9 @@
         <v>52</v>
       </c>
       <c r="D50" s="6"/>
-      <c r="E50" s="4"/>
+      <c r="E50" s="4" t="s">
+        <v>515</v>
+      </c>
     </row>
     <row r="51" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
@@ -2610,7 +3395,9 @@
         <v>52</v>
       </c>
       <c r="D51" s="6"/>
-      <c r="E51" s="4"/>
+      <c r="E51" s="4" t="s">
+        <v>516</v>
+      </c>
     </row>
     <row r="52" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
@@ -2623,7 +3410,9 @@
         <v>52</v>
       </c>
       <c r="D52" s="6"/>
-      <c r="E52" s="4"/>
+      <c r="E52" s="4" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="53" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
@@ -2636,7 +3425,9 @@
         <v>52</v>
       </c>
       <c r="D53" s="6"/>
-      <c r="E53" s="4"/>
+      <c r="E53" s="4" t="s">
+        <v>518</v>
+      </c>
     </row>
     <row r="54" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
@@ -2649,7 +3440,9 @@
         <v>52</v>
       </c>
       <c r="D54" s="6"/>
-      <c r="E54" s="4"/>
+      <c r="E54" s="4" t="s">
+        <v>519</v>
+      </c>
     </row>
     <row r="55" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
@@ -2662,7 +3455,9 @@
         <v>52</v>
       </c>
       <c r="D55" s="6"/>
-      <c r="E55" s="4"/>
+      <c r="E55" s="4" t="s">
+        <v>520</v>
+      </c>
     </row>
     <row r="56" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
@@ -2675,7 +3470,9 @@
         <v>52</v>
       </c>
       <c r="D56" s="8"/>
-      <c r="E56" s="4"/>
+      <c r="E56" s="4" t="s">
+        <v>521</v>
+      </c>
     </row>
     <row r="57" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
@@ -2690,7 +3487,9 @@
       <c r="D57" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="E57" s="4"/>
+      <c r="E57" s="4" t="s">
+        <v>522</v>
+      </c>
     </row>
     <row r="58" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
@@ -2705,7 +3504,9 @@
       <c r="D58" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E58" s="4"/>
+      <c r="E58" s="4" t="s">
+        <v>523</v>
+      </c>
     </row>
     <row r="59" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
@@ -2720,7 +3521,9 @@
       <c r="D59" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E59" s="4"/>
+      <c r="E59" s="4" t="s">
+        <v>524</v>
+      </c>
     </row>
     <row r="60" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
@@ -2735,7 +3538,9 @@
       <c r="D60" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E60" s="4"/>
+      <c r="E60" s="4" t="s">
+        <v>525</v>
+      </c>
     </row>
     <row r="61" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
@@ -2750,7 +3555,9 @@
       <c r="D61" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E61" s="4"/>
+      <c r="E61" s="4" t="s">
+        <v>526</v>
+      </c>
     </row>
     <row r="62" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
@@ -2765,7 +3572,9 @@
       <c r="D62" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="E62" s="4"/>
+      <c r="E62" s="4" t="s">
+        <v>527</v>
+      </c>
     </row>
     <row r="63" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
@@ -2780,7 +3589,9 @@
       <c r="D63" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E63" s="4"/>
+      <c r="E63" s="4" t="s">
+        <v>528</v>
+      </c>
     </row>
     <row r="64" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
@@ -2795,7 +3606,9 @@
       <c r="D64" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E64" s="4"/>
+      <c r="E64" s="4" t="s">
+        <v>529</v>
+      </c>
     </row>
     <row r="65" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
@@ -2810,7 +3623,9 @@
       <c r="D65" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E65" s="4"/>
+      <c r="E65" s="4" t="s">
+        <v>530</v>
+      </c>
     </row>
     <row r="66" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
@@ -2825,7 +3640,9 @@
       <c r="D66" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E66" s="4"/>
+      <c r="E66" s="4" t="s">
+        <v>531</v>
+      </c>
     </row>
     <row r="67" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
@@ -2840,7 +3657,9 @@
       <c r="D67" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="E67" s="4"/>
+      <c r="E67" s="4" t="s">
+        <v>532</v>
+      </c>
     </row>
     <row r="68" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
@@ -2855,7 +3674,9 @@
       <c r="D68" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E68" s="4"/>
+      <c r="E68" s="4" t="s">
+        <v>533</v>
+      </c>
     </row>
     <row r="69" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
@@ -2870,7 +3691,9 @@
       <c r="D69" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E69" s="4"/>
+      <c r="E69" s="4" t="s">
+        <v>534</v>
+      </c>
     </row>
     <row r="70" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
@@ -2885,7 +3708,9 @@
       <c r="D70" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E70" s="4"/>
+      <c r="E70" s="4" t="s">
+        <v>535</v>
+      </c>
     </row>
     <row r="71" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
@@ -2898,7 +3723,9 @@
         <v>82</v>
       </c>
       <c r="D71" s="6"/>
-      <c r="E71" s="4"/>
+      <c r="E71" s="4" t="s">
+        <v>536</v>
+      </c>
     </row>
     <row r="72" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
@@ -2911,7 +3738,9 @@
         <v>82</v>
       </c>
       <c r="D72" s="6"/>
-      <c r="E72" s="4"/>
+      <c r="E72" s="4" t="s">
+        <v>537</v>
+      </c>
     </row>
     <row r="73" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
@@ -2924,7 +3753,9 @@
         <v>82</v>
       </c>
       <c r="D73" s="6"/>
-      <c r="E73" s="4"/>
+      <c r="E73" s="4" t="s">
+        <v>538</v>
+      </c>
     </row>
     <row r="74" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
@@ -2937,7 +3768,9 @@
         <v>82</v>
       </c>
       <c r="D74" s="6"/>
-      <c r="E74" s="4"/>
+      <c r="E74" s="4" t="s">
+        <v>539</v>
+      </c>
     </row>
     <row r="75" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
@@ -2950,7 +3783,9 @@
         <v>82</v>
       </c>
       <c r="D75" s="6"/>
-      <c r="E75" s="4"/>
+      <c r="E75" s="4" t="s">
+        <v>540</v>
+      </c>
     </row>
     <row r="76" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
@@ -2963,7 +3798,9 @@
         <v>82</v>
       </c>
       <c r="D76" s="6"/>
-      <c r="E76" s="4"/>
+      <c r="E76" s="4" t="s">
+        <v>541</v>
+      </c>
     </row>
     <row r="77" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
@@ -2976,7 +3813,9 @@
         <v>82</v>
       </c>
       <c r="D77" s="6"/>
-      <c r="E77" s="4"/>
+      <c r="E77" s="4" t="s">
+        <v>542</v>
+      </c>
     </row>
     <row r="78" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
@@ -2989,7 +3828,9 @@
         <v>82</v>
       </c>
       <c r="D78" s="6"/>
-      <c r="E78" s="4"/>
+      <c r="E78" s="4" t="s">
+        <v>543</v>
+      </c>
     </row>
     <row r="79" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
@@ -3002,7 +3843,9 @@
         <v>82</v>
       </c>
       <c r="D79" s="6"/>
-      <c r="E79" s="4"/>
+      <c r="E79" s="4" t="s">
+        <v>544</v>
+      </c>
     </row>
     <row r="80" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
@@ -3015,7 +3858,9 @@
         <v>82</v>
       </c>
       <c r="D80" s="6"/>
-      <c r="E80" s="4"/>
+      <c r="E80" s="4" t="s">
+        <v>545</v>
+      </c>
     </row>
     <row r="81" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
@@ -3028,7 +3873,9 @@
         <v>82</v>
       </c>
       <c r="D81" s="6"/>
-      <c r="E81" s="4"/>
+      <c r="E81" s="4" t="s">
+        <v>546</v>
+      </c>
     </row>
     <row r="82" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
@@ -3041,7 +3888,9 @@
         <v>82</v>
       </c>
       <c r="D82" s="6"/>
-      <c r="E82" s="4"/>
+      <c r="E82" s="4" t="s">
+        <v>547</v>
+      </c>
     </row>
     <row r="83" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
@@ -3054,7 +3903,9 @@
         <v>82</v>
       </c>
       <c r="D83" s="6"/>
-      <c r="E83" s="4"/>
+      <c r="E83" s="4" t="s">
+        <v>548</v>
+      </c>
     </row>
     <row r="84" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A84" s="7" t="s">
@@ -3067,7 +3918,9 @@
         <v>82</v>
       </c>
       <c r="D84" s="8"/>
-      <c r="E84" s="4"/>
+      <c r="E84" s="4" t="s">
+        <v>549</v>
+      </c>
     </row>
     <row r="85" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
@@ -3080,7 +3933,9 @@
         <v>96</v>
       </c>
       <c r="D85" s="6"/>
-      <c r="E85" s="4"/>
+      <c r="E85" s="4" t="s">
+        <v>550</v>
+      </c>
     </row>
     <row r="86" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
@@ -3093,7 +3948,9 @@
         <v>96</v>
       </c>
       <c r="D86" s="6"/>
-      <c r="E86" s="4"/>
+      <c r="E86" s="4" t="s">
+        <v>551</v>
+      </c>
     </row>
     <row r="87" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
@@ -3106,7 +3963,9 @@
         <v>96</v>
       </c>
       <c r="D87" s="6"/>
-      <c r="E87" s="4"/>
+      <c r="E87" s="4" t="s">
+        <v>552</v>
+      </c>
     </row>
     <row r="88" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
@@ -3119,7 +3978,9 @@
         <v>96</v>
       </c>
       <c r="D88" s="6"/>
-      <c r="E88" s="4"/>
+      <c r="E88" s="4" t="s">
+        <v>553</v>
+      </c>
     </row>
     <row r="89" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
@@ -3132,7 +3993,9 @@
         <v>96</v>
       </c>
       <c r="D89" s="6"/>
-      <c r="E89" s="4"/>
+      <c r="E89" s="4" t="s">
+        <v>554</v>
+      </c>
     </row>
     <row r="90" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
@@ -3145,7 +4008,9 @@
         <v>96</v>
       </c>
       <c r="D90" s="6"/>
-      <c r="E90" s="4"/>
+      <c r="E90" s="4" t="s">
+        <v>555</v>
+      </c>
     </row>
     <row r="91" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
@@ -3158,7 +4023,9 @@
         <v>96</v>
       </c>
       <c r="D91" s="6"/>
-      <c r="E91" s="4"/>
+      <c r="E91" s="4" t="s">
+        <v>556</v>
+      </c>
     </row>
     <row r="92" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
@@ -3171,7 +4038,9 @@
         <v>96</v>
       </c>
       <c r="D92" s="6"/>
-      <c r="E92" s="4"/>
+      <c r="E92" s="4" t="s">
+        <v>557</v>
+      </c>
     </row>
     <row r="93" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
@@ -3184,7 +4053,9 @@
         <v>96</v>
       </c>
       <c r="D93" s="6"/>
-      <c r="E93" s="4"/>
+      <c r="E93" s="4" t="s">
+        <v>558</v>
+      </c>
     </row>
     <row r="94" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
@@ -3197,7 +4068,9 @@
         <v>96</v>
       </c>
       <c r="D94" s="6"/>
-      <c r="E94" s="4"/>
+      <c r="E94" s="4" t="s">
+        <v>559</v>
+      </c>
     </row>
     <row r="95" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
@@ -3210,7 +4083,9 @@
         <v>96</v>
       </c>
       <c r="D95" s="6"/>
-      <c r="E95" s="4"/>
+      <c r="E95" s="4" t="s">
+        <v>560</v>
+      </c>
     </row>
     <row r="96" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
@@ -3223,7 +4098,9 @@
         <v>96</v>
       </c>
       <c r="D96" s="6"/>
-      <c r="E96" s="4"/>
+      <c r="E96" s="4" t="s">
+        <v>561</v>
+      </c>
     </row>
     <row r="97" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
@@ -3236,7 +4113,9 @@
         <v>96</v>
       </c>
       <c r="D97" s="6"/>
-      <c r="E97" s="4"/>
+      <c r="E97" s="4" t="s">
+        <v>562</v>
+      </c>
     </row>
     <row r="98" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A98" s="7" t="s">
@@ -3249,7 +4128,9 @@
         <v>96</v>
       </c>
       <c r="D98" s="8"/>
-      <c r="E98" s="4"/>
+      <c r="E98" s="4" t="s">
+        <v>563</v>
+      </c>
     </row>
     <row r="99" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
@@ -3262,7 +4143,9 @@
         <v>110</v>
       </c>
       <c r="D99" s="6"/>
-      <c r="E99" s="4"/>
+      <c r="E99" s="4" t="s">
+        <v>564</v>
+      </c>
     </row>
     <row r="100" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
@@ -3275,7 +4158,9 @@
         <v>68</v>
       </c>
       <c r="D100" s="6"/>
-      <c r="E100" s="4"/>
+      <c r="E100" s="4" t="s">
+        <v>565</v>
+      </c>
     </row>
     <row r="101" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
@@ -3288,7 +4173,9 @@
         <v>68</v>
       </c>
       <c r="D101" s="6"/>
-      <c r="E101" s="4"/>
+      <c r="E101" s="4" t="s">
+        <v>566</v>
+      </c>
     </row>
     <row r="102" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
@@ -3301,7 +4188,9 @@
         <v>113</v>
       </c>
       <c r="D102" s="6"/>
-      <c r="E102" s="4"/>
+      <c r="E102" s="4" t="s">
+        <v>567</v>
+      </c>
     </row>
     <row r="103" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
@@ -3314,7 +4203,9 @@
         <v>113</v>
       </c>
       <c r="D103" s="6"/>
-      <c r="E103" s="4"/>
+      <c r="E103" s="4" t="s">
+        <v>568</v>
+      </c>
     </row>
     <row r="104" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
@@ -3327,7 +4218,9 @@
         <v>68</v>
       </c>
       <c r="D104" s="6"/>
-      <c r="E104" s="4"/>
+      <c r="E104" s="4" t="s">
+        <v>569</v>
+      </c>
     </row>
     <row r="105" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
@@ -3340,7 +4233,9 @@
         <v>68</v>
       </c>
       <c r="D105" s="6"/>
-      <c r="E105" s="4"/>
+      <c r="E105" s="4" t="s">
+        <v>570</v>
+      </c>
     </row>
     <row r="106" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
@@ -3353,7 +4248,9 @@
         <v>113</v>
       </c>
       <c r="D106" s="6"/>
-      <c r="E106" s="4"/>
+      <c r="E106" s="4" t="s">
+        <v>571</v>
+      </c>
     </row>
     <row r="107" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
@@ -3366,7 +4263,9 @@
         <v>113</v>
       </c>
       <c r="D107" s="6"/>
-      <c r="E107" s="4"/>
+      <c r="E107" s="4" t="s">
+        <v>572</v>
+      </c>
     </row>
     <row r="108" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
@@ -3379,7 +4278,9 @@
         <v>68</v>
       </c>
       <c r="D108" s="6"/>
-      <c r="E108" s="4"/>
+      <c r="E108" s="4" t="s">
+        <v>573</v>
+      </c>
     </row>
     <row r="109" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
@@ -3392,7 +4293,9 @@
         <v>110</v>
       </c>
       <c r="D109" s="6"/>
-      <c r="E109" s="4"/>
+      <c r="E109" s="4" t="s">
+        <v>574</v>
+      </c>
     </row>
     <row r="110" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
@@ -3405,7 +4308,9 @@
         <v>110</v>
       </c>
       <c r="D110" s="6"/>
-      <c r="E110" s="4"/>
+      <c r="E110" s="4" t="s">
+        <v>575</v>
+      </c>
     </row>
     <row r="111" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
@@ -3418,7 +4323,9 @@
         <v>110</v>
       </c>
       <c r="D111" s="6"/>
-      <c r="E111" s="4"/>
+      <c r="E111" s="4" t="s">
+        <v>576</v>
+      </c>
     </row>
     <row r="112" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
@@ -3431,7 +4338,9 @@
         <v>68</v>
       </c>
       <c r="D112" s="6"/>
-      <c r="E112" s="4"/>
+      <c r="E112" s="4" t="s">
+        <v>577</v>
+      </c>
     </row>
     <row r="113" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A113" s="7" t="s">
@@ -3444,7 +4353,9 @@
         <v>113</v>
       </c>
       <c r="D113" s="8"/>
-      <c r="E113" s="4"/>
+      <c r="E113" s="4" t="s">
+        <v>578</v>
+      </c>
     </row>
     <row r="114" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
@@ -3457,7 +4368,9 @@
         <v>126</v>
       </c>
       <c r="D114" s="6"/>
-      <c r="E114" s="4"/>
+      <c r="E114" s="4" t="s">
+        <v>579</v>
+      </c>
     </row>
     <row r="115" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
@@ -3470,7 +4383,9 @@
         <v>126</v>
       </c>
       <c r="D115" s="6"/>
-      <c r="E115" s="4"/>
+      <c r="E115" s="4" t="s">
+        <v>580</v>
+      </c>
     </row>
     <row r="116" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
@@ -3483,7 +4398,9 @@
         <v>126</v>
       </c>
       <c r="D116" s="6"/>
-      <c r="E116" s="4"/>
+      <c r="E116" s="4" t="s">
+        <v>581</v>
+      </c>
     </row>
     <row r="117" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="s">
@@ -3496,7 +4413,9 @@
         <v>126</v>
       </c>
       <c r="D117" s="6"/>
-      <c r="E117" s="4"/>
+      <c r="E117" s="4" t="s">
+        <v>582</v>
+      </c>
     </row>
     <row r="118" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
@@ -3509,7 +4428,9 @@
         <v>126</v>
       </c>
       <c r="D118" s="6"/>
-      <c r="E118" s="4"/>
+      <c r="E118" s="4" t="s">
+        <v>583</v>
+      </c>
     </row>
     <row r="119" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A119" s="5" t="s">
@@ -3522,7 +4443,9 @@
         <v>126</v>
       </c>
       <c r="D119" s="6"/>
-      <c r="E119" s="4"/>
+      <c r="E119" s="4" t="s">
+        <v>584</v>
+      </c>
     </row>
     <row r="120" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A120" s="5" t="s">
@@ -3535,7 +4458,9 @@
         <v>126</v>
       </c>
       <c r="D120" s="6"/>
-      <c r="E120" s="4"/>
+      <c r="E120" s="4" t="s">
+        <v>585</v>
+      </c>
     </row>
     <row r="121" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="s">
@@ -3548,7 +4473,9 @@
         <v>126</v>
       </c>
       <c r="D121" s="6"/>
-      <c r="E121" s="4"/>
+      <c r="E121" s="4" t="s">
+        <v>586</v>
+      </c>
     </row>
     <row r="122" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A122" s="5" t="s">
@@ -3561,7 +4488,9 @@
         <v>126</v>
       </c>
       <c r="D122" s="6"/>
-      <c r="E122" s="4"/>
+      <c r="E122" s="4" t="s">
+        <v>587</v>
+      </c>
     </row>
     <row r="123" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
@@ -3574,7 +4503,9 @@
         <v>126</v>
       </c>
       <c r="D123" s="6"/>
-      <c r="E123" s="4"/>
+      <c r="E123" s="4" t="s">
+        <v>588</v>
+      </c>
     </row>
     <row r="124" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
@@ -3587,7 +4518,9 @@
         <v>126</v>
       </c>
       <c r="D124" s="6"/>
-      <c r="E124" s="4"/>
+      <c r="E124" s="4" t="s">
+        <v>589</v>
+      </c>
     </row>
     <row r="125" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
@@ -3600,7 +4533,9 @@
         <v>126</v>
       </c>
       <c r="D125" s="6"/>
-      <c r="E125" s="4"/>
+      <c r="E125" s="4" t="s">
+        <v>590</v>
+      </c>
     </row>
     <row r="126" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
@@ -3613,7 +4548,9 @@
         <v>126</v>
       </c>
       <c r="D126" s="6"/>
-      <c r="E126" s="4"/>
+      <c r="E126" s="4" t="s">
+        <v>591</v>
+      </c>
     </row>
     <row r="127" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A127" s="7" t="s">
@@ -3626,7 +4563,9 @@
         <v>126</v>
       </c>
       <c r="D127" s="8"/>
-      <c r="E127" s="4"/>
+      <c r="E127" s="4" t="s">
+        <v>592</v>
+      </c>
     </row>
     <row r="128" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A128" s="5" t="s">
@@ -3639,7 +4578,9 @@
         <v>126</v>
       </c>
       <c r="D128" s="6"/>
-      <c r="E128" s="4"/>
+      <c r="E128" s="4" t="s">
+        <v>593</v>
+      </c>
     </row>
     <row r="129" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A129" s="5" t="s">
@@ -3652,7 +4593,9 @@
         <v>126</v>
       </c>
       <c r="D129" s="6"/>
-      <c r="E129" s="4"/>
+      <c r="E129" s="4" t="s">
+        <v>594</v>
+      </c>
     </row>
     <row r="130" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
@@ -3665,7 +4608,9 @@
         <v>126</v>
       </c>
       <c r="D130" s="6"/>
-      <c r="E130" s="4"/>
+      <c r="E130" s="4" t="s">
+        <v>595</v>
+      </c>
     </row>
     <row r="131" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A131" s="5" t="s">
@@ -3678,7 +4623,9 @@
         <v>126</v>
       </c>
       <c r="D131" s="6"/>
-      <c r="E131" s="4"/>
+      <c r="E131" s="4" t="s">
+        <v>596</v>
+      </c>
     </row>
     <row r="132" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A132" s="5" t="s">
@@ -3691,7 +4638,9 @@
         <v>126</v>
       </c>
       <c r="D132" s="6"/>
-      <c r="E132" s="4"/>
+      <c r="E132" s="4" t="s">
+        <v>597</v>
+      </c>
     </row>
     <row r="133" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A133" s="5" t="s">
@@ -3704,7 +4653,9 @@
         <v>126</v>
       </c>
       <c r="D133" s="6"/>
-      <c r="E133" s="4"/>
+      <c r="E133" s="4" t="s">
+        <v>598</v>
+      </c>
     </row>
     <row r="134" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A134" s="5" t="s">
@@ -3717,7 +4668,9 @@
         <v>126</v>
       </c>
       <c r="D134" s="6"/>
-      <c r="E134" s="4"/>
+      <c r="E134" s="4" t="s">
+        <v>599</v>
+      </c>
     </row>
     <row r="135" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A135" s="5" t="s">
@@ -3730,7 +4683,9 @@
         <v>126</v>
       </c>
       <c r="D135" s="6"/>
-      <c r="E135" s="4"/>
+      <c r="E135" s="4" t="s">
+        <v>600</v>
+      </c>
     </row>
     <row r="136" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A136" s="5" t="s">
@@ -3743,7 +4698,9 @@
         <v>126</v>
       </c>
       <c r="D136" s="6"/>
-      <c r="E136" s="4"/>
+      <c r="E136" s="4" t="s">
+        <v>601</v>
+      </c>
     </row>
     <row r="137" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A137" s="5" t="s">
@@ -3756,7 +4713,9 @@
         <v>126</v>
       </c>
       <c r="D137" s="6"/>
-      <c r="E137" s="4"/>
+      <c r="E137" s="4" t="s">
+        <v>602</v>
+      </c>
     </row>
     <row r="138" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A138" s="5" t="s">
@@ -3769,7 +4728,9 @@
         <v>126</v>
       </c>
       <c r="D138" s="6"/>
-      <c r="E138" s="4"/>
+      <c r="E138" s="4" t="s">
+        <v>603</v>
+      </c>
     </row>
     <row r="139" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A139" s="5" t="s">
@@ -3782,7 +4743,9 @@
         <v>126</v>
       </c>
       <c r="D139" s="6"/>
-      <c r="E139" s="4"/>
+      <c r="E139" s="4" t="s">
+        <v>604</v>
+      </c>
     </row>
     <row r="140" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A140" s="5" t="s">
@@ -3795,7 +4758,9 @@
         <v>126</v>
       </c>
       <c r="D140" s="6"/>
-      <c r="E140" s="4"/>
+      <c r="E140" s="4" t="s">
+        <v>605</v>
+      </c>
     </row>
     <row r="141" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A141" s="5" t="s">
@@ -3808,7 +4773,9 @@
         <v>126</v>
       </c>
       <c r="D141" s="6"/>
-      <c r="E141" s="4"/>
+      <c r="E141" s="4" t="s">
+        <v>606</v>
+      </c>
     </row>
     <row r="142" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A142" s="5" t="s">
@@ -3821,7 +4788,9 @@
         <v>82</v>
       </c>
       <c r="D142" s="6"/>
-      <c r="E142" s="4"/>
+      <c r="E142" s="4" t="s">
+        <v>607</v>
+      </c>
     </row>
     <row r="143" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A143" s="5" t="s">
@@ -3834,7 +4803,9 @@
         <v>82</v>
       </c>
       <c r="D143" s="6"/>
-      <c r="E143" s="4"/>
+      <c r="E143" s="4" t="s">
+        <v>608</v>
+      </c>
     </row>
     <row r="144" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A144" s="5" t="s">
@@ -3847,7 +4818,9 @@
         <v>82</v>
       </c>
       <c r="D144" s="6"/>
-      <c r="E144" s="4"/>
+      <c r="E144" s="4" t="s">
+        <v>609</v>
+      </c>
     </row>
     <row r="145" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A145" s="5" t="s">
@@ -3860,7 +4833,9 @@
         <v>82</v>
       </c>
       <c r="D145" s="6"/>
-      <c r="E145" s="4"/>
+      <c r="E145" s="4" t="s">
+        <v>610</v>
+      </c>
     </row>
     <row r="146" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A146" s="5" t="s">
@@ -3873,7 +4848,9 @@
         <v>82</v>
       </c>
       <c r="D146" s="6"/>
-      <c r="E146" s="4"/>
+      <c r="E146" s="4" t="s">
+        <v>611</v>
+      </c>
     </row>
     <row r="147" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A147" s="5" t="s">
@@ -3886,7 +4863,9 @@
         <v>82</v>
       </c>
       <c r="D147" s="6"/>
-      <c r="E147" s="4"/>
+      <c r="E147" s="4" t="s">
+        <v>612</v>
+      </c>
     </row>
     <row r="148" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A148" s="5" t="s">
@@ -3899,7 +4878,9 @@
         <v>82</v>
       </c>
       <c r="D148" s="6"/>
-      <c r="E148" s="4"/>
+      <c r="E148" s="4" t="s">
+        <v>613</v>
+      </c>
     </row>
     <row r="149" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A149" s="5" t="s">
@@ -3912,7 +4893,9 @@
         <v>82</v>
       </c>
       <c r="D149" s="6"/>
-      <c r="E149" s="4"/>
+      <c r="E149" s="4" t="s">
+        <v>614</v>
+      </c>
     </row>
     <row r="150" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A150" s="5" t="s">
@@ -3925,7 +4908,9 @@
         <v>82</v>
       </c>
       <c r="D150" s="6"/>
-      <c r="E150" s="4"/>
+      <c r="E150" s="4" t="s">
+        <v>615</v>
+      </c>
     </row>
     <row r="151" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A151" s="5" t="s">
@@ -3938,7 +4923,9 @@
         <v>82</v>
       </c>
       <c r="D151" s="6"/>
-      <c r="E151" s="4"/>
+      <c r="E151" s="4" t="s">
+        <v>616</v>
+      </c>
     </row>
     <row r="152" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A152" s="5" t="s">
@@ -3951,7 +4938,9 @@
         <v>82</v>
       </c>
       <c r="D152" s="6"/>
-      <c r="E152" s="4"/>
+      <c r="E152" s="4" t="s">
+        <v>617</v>
+      </c>
     </row>
     <row r="153" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A153" s="5" t="s">
@@ -3964,7 +4953,9 @@
         <v>82</v>
       </c>
       <c r="D153" s="6"/>
-      <c r="E153" s="4"/>
+      <c r="E153" s="4" t="s">
+        <v>618</v>
+      </c>
     </row>
     <row r="154" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A154" s="5" t="s">
@@ -3977,7 +4968,9 @@
         <v>82</v>
       </c>
       <c r="D154" s="6"/>
-      <c r="E154" s="4"/>
+      <c r="E154" s="4" t="s">
+        <v>619</v>
+      </c>
     </row>
     <row r="155" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A155" s="7" t="s">
@@ -3990,7 +4983,9 @@
         <v>82</v>
       </c>
       <c r="D155" s="8"/>
-      <c r="E155" s="4"/>
+      <c r="E155" s="4" t="s">
+        <v>620</v>
+      </c>
     </row>
     <row r="156" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A156" s="5" t="s">
@@ -4005,7 +5000,9 @@
       <c r="D156" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E156" s="4"/>
+      <c r="E156" s="4" t="s">
+        <v>621</v>
+      </c>
     </row>
     <row r="157" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A157" s="5" t="s">
@@ -4020,7 +5017,9 @@
       <c r="D157" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E157" s="4"/>
+      <c r="E157" s="4" t="s">
+        <v>622</v>
+      </c>
     </row>
     <row r="158" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A158" s="5" t="s">
@@ -4035,7 +5034,9 @@
       <c r="D158" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="E158" s="4"/>
+      <c r="E158" s="4" t="s">
+        <v>623</v>
+      </c>
     </row>
     <row r="159" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A159" s="5" t="s">
@@ -4050,7 +5051,9 @@
       <c r="D159" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E159" s="4"/>
+      <c r="E159" s="4" t="s">
+        <v>624</v>
+      </c>
     </row>
     <row r="160" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A160" s="5" t="s">
@@ -4065,7 +5068,9 @@
       <c r="D160" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E160" s="4"/>
+      <c r="E160" s="4" t="s">
+        <v>625</v>
+      </c>
     </row>
     <row r="161" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A161" s="5" t="s">
@@ -4080,7 +5085,9 @@
       <c r="D161" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E161" s="4"/>
+      <c r="E161" s="4" t="s">
+        <v>626</v>
+      </c>
     </row>
     <row r="162" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A162" s="5" t="s">
@@ -4095,7 +5102,9 @@
       <c r="D162" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="E162" s="4"/>
+      <c r="E162" s="4" t="s">
+        <v>627</v>
+      </c>
     </row>
     <row r="163" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A163" s="5" t="s">
@@ -4110,7 +5119,9 @@
       <c r="D163" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E163" s="4"/>
+      <c r="E163" s="4" t="s">
+        <v>628</v>
+      </c>
     </row>
     <row r="164" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A164" s="5" t="s">
@@ -4125,7 +5136,9 @@
       <c r="D164" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E164" s="4"/>
+      <c r="E164" s="4" t="s">
+        <v>629</v>
+      </c>
     </row>
     <row r="165" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A165" s="5" t="s">
@@ -4140,7 +5153,9 @@
       <c r="D165" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E165" s="4"/>
+      <c r="E165" s="4" t="s">
+        <v>630</v>
+      </c>
     </row>
     <row r="166" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A166" s="5" t="s">
@@ -4155,7 +5170,9 @@
       <c r="D166" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E166" s="4"/>
+      <c r="E166" s="4" t="s">
+        <v>631</v>
+      </c>
     </row>
     <row r="167" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A167" s="5" t="s">
@@ -4170,7 +5187,9 @@
       <c r="D167" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E167" s="4"/>
+      <c r="E167" s="4" t="s">
+        <v>632</v>
+      </c>
     </row>
     <row r="168" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A168" s="5" t="s">
@@ -4185,7 +5204,9 @@
       <c r="D168" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E168" s="4"/>
+      <c r="E168" s="4" t="s">
+        <v>633</v>
+      </c>
     </row>
     <row r="169" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A169" s="7" t="s">
@@ -4200,7 +5221,9 @@
       <c r="D169" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="E169" s="4"/>
+      <c r="E169" s="4" t="s">
+        <v>634</v>
+      </c>
     </row>
     <row r="170" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A170" s="5" t="s">
@@ -4213,7 +5236,9 @@
         <v>52</v>
       </c>
       <c r="D170" s="1"/>
-      <c r="E170" s="4"/>
+      <c r="E170" s="4" t="s">
+        <v>635</v>
+      </c>
     </row>
     <row r="171" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A171" s="5" t="s">
@@ -4226,7 +5251,9 @@
         <v>52</v>
       </c>
       <c r="D171" s="1"/>
-      <c r="E171" s="4"/>
+      <c r="E171" s="4" t="s">
+        <v>636</v>
+      </c>
     </row>
     <row r="172" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A172" s="5" t="s">
@@ -4239,7 +5266,9 @@
         <v>52</v>
       </c>
       <c r="D172" s="1"/>
-      <c r="E172" s="4"/>
+      <c r="E172" s="4" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="173" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A173" s="5" t="s">
@@ -4252,7 +5281,9 @@
         <v>52</v>
       </c>
       <c r="D173" s="1"/>
-      <c r="E173" s="4"/>
+      <c r="E173" s="4" t="s">
+        <v>638</v>
+      </c>
     </row>
     <row r="174" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A174" s="5" t="s">
@@ -4265,7 +5296,9 @@
         <v>52</v>
       </c>
       <c r="D174" s="1"/>
-      <c r="E174" s="4"/>
+      <c r="E174" s="4" t="s">
+        <v>639</v>
+      </c>
     </row>
     <row r="175" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A175" s="5" t="s">
@@ -4278,7 +5311,9 @@
         <v>52</v>
       </c>
       <c r="D175" s="1"/>
-      <c r="E175" s="4"/>
+      <c r="E175" s="4" t="s">
+        <v>640</v>
+      </c>
     </row>
     <row r="176" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A176" s="5" t="s">
@@ -4291,7 +5326,9 @@
         <v>52</v>
       </c>
       <c r="D176" s="1"/>
-      <c r="E176" s="4"/>
+      <c r="E176" s="4" t="s">
+        <v>641</v>
+      </c>
     </row>
     <row r="177" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A177" s="5" t="s">
@@ -4304,7 +5341,9 @@
         <v>52</v>
       </c>
       <c r="D177" s="1"/>
-      <c r="E177" s="4"/>
+      <c r="E177" s="4" t="s">
+        <v>642</v>
+      </c>
     </row>
     <row r="178" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A178" s="5" t="s">
@@ -4317,7 +5356,9 @@
         <v>52</v>
       </c>
       <c r="D178" s="1"/>
-      <c r="E178" s="4"/>
+      <c r="E178" s="4" t="s">
+        <v>643</v>
+      </c>
     </row>
     <row r="179" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A179" s="5" t="s">
@@ -4330,7 +5371,9 @@
         <v>52</v>
       </c>
       <c r="D179" s="1"/>
-      <c r="E179" s="4"/>
+      <c r="E179" s="4" t="s">
+        <v>644</v>
+      </c>
     </row>
     <row r="180" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A180" s="5" t="s">
@@ -4343,7 +5386,9 @@
         <v>52</v>
       </c>
       <c r="D180" s="1"/>
-      <c r="E180" s="4"/>
+      <c r="E180" s="4" t="s">
+        <v>645</v>
+      </c>
     </row>
     <row r="181" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A181" s="5" t="s">
@@ -4356,7 +5401,9 @@
         <v>52</v>
       </c>
       <c r="D181" s="1"/>
-      <c r="E181" s="4"/>
+      <c r="E181" s="4" t="s">
+        <v>646</v>
+      </c>
     </row>
     <row r="182" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A182" s="5" t="s">
@@ -4369,7 +5416,9 @@
         <v>52</v>
       </c>
       <c r="D182" s="1"/>
-      <c r="E182" s="4"/>
+      <c r="E182" s="4" t="s">
+        <v>647</v>
+      </c>
     </row>
     <row r="183" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A183" s="7" t="s">
@@ -4382,7 +5431,9 @@
         <v>52</v>
       </c>
       <c r="D183" s="1"/>
-      <c r="E183" s="4"/>
+      <c r="E183" s="4" t="s">
+        <v>648</v>
+      </c>
     </row>
     <row r="184" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A184" s="5" t="s">
@@ -4397,7 +5448,9 @@
       <c r="D184" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E184" s="4"/>
+      <c r="E184" s="4" t="s">
+        <v>649</v>
+      </c>
     </row>
     <row r="185" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A185" s="5" t="s">
@@ -4412,7 +5465,9 @@
       <c r="D185" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E185" s="4"/>
+      <c r="E185" s="4" t="s">
+        <v>650</v>
+      </c>
     </row>
     <row r="186" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A186" s="5" t="s">
@@ -4427,7 +5482,9 @@
       <c r="D186" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E186" s="4"/>
+      <c r="E186" s="4" t="s">
+        <v>651</v>
+      </c>
     </row>
     <row r="187" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A187" s="5" t="s">
@@ -4442,7 +5499,9 @@
       <c r="D187" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E187" s="4"/>
+      <c r="E187" s="4" t="s">
+        <v>652</v>
+      </c>
     </row>
     <row r="188" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A188" s="5" t="s">
@@ -4457,7 +5516,9 @@
       <c r="D188" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E188" s="4"/>
+      <c r="E188" s="4" t="s">
+        <v>653</v>
+      </c>
     </row>
     <row r="189" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A189" s="5" t="s">
@@ -4472,7 +5533,9 @@
       <c r="D189" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E189" s="4"/>
+      <c r="E189" s="4" t="s">
+        <v>654</v>
+      </c>
     </row>
     <row r="190" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A190" s="5" t="s">
@@ -4487,7 +5550,9 @@
       <c r="D190" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E190" s="4"/>
+      <c r="E190" s="4" t="s">
+        <v>655</v>
+      </c>
     </row>
     <row r="191" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A191" s="5" t="s">
@@ -4502,7 +5567,9 @@
       <c r="D191" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E191" s="4"/>
+      <c r="E191" s="4" t="s">
+        <v>656</v>
+      </c>
     </row>
     <row r="192" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A192" s="5" t="s">
@@ -4517,7 +5584,9 @@
       <c r="D192" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E192" s="4"/>
+      <c r="E192" s="4" t="s">
+        <v>657</v>
+      </c>
     </row>
     <row r="193" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A193" s="5" t="s">
@@ -4532,7 +5601,9 @@
       <c r="D193" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E193" s="4"/>
+      <c r="E193" s="4" t="s">
+        <v>658</v>
+      </c>
     </row>
     <row r="194" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A194" s="5" t="s">
@@ -4547,7 +5618,9 @@
       <c r="D194" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E194" s="4"/>
+      <c r="E194" s="4" t="s">
+        <v>659</v>
+      </c>
     </row>
     <row r="195" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A195" s="5" t="s">
@@ -4562,7 +5635,9 @@
       <c r="D195" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E195" s="4"/>
+      <c r="E195" s="4" t="s">
+        <v>660</v>
+      </c>
     </row>
     <row r="196" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A196" s="5" t="s">
@@ -4577,7 +5652,9 @@
       <c r="D196" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E196" s="4"/>
+      <c r="E196" s="4" t="s">
+        <v>661</v>
+      </c>
     </row>
     <row r="197" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A197" s="7" t="s">
@@ -4592,7 +5669,9 @@
       <c r="D197" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E197" s="4"/>
+      <c r="E197" s="4" t="s">
+        <v>662</v>
+      </c>
     </row>
     <row r="198" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A198" s="5" t="s">
@@ -4607,7 +5686,9 @@
       <c r="D198" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E198" s="4"/>
+      <c r="E198" s="4" t="s">
+        <v>663</v>
+      </c>
     </row>
     <row r="199" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A199" s="5" t="s">
@@ -4622,7 +5703,9 @@
       <c r="D199" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E199" s="4"/>
+      <c r="E199" s="4" t="s">
+        <v>664</v>
+      </c>
     </row>
     <row r="200" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A200" s="5" t="s">
@@ -4637,7 +5720,9 @@
       <c r="D200" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E200" s="4"/>
+      <c r="E200" s="4" t="s">
+        <v>665</v>
+      </c>
     </row>
     <row r="201" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A201" s="5" t="s">
@@ -4652,7 +5737,9 @@
       <c r="D201" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E201" s="4"/>
+      <c r="E201" s="4" t="s">
+        <v>666</v>
+      </c>
     </row>
     <row r="202" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A202" s="5" t="s">
@@ -4667,7 +5754,9 @@
       <c r="D202" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E202" s="4"/>
+      <c r="E202" s="4" t="s">
+        <v>667</v>
+      </c>
     </row>
     <row r="203" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A203" s="5" t="s">
@@ -4682,7 +5771,9 @@
       <c r="D203" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E203" s="4"/>
+      <c r="E203" s="4" t="s">
+        <v>668</v>
+      </c>
     </row>
     <row r="204" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A204" s="5" t="s">
@@ -4697,7 +5788,9 @@
       <c r="D204" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E204" s="4"/>
+      <c r="E204" s="4" t="s">
+        <v>669</v>
+      </c>
     </row>
     <row r="205" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A205" s="5" t="s">
@@ -4712,7 +5805,9 @@
       <c r="D205" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E205" s="4"/>
+      <c r="E205" s="4" t="s">
+        <v>670</v>
+      </c>
     </row>
     <row r="206" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A206" s="5" t="s">
@@ -4727,7 +5822,9 @@
       <c r="D206" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E206" s="4"/>
+      <c r="E206" s="4" t="s">
+        <v>671</v>
+      </c>
     </row>
     <row r="207" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A207" s="5" t="s">
@@ -4742,7 +5839,9 @@
       <c r="D207" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E207" s="4"/>
+      <c r="E207" s="4" t="s">
+        <v>672</v>
+      </c>
     </row>
     <row r="208" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A208" s="5" t="s">
@@ -4757,7 +5856,9 @@
       <c r="D208" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E208" s="4"/>
+      <c r="E208" s="4" t="s">
+        <v>673</v>
+      </c>
     </row>
     <row r="209" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A209" s="5" t="s">
@@ -4772,7 +5873,9 @@
       <c r="D209" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E209" s="4"/>
+      <c r="E209" s="4" t="s">
+        <v>674</v>
+      </c>
     </row>
     <row r="210" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A210" s="5" t="s">
@@ -4787,7 +5890,9 @@
       <c r="D210" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E210" s="4"/>
+      <c r="E210" s="4" t="s">
+        <v>675</v>
+      </c>
     </row>
     <row r="211" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A211" s="7" t="s">
@@ -4802,7 +5907,9 @@
       <c r="D211" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E211" s="4"/>
+      <c r="E211" s="4" t="s">
+        <v>676</v>
+      </c>
     </row>
     <row r="212" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A212" s="5" t="s">
@@ -4817,7 +5924,9 @@
       <c r="D212" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E212" s="4"/>
+      <c r="E212" s="4" t="s">
+        <v>677</v>
+      </c>
     </row>
     <row r="213" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A213" s="5" t="s">
@@ -4832,7 +5941,9 @@
       <c r="D213" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E213" s="4"/>
+      <c r="E213" s="4" t="s">
+        <v>678</v>
+      </c>
     </row>
     <row r="214" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A214" s="5" t="s">
@@ -4847,7 +5958,9 @@
       <c r="D214" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E214" s="4"/>
+      <c r="E214" s="4" t="s">
+        <v>679</v>
+      </c>
     </row>
     <row r="215" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A215" s="5" t="s">
@@ -4862,7 +5975,9 @@
       <c r="D215" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E215" s="4"/>
+      <c r="E215" s="4" t="s">
+        <v>680</v>
+      </c>
     </row>
     <row r="216" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A216" s="5" t="s">
@@ -4877,7 +5992,9 @@
       <c r="D216" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E216" s="4"/>
+      <c r="E216" s="4" t="s">
+        <v>681</v>
+      </c>
     </row>
     <row r="217" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A217" s="5" t="s">
@@ -4892,7 +6009,9 @@
       <c r="D217" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E217" s="4"/>
+      <c r="E217" s="4" t="s">
+        <v>682</v>
+      </c>
     </row>
     <row r="218" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A218" s="5" t="s">
@@ -4907,7 +6026,9 @@
       <c r="D218" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E218" s="4"/>
+      <c r="E218" s="4" t="s">
+        <v>683</v>
+      </c>
     </row>
     <row r="219" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A219" s="5" t="s">
@@ -4922,7 +6043,9 @@
       <c r="D219" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E219" s="4"/>
+      <c r="E219" s="4" t="s">
+        <v>684</v>
+      </c>
     </row>
     <row r="220" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A220" s="5" t="s">
@@ -4937,7 +6060,9 @@
       <c r="D220" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E220" s="11"/>
+      <c r="E220" s="11" t="s">
+        <v>685</v>
+      </c>
     </row>
     <row r="221" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A221" s="5" t="s">
@@ -4952,7 +6077,9 @@
       <c r="D221" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E221" s="4"/>
+      <c r="E221" s="4" t="s">
+        <v>686</v>
+      </c>
     </row>
     <row r="222" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A222" s="5" t="s">
@@ -4967,7 +6094,9 @@
       <c r="D222" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E222" s="4"/>
+      <c r="E222" s="4" t="s">
+        <v>687</v>
+      </c>
     </row>
     <row r="223" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A223" s="5" t="s">
@@ -4982,7 +6111,9 @@
       <c r="D223" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E223" s="4"/>
+      <c r="E223" s="4" t="s">
+        <v>688</v>
+      </c>
     </row>
     <row r="224" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A224" s="5" t="s">
@@ -4997,7 +6128,9 @@
       <c r="D224" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E224" s="4"/>
+      <c r="E224" s="4" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="225" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A225" s="7" t="s">
@@ -5012,7 +6145,9 @@
       <c r="D225" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E225" s="4"/>
+      <c r="E225" s="4" t="s">
+        <v>690</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2">

</xml_diff>

<commit_message>
Updated data models for cleaner challenge creation
</commit_message>
<xml_diff>
--- a/models/mock-data/FakeUsers.xlsx
+++ b/models/mock-data/FakeUsers.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1180" windowWidth="28160" windowHeight="15220" tabRatio="500"/>
+    <workbookView xWindow="28800" yWindow="-4600" windowWidth="51200" windowHeight="26740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1012" uniqueCount="691">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1017" uniqueCount="694">
   <si>
     <t>Spot</t>
   </si>
@@ -2097,6 +2097,15 @@
   </si>
   <si>
     <t xml:space="preserve"> Krebsbach.938</t>
+  </si>
+  <si>
+    <t>A5</t>
+  </si>
+  <si>
+    <t>Kyle Thompson</t>
+  </si>
+  <si>
+    <t>Thompson.1234</t>
   </si>
 </sst>
 </file>
@@ -2231,27 +2240,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2535,10 +2524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E225"/>
+  <dimension ref="A1:E226"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="E6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2637,78 +2626,78 @@
     </row>
     <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>11</v>
+        <v>691</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>249</v>
+        <v>692</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>471</v>
+        <v>693</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>5</v>
@@ -2717,117 +2706,117 @@
         <v>10</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B14" s="6" t="s">
         <v>256</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="6" t="s">
+      <c r="C14" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E14" s="4" t="s">
         <v>478</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+    <row r="15" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B15" s="8" t="s">
         <v>257</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="8" t="s">
+      <c r="C15" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E15" s="4" t="s">
         <v>479</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>258</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>480</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>5</v>
@@ -2836,32 +2825,32 @@
         <v>23</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>5</v>
@@ -2870,49 +2859,49 @@
         <v>21</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>5</v>
@@ -2921,15 +2910,15 @@
         <v>21</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>5</v>
@@ -2938,32 +2927,32 @@
         <v>21</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>5</v>
@@ -2972,15 +2961,15 @@
         <v>23</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>5</v>
@@ -2989,15 +2978,15 @@
         <v>23</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>5</v>
@@ -3006,66 +2995,66 @@
         <v>23</v>
       </c>
       <c r="E27" s="4" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E28" s="4" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A28" s="7" t="s">
+    <row r="29" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="B29" s="8" t="s">
         <v>271</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D28" s="8" t="s">
+      <c r="C29" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="E29" s="4" t="s">
         <v>493</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>272</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>494</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D30" s="9" t="s">
+      <c r="D30" s="6" t="s">
         <v>37</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>5</v>
@@ -3074,15 +3063,15 @@
         <v>37</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>5</v>
@@ -3091,15 +3080,15 @@
         <v>37</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>5</v>
@@ -3108,15 +3097,15 @@
         <v>37</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>5</v>
@@ -3125,15 +3114,15 @@
         <v>37</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>5</v>
@@ -3142,15 +3131,15 @@
         <v>37</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>5</v>
@@ -3159,15 +3148,15 @@
         <v>37</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>5</v>
@@ -3176,15 +3165,15 @@
         <v>37</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>5</v>
@@ -3193,15 +3182,15 @@
         <v>37</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>5</v>
@@ -3210,15 +3199,15 @@
         <v>37</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>5</v>
@@ -3227,15 +3216,15 @@
         <v>37</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>5</v>
@@ -3244,293 +3233,293 @@
         <v>37</v>
       </c>
       <c r="E41" s="4" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E42" s="4" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A42" s="7" t="s">
+    <row r="43" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A43" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B42" s="8" t="s">
+      <c r="B43" s="8" t="s">
         <v>285</v>
       </c>
-      <c r="C42" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D42" s="10" t="s">
+      <c r="C43" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D43" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E42" s="4" t="s">
+      <c r="E43" s="4" t="s">
         <v>507</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A43" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B43" s="6" t="s">
-        <v>286</v>
-      </c>
-      <c r="C43" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D43" s="6"/>
-      <c r="E43" s="4" t="s">
-        <v>508</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C44" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D44" s="6"/>
       <c r="E44" s="4" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C45" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D45" s="6"/>
       <c r="E45" s="4" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C46" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D46" s="6"/>
       <c r="E46" s="4" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C47" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D47" s="6"/>
       <c r="E47" s="4" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C48" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D48" s="6"/>
       <c r="E48" s="4" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C49" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D49" s="6"/>
       <c r="E49" s="4" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C50" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D50" s="6"/>
       <c r="E50" s="4" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C51" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D51" s="6"/>
       <c r="E51" s="4" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C52" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D52" s="6"/>
       <c r="E52" s="4" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C53" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D53" s="6"/>
       <c r="E53" s="4" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C54" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D54" s="6"/>
       <c r="E54" s="4" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C55" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D55" s="6"/>
       <c r="E55" s="4" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A56" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="B56" s="8" t="s">
-        <v>299</v>
+      <c r="A56" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>298</v>
       </c>
       <c r="C56" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D56" s="8"/>
+      <c r="D56" s="6"/>
       <c r="E56" s="4" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A57" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B57" s="8" t="s">
+        <v>299</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D57" s="8"/>
+      <c r="E57" s="4" t="s">
         <v>521</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A57" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="B57" s="6" t="s">
-        <v>300</v>
-      </c>
-      <c r="C57" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D57" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="E57" s="4" t="s">
-        <v>522</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C58" s="6" t="s">
         <v>67</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>23</v>
+        <v>68</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C59" s="6" t="s">
         <v>67</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C60" s="6" t="s">
         <v>67</v>
@@ -3539,1596 +3528,1596 @@
         <v>21</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C61" s="6" t="s">
         <v>67</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C62" s="6" t="s">
         <v>67</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>68</v>
+        <v>23</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
-        <v>234</v>
+        <v>73</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C63" s="6" t="s">
         <v>67</v>
       </c>
       <c r="D63" s="6" t="s">
-        <v>21</v>
+        <v>68</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
-        <v>74</v>
+        <v>234</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C64" s="6" t="s">
         <v>67</v>
       </c>
       <c r="D64" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C65" s="6" t="s">
         <v>67</v>
       </c>
       <c r="D65" s="6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C66" s="6" t="s">
         <v>67</v>
       </c>
       <c r="D66" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C67" s="6" t="s">
         <v>67</v>
       </c>
       <c r="D67" s="6" t="s">
-        <v>68</v>
+        <v>23</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C68" s="6" t="s">
         <v>67</v>
       </c>
       <c r="D68" s="6" t="s">
-        <v>23</v>
+        <v>68</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C69" s="6" t="s">
         <v>67</v>
       </c>
       <c r="D69" s="6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A70" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="B70" s="8" t="s">
-        <v>313</v>
+      <c r="A70" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B70" s="6" t="s">
+        <v>312</v>
       </c>
       <c r="C70" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="D70" s="8" t="s">
+      <c r="D70" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E70" s="4" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A71" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B71" s="8" t="s">
+        <v>313</v>
+      </c>
+      <c r="C71" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D71" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E70" s="4" t="s">
+      <c r="E71" s="4" t="s">
         <v>535</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A71" s="5" t="s">
-        <v>235</v>
-      </c>
-      <c r="B71" s="6" t="s">
-        <v>314</v>
-      </c>
-      <c r="C71" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="D71" s="6"/>
-      <c r="E71" s="4" t="s">
-        <v>536</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
-        <v>81</v>
+        <v>235</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C72" s="6" t="s">
         <v>82</v>
       </c>
       <c r="D72" s="6"/>
       <c r="E72" s="4" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C73" s="6" t="s">
         <v>82</v>
       </c>
       <c r="D73" s="6"/>
       <c r="E73" s="4" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C74" s="6" t="s">
         <v>82</v>
       </c>
       <c r="D74" s="6"/>
       <c r="E74" s="4" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C75" s="6" t="s">
         <v>82</v>
       </c>
       <c r="D75" s="6"/>
       <c r="E75" s="4" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C76" s="6" t="s">
         <v>82</v>
       </c>
       <c r="D76" s="6"/>
       <c r="E76" s="4" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B77" s="6" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C77" s="6" t="s">
         <v>82</v>
       </c>
       <c r="D77" s="6"/>
       <c r="E77" s="4" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C78" s="6" t="s">
         <v>82</v>
       </c>
       <c r="D78" s="6"/>
       <c r="E78" s="4" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C79" s="6" t="s">
         <v>82</v>
       </c>
       <c r="D79" s="6"/>
       <c r="E79" s="4" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C80" s="6" t="s">
         <v>82</v>
       </c>
       <c r="D80" s="6"/>
       <c r="E80" s="4" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C81" s="6" t="s">
         <v>82</v>
       </c>
       <c r="D81" s="6"/>
       <c r="E81" s="4" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C82" s="6" t="s">
         <v>82</v>
       </c>
       <c r="D82" s="6"/>
       <c r="E82" s="4" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C83" s="6" t="s">
         <v>82</v>
       </c>
       <c r="D83" s="6"/>
       <c r="E83" s="4" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A84" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="B84" s="8" t="s">
-        <v>327</v>
+      <c r="A84" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B84" s="6" t="s">
+        <v>326</v>
       </c>
       <c r="C84" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="D84" s="8"/>
+      <c r="D84" s="6"/>
       <c r="E84" s="4" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A85" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B85" s="8" t="s">
+        <v>327</v>
+      </c>
+      <c r="C85" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D85" s="8"/>
+      <c r="E85" s="4" t="s">
         <v>549</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A85" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="B85" s="6" t="s">
-        <v>328</v>
-      </c>
-      <c r="C85" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="D85" s="6"/>
-      <c r="E85" s="4" t="s">
-        <v>550</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C86" s="6" t="s">
         <v>96</v>
       </c>
       <c r="D86" s="6"/>
       <c r="E86" s="4" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C87" s="6" t="s">
         <v>96</v>
       </c>
       <c r="D87" s="6"/>
       <c r="E87" s="4" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C88" s="6" t="s">
         <v>96</v>
       </c>
       <c r="D88" s="6"/>
       <c r="E88" s="4" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C89" s="6" t="s">
         <v>96</v>
       </c>
       <c r="D89" s="6"/>
       <c r="E89" s="4" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C90" s="6" t="s">
         <v>96</v>
       </c>
       <c r="D90" s="6"/>
       <c r="E90" s="4" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B91" s="6" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C91" s="6" t="s">
         <v>96</v>
       </c>
       <c r="D91" s="6"/>
       <c r="E91" s="4" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B92" s="6" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C92" s="6" t="s">
         <v>96</v>
       </c>
       <c r="D92" s="6"/>
       <c r="E92" s="4" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B93" s="6" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C93" s="6" t="s">
         <v>96</v>
       </c>
       <c r="D93" s="6"/>
       <c r="E93" s="4" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B94" s="6" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C94" s="6" t="s">
         <v>96</v>
       </c>
       <c r="D94" s="6"/>
       <c r="E94" s="4" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C95" s="6" t="s">
         <v>96</v>
       </c>
       <c r="D95" s="6"/>
       <c r="E95" s="4" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B96" s="6" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C96" s="6" t="s">
         <v>96</v>
       </c>
       <c r="D96" s="6"/>
       <c r="E96" s="4" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
-        <v>236</v>
+        <v>107</v>
       </c>
       <c r="B97" s="6" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C97" s="6" t="s">
         <v>96</v>
       </c>
       <c r="D97" s="6"/>
       <c r="E97" s="4" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A98" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="B98" s="8" t="s">
-        <v>341</v>
+      <c r="A98" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="B98" s="6" t="s">
+        <v>340</v>
       </c>
       <c r="C98" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="D98" s="8"/>
+      <c r="D98" s="6"/>
       <c r="E98" s="4" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A99" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="B99" s="8" t="s">
+        <v>341</v>
+      </c>
+      <c r="C99" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="D99" s="8"/>
+      <c r="E99" s="4" t="s">
         <v>563</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A99" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="B99" s="6" t="s">
-        <v>342</v>
-      </c>
-      <c r="C99" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D99" s="6"/>
-      <c r="E99" s="4" t="s">
-        <v>564</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
-        <v>237</v>
+        <v>109</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C100" s="6" t="s">
-        <v>68</v>
+        <v>110</v>
       </c>
       <c r="D100" s="6"/>
       <c r="E100" s="4" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="101" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
-        <v>111</v>
+        <v>237</v>
       </c>
       <c r="B101" s="6" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C101" s="6" t="s">
         <v>68</v>
       </c>
       <c r="D101" s="6"/>
       <c r="E101" s="4" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B102" s="6" t="s">
-        <v>242</v>
+        <v>344</v>
       </c>
       <c r="C102" s="6" t="s">
-        <v>113</v>
+        <v>68</v>
       </c>
       <c r="D102" s="6"/>
       <c r="E102" s="4" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="103" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B103" s="6" t="s">
-        <v>345</v>
+        <v>242</v>
       </c>
       <c r="C103" s="6" t="s">
         <v>113</v>
       </c>
       <c r="D103" s="6"/>
       <c r="E103" s="4" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="104" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B104" s="6" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C104" s="6" t="s">
-        <v>68</v>
+        <v>113</v>
       </c>
       <c r="D104" s="6"/>
       <c r="E104" s="4" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="105" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B105" s="6" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C105" s="6" t="s">
         <v>68</v>
       </c>
       <c r="D105" s="6"/>
       <c r="E105" s="4" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="106" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B106" s="6" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C106" s="6" t="s">
-        <v>113</v>
+        <v>68</v>
       </c>
       <c r="D106" s="6"/>
       <c r="E106" s="4" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="107" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B107" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C107" s="6" t="s">
         <v>113</v>
       </c>
       <c r="D107" s="6"/>
       <c r="E107" s="4" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="108" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B108" s="6" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C108" s="6" t="s">
-        <v>68</v>
+        <v>113</v>
       </c>
       <c r="D108" s="6"/>
       <c r="E108" s="4" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="109" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B109" s="6" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C109" s="6" t="s">
-        <v>110</v>
+        <v>68</v>
       </c>
       <c r="D109" s="6"/>
       <c r="E109" s="4" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="110" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B110" s="6" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C110" s="6" t="s">
         <v>110</v>
       </c>
       <c r="D110" s="6"/>
       <c r="E110" s="4" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="111" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B111" s="6" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C111" s="6" t="s">
         <v>110</v>
       </c>
       <c r="D111" s="6"/>
       <c r="E111" s="4" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="112" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B112" s="6" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C112" s="6" t="s">
-        <v>68</v>
+        <v>110</v>
       </c>
       <c r="D112" s="6"/>
       <c r="E112" s="4" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A113" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B113" s="6" t="s">
+        <v>354</v>
+      </c>
+      <c r="C113" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D113" s="6"/>
+      <c r="E113" s="4" t="s">
         <v>577</v>
       </c>
     </row>
-    <row r="113" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A113" s="7" t="s">
+    <row r="114" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A114" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="B113" s="8" t="s">
+      <c r="B114" s="8" t="s">
         <v>355</v>
       </c>
-      <c r="C113" s="8" t="s">
+      <c r="C114" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="D113" s="8"/>
-      <c r="E113" s="4" t="s">
+      <c r="D114" s="8"/>
+      <c r="E114" s="4" t="s">
         <v>578</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A114" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="B114" s="6" t="s">
-        <v>356</v>
-      </c>
-      <c r="C114" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="D114" s="6"/>
-      <c r="E114" s="4" t="s">
-        <v>579</v>
       </c>
     </row>
     <row r="115" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B115" s="6" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C115" s="6" t="s">
         <v>126</v>
       </c>
       <c r="D115" s="6"/>
       <c r="E115" s="4" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="116" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B116" s="6" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C116" s="6" t="s">
         <v>126</v>
       </c>
       <c r="D116" s="6"/>
       <c r="E116" s="4" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="117" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="s">
-        <v>238</v>
+        <v>128</v>
       </c>
       <c r="B117" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C117" s="6" t="s">
         <v>126</v>
       </c>
       <c r="D117" s="6"/>
       <c r="E117" s="4" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="118" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
-        <v>129</v>
+        <v>238</v>
       </c>
       <c r="B118" s="6" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C118" s="6" t="s">
         <v>126</v>
       </c>
       <c r="D118" s="6"/>
       <c r="E118" s="4" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="119" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A119" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B119" s="6" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C119" s="6" t="s">
         <v>126</v>
       </c>
       <c r="D119" s="6"/>
       <c r="E119" s="4" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="120" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A120" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B120" s="6" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C120" s="6" t="s">
         <v>126</v>
       </c>
       <c r="D120" s="6"/>
       <c r="E120" s="4" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="121" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B121" s="6" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C121" s="6" t="s">
         <v>126</v>
       </c>
       <c r="D121" s="6"/>
       <c r="E121" s="4" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="122" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A122" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B122" s="6" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C122" s="6" t="s">
         <v>126</v>
       </c>
       <c r="D122" s="6"/>
       <c r="E122" s="4" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="123" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B123" s="6" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C123" s="6" t="s">
         <v>126</v>
       </c>
       <c r="D123" s="6"/>
       <c r="E123" s="4" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="124" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B124" s="6" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C124" s="6" t="s">
         <v>126</v>
       </c>
       <c r="D124" s="6"/>
       <c r="E124" s="4" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="125" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B125" s="6" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C125" s="6" t="s">
         <v>126</v>
       </c>
       <c r="D125" s="6"/>
       <c r="E125" s="4" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="126" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B126" s="6" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C126" s="6" t="s">
         <v>126</v>
       </c>
       <c r="D126" s="6"/>
       <c r="E126" s="4" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="127" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A127" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="B127" s="8" t="s">
-        <v>369</v>
+      <c r="A127" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="B127" s="6" t="s">
+        <v>368</v>
       </c>
       <c r="C127" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="D127" s="8"/>
+      <c r="D127" s="6"/>
       <c r="E127" s="4" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="128" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A128" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="B128" s="6" t="s">
-        <v>370</v>
+      <c r="A128" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="B128" s="8" t="s">
+        <v>369</v>
       </c>
       <c r="C128" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="D128" s="6"/>
+      <c r="D128" s="8"/>
       <c r="E128" s="4" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="129" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A129" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B129" s="6" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C129" s="6" t="s">
         <v>126</v>
       </c>
       <c r="D129" s="6"/>
       <c r="E129" s="4" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="130" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B130" s="6" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C130" s="6" t="s">
         <v>126</v>
       </c>
       <c r="D130" s="6"/>
       <c r="E130" s="4" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="131" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A131" s="5" t="s">
-        <v>240</v>
+        <v>141</v>
       </c>
       <c r="B131" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C131" s="6" t="s">
         <v>126</v>
       </c>
       <c r="D131" s="6"/>
       <c r="E131" s="4" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="132" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A132" s="5" t="s">
-        <v>142</v>
+        <v>240</v>
       </c>
       <c r="B132" s="6" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C132" s="6" t="s">
         <v>126</v>
       </c>
       <c r="D132" s="6"/>
       <c r="E132" s="4" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="133" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A133" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B133" s="6" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C133" s="6" t="s">
         <v>126</v>
       </c>
       <c r="D133" s="6"/>
       <c r="E133" s="4" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="134" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A134" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B134" s="6" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C134" s="6" t="s">
         <v>126</v>
       </c>
       <c r="D134" s="6"/>
       <c r="E134" s="4" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="135" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A135" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B135" s="6" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C135" s="6" t="s">
         <v>126</v>
       </c>
       <c r="D135" s="6"/>
       <c r="E135" s="4" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="136" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A136" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B136" s="6" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C136" s="6" t="s">
         <v>126</v>
       </c>
       <c r="D136" s="6"/>
       <c r="E136" s="4" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="137" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A137" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B137" s="6" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C137" s="6" t="s">
         <v>126</v>
       </c>
       <c r="D137" s="6"/>
       <c r="E137" s="4" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="138" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A138" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B138" s="6" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C138" s="6" t="s">
         <v>126</v>
       </c>
       <c r="D138" s="6"/>
       <c r="E138" s="4" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="139" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A139" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B139" s="6" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C139" s="6" t="s">
         <v>126</v>
       </c>
       <c r="D139" s="6"/>
       <c r="E139" s="4" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="140" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A140" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B140" s="6" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C140" s="6" t="s">
         <v>126</v>
       </c>
       <c r="D140" s="6"/>
       <c r="E140" s="4" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="141" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A141" s="5" t="s">
-        <v>239</v>
+        <v>150</v>
       </c>
       <c r="B141" s="6" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C141" s="6" t="s">
         <v>126</v>
       </c>
       <c r="D141" s="6"/>
       <c r="E141" s="4" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="142" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A142" s="5" t="s">
-        <v>151</v>
+        <v>239</v>
       </c>
       <c r="B142" s="6" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C142" s="6" t="s">
-        <v>82</v>
+        <v>126</v>
       </c>
       <c r="D142" s="6"/>
       <c r="E142" s="4" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="143" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A143" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B143" s="6" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C143" s="6" t="s">
         <v>82</v>
       </c>
       <c r="D143" s="6"/>
       <c r="E143" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="144" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A144" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B144" s="6" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C144" s="6" t="s">
         <v>82</v>
       </c>
       <c r="D144" s="6"/>
       <c r="E144" s="4" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="145" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A145" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B145" s="6" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C145" s="6" t="s">
         <v>82</v>
       </c>
       <c r="D145" s="6"/>
       <c r="E145" s="4" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="146" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A146" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B146" s="6" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C146" s="6" t="s">
         <v>82</v>
       </c>
       <c r="D146" s="6"/>
       <c r="E146" s="4" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="147" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A147" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B147" s="6" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C147" s="6" t="s">
         <v>82</v>
       </c>
       <c r="D147" s="6"/>
       <c r="E147" s="4" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="148" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A148" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B148" s="6" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C148" s="6" t="s">
         <v>82</v>
       </c>
       <c r="D148" s="6"/>
       <c r="E148" s="4" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="149" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A149" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B149" s="6" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C149" s="6" t="s">
         <v>82</v>
       </c>
       <c r="D149" s="6"/>
       <c r="E149" s="4" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="150" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A150" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B150" s="6" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C150" s="6" t="s">
         <v>82</v>
       </c>
       <c r="D150" s="6"/>
       <c r="E150" s="4" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="151" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A151" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B151" s="6" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C151" s="6" t="s">
         <v>82</v>
       </c>
       <c r="D151" s="6"/>
       <c r="E151" s="4" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="152" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A152" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B152" s="6" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C152" s="6" t="s">
         <v>82</v>
       </c>
       <c r="D152" s="6"/>
       <c r="E152" s="4" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="153" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A153" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B153" s="6" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C153" s="6" t="s">
         <v>82</v>
       </c>
       <c r="D153" s="6"/>
       <c r="E153" s="4" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="154" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A154" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B154" s="6" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C154" s="6" t="s">
         <v>82</v>
       </c>
       <c r="D154" s="6"/>
       <c r="E154" s="4" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="155" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A155" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="B155" s="8" t="s">
-        <v>397</v>
+      <c r="A155" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="B155" s="6" t="s">
+        <v>396</v>
       </c>
       <c r="C155" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="D155" s="8"/>
+      <c r="D155" s="6"/>
       <c r="E155" s="4" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A156" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="B156" s="8" t="s">
+        <v>397</v>
+      </c>
+      <c r="C156" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D156" s="8"/>
+      <c r="E156" s="4" t="s">
         <v>620</v>
-      </c>
-    </row>
-    <row r="156" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A156" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="B156" s="6" t="s">
-        <v>398</v>
-      </c>
-      <c r="C156" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D156" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E156" s="4" t="s">
-        <v>621</v>
       </c>
     </row>
     <row r="157" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A157" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B157" s="6" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C157" s="6" t="s">
         <v>67</v>
       </c>
       <c r="D157" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E157" s="4" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="158" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A158" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B158" s="6" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C158" s="6" t="s">
         <v>67</v>
       </c>
       <c r="D158" s="6" t="s">
-        <v>68</v>
+        <v>23</v>
       </c>
       <c r="E158" s="4" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="159" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A159" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B159" s="6" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C159" s="6" t="s">
         <v>67</v>
       </c>
       <c r="D159" s="6" t="s">
-        <v>21</v>
+        <v>68</v>
       </c>
       <c r="E159" s="4" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="160" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A160" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B160" s="6" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C160" s="6" t="s">
         <v>67</v>
       </c>
       <c r="D160" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E160" s="4" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="161" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A161" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B161" s="6" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C161" s="6" t="s">
         <v>67</v>
       </c>
       <c r="D161" s="6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E161" s="4" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="162" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A162" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B162" s="6" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C162" s="6" t="s">
         <v>67</v>
       </c>
       <c r="D162" s="6" t="s">
-        <v>68</v>
+        <v>21</v>
       </c>
       <c r="E162" s="4" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="163" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A163" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B163" s="6" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C163" s="6" t="s">
         <v>67</v>
       </c>
       <c r="D163" s="6" t="s">
-        <v>23</v>
+        <v>68</v>
       </c>
       <c r="E163" s="4" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="164" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A164" s="5" t="s">
-        <v>241</v>
+        <v>172</v>
       </c>
       <c r="B164" s="6" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C164" s="6" t="s">
         <v>67</v>
@@ -5137,15 +5126,15 @@
         <v>23</v>
       </c>
       <c r="E164" s="4" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="165" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A165" s="5" t="s">
-        <v>173</v>
+        <v>241</v>
       </c>
       <c r="B165" s="6" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C165" s="6" t="s">
         <v>67</v>
@@ -5154,548 +5143,548 @@
         <v>23</v>
       </c>
       <c r="E165" s="4" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="166" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A166" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B166" s="6" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C166" s="6" t="s">
         <v>67</v>
       </c>
       <c r="D166" s="6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E166" s="4" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="167" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A167" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B167" s="6" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C167" s="6" t="s">
         <v>67</v>
       </c>
       <c r="D167" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E167" s="4" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="168" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A168" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B168" s="6" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C168" s="6" t="s">
         <v>67</v>
       </c>
       <c r="D168" s="6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E168" s="4" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="169" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A169" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="B169" s="8" t="s">
-        <v>411</v>
+      <c r="A169" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="B169" s="6" t="s">
+        <v>410</v>
       </c>
       <c r="C169" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="D169" s="8" t="s">
+      <c r="D169" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E169" s="4" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A170" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="B170" s="8" t="s">
+        <v>411</v>
+      </c>
+      <c r="C170" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D170" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="E169" s="4" t="s">
+      <c r="E170" s="4" t="s">
         <v>634</v>
-      </c>
-    </row>
-    <row r="170" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A170" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="B170" s="6" t="s">
-        <v>412</v>
-      </c>
-      <c r="C170" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D170" s="1"/>
-      <c r="E170" s="4" t="s">
-        <v>635</v>
       </c>
     </row>
     <row r="171" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A171" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B171" s="6" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C171" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D171" s="1"/>
       <c r="E171" s="4" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="172" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A172" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B172" s="6" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C172" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D172" s="1"/>
       <c r="E172" s="4" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="173" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A173" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B173" s="6" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C173" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D173" s="1"/>
       <c r="E173" s="4" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="174" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A174" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B174" s="6" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C174" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D174" s="1"/>
       <c r="E174" s="4" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="175" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A175" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B175" s="6" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C175" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D175" s="1"/>
       <c r="E175" s="4" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="176" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A176" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B176" s="6" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C176" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D176" s="1"/>
       <c r="E176" s="4" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="177" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A177" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B177" s="6" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C177" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D177" s="1"/>
       <c r="E177" s="4" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="178" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A178" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B178" s="6" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C178" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D178" s="1"/>
       <c r="E178" s="4" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="179" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A179" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B179" s="6" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C179" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D179" s="1"/>
       <c r="E179" s="4" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="180" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A180" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B180" s="6" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C180" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D180" s="1"/>
       <c r="E180" s="4" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="181" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A181" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B181" s="6" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C181" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D181" s="1"/>
       <c r="E181" s="4" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="182" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A182" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B182" s="6" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C182" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D182" s="1"/>
       <c r="E182" s="4" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="183" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A183" s="7" t="s">
-        <v>191</v>
-      </c>
-      <c r="B183" s="8" t="s">
-        <v>425</v>
-      </c>
-      <c r="C183" s="8" t="s">
+      <c r="A183" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="B183" s="6" t="s">
+        <v>424</v>
+      </c>
+      <c r="C183" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D183" s="1"/>
       <c r="E183" s="4" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A184" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="B184" s="8" t="s">
+        <v>425</v>
+      </c>
+      <c r="C184" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D184" s="1"/>
+      <c r="E184" s="4" t="s">
         <v>648</v>
-      </c>
-    </row>
-    <row r="184" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A184" s="5" t="s">
-        <v>192</v>
-      </c>
-      <c r="B184" s="6" t="s">
-        <v>426</v>
-      </c>
-      <c r="C184" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D184" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E184" s="4" t="s">
-        <v>649</v>
       </c>
     </row>
     <row r="185" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A185" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B185" s="6" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C185" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D185" s="6" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="E185" s="4" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="186" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A186" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B186" s="6" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C186" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D186" s="6" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="E186" s="4" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="187" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A187" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B187" s="6" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C187" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D187" s="6" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="E187" s="4" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="188" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A188" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B188" s="6" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C188" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D188" s="6" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="E188" s="4" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="189" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A189" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B189" s="6" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C189" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D189" s="6" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="E189" s="4" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="190" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A190" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B190" s="6" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C190" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D190" s="6" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="E190" s="4" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="191" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A191" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B191" s="6" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C191" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D191" s="6" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="E191" s="4" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="192" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A192" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B192" s="6" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C192" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D192" s="6" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="E192" s="4" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="193" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A193" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B193" s="6" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C193" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D193" s="6" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="E193" s="4" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="194" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A194" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B194" s="6" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C194" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D194" s="6" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="E194" s="4" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="195" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A195" s="5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B195" s="6" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C195" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D195" s="6" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="E195" s="4" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="196" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A196" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="B196" s="6" t="s">
+        <v>437</v>
+      </c>
+      <c r="C196" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D196" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E196" s="4" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A197" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="B196" s="6" t="s">
+      <c r="B197" s="6" t="s">
         <v>438</v>
       </c>
-      <c r="C196" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D196" s="6" t="s">
+      <c r="C197" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D197" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E196" s="4" t="s">
+      <c r="E197" s="4" t="s">
         <v>661</v>
       </c>
     </row>
-    <row r="197" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A197" s="7" t="s">
+    <row r="198" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A198" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="B197" s="8" t="s">
+      <c r="B198" s="8" t="s">
         <v>439</v>
       </c>
-      <c r="C197" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D197" s="8" t="s">
+      <c r="C198" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D198" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E197" s="4" t="s">
+      <c r="E198" s="4" t="s">
         <v>662</v>
-      </c>
-    </row>
-    <row r="198" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A198" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="B198" s="6" t="s">
-        <v>440</v>
-      </c>
-      <c r="C198" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D198" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E198" s="4" t="s">
-        <v>663</v>
       </c>
     </row>
     <row r="199" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A199" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B199" s="6" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C199" s="6" t="s">
         <v>5</v>
@@ -5704,32 +5693,32 @@
         <v>21</v>
       </c>
       <c r="E199" s="4" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="200" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A200" s="5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B200" s="6" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C200" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D200" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E200" s="4" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="201" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A201" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B201" s="6" t="s">
-        <v>243</v>
+        <v>442</v>
       </c>
       <c r="C201" s="6" t="s">
         <v>5</v>
@@ -5738,49 +5727,49 @@
         <v>23</v>
       </c>
       <c r="E201" s="4" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="202" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A202" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B202" s="6" t="s">
-        <v>443</v>
+        <v>243</v>
       </c>
       <c r="C202" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D202" s="6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E202" s="4" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="203" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A203" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B203" s="6" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C203" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D203" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E203" s="4" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="204" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A204" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B204" s="6" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C204" s="6" t="s">
         <v>5</v>
@@ -5789,32 +5778,32 @@
         <v>23</v>
       </c>
       <c r="E204" s="4" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="205" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A205" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B205" s="6" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C205" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D205" s="6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E205" s="4" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="206" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A206" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B206" s="6" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C206" s="6" t="s">
         <v>5</v>
@@ -5823,151 +5812,151 @@
         <v>21</v>
       </c>
       <c r="E206" s="4" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="207" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A207" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B207" s="6" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C207" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D207" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E207" s="4" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="208" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A208" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B208" s="6" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C208" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D208" s="6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E208" s="4" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="209" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A209" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B209" s="6" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C209" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D209" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E209" s="4" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="210" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A210" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="B210" s="6" t="s">
+        <v>450</v>
+      </c>
+      <c r="C210" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D210" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E210" s="4" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A211" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="B210" s="6" t="s">
+      <c r="B211" s="6" t="s">
         <v>451</v>
       </c>
-      <c r="C210" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D210" s="6" t="s">
+      <c r="C211" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D211" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E210" s="4" t="s">
+      <c r="E211" s="4" t="s">
         <v>675</v>
       </c>
     </row>
-    <row r="211" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A211" s="7" t="s">
+    <row r="212" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A212" s="7" t="s">
         <v>219</v>
       </c>
-      <c r="B211" s="8" t="s">
+      <c r="B212" s="8" t="s">
         <v>452</v>
       </c>
-      <c r="C211" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D211" s="8" t="s">
+      <c r="C212" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D212" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E211" s="4" t="s">
+      <c r="E212" s="4" t="s">
         <v>676</v>
-      </c>
-    </row>
-    <row r="212" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A212" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="B212" s="6" t="s">
-        <v>453</v>
-      </c>
-      <c r="C212" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D212" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E212" s="4" t="s">
-        <v>677</v>
       </c>
     </row>
     <row r="213" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A213" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B213" s="6" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C213" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D213" s="6" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E213" s="4" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="214" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A214" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B214" s="6" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C214" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D214" s="6" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E214" s="4" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="215" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A215" s="5" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B215" s="6" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C215" s="6" t="s">
         <v>5</v>
@@ -5976,32 +5965,32 @@
         <v>10</v>
       </c>
       <c r="E215" s="4" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="216" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A216" s="5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B216" s="6" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C216" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D216" s="6" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E216" s="4" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="217" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A217" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B217" s="6" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C217" s="6" t="s">
         <v>5</v>
@@ -6010,49 +5999,49 @@
         <v>6</v>
       </c>
       <c r="E217" s="4" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="218" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A218" s="5" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B218" s="6" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C218" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D218" s="6" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E218" s="4" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="219" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A219" s="5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B219" s="6" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C219" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D219" s="6" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E219" s="4" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="220" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A220" s="5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B220" s="6" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C220" s="6" t="s">
         <v>5</v>
@@ -6060,16 +6049,16 @@
       <c r="D220" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E220" s="11" t="s">
-        <v>685</v>
+      <c r="E220" s="4" t="s">
+        <v>684</v>
       </c>
     </row>
     <row r="221" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A221" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B221" s="6" t="s">
-        <v>244</v>
+        <v>461</v>
       </c>
       <c r="C221" s="6" t="s">
         <v>5</v>
@@ -6077,50 +6066,50 @@
       <c r="D221" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E221" s="4" t="s">
-        <v>686</v>
+      <c r="E221" s="11" t="s">
+        <v>685</v>
       </c>
     </row>
     <row r="222" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A222" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B222" s="6" t="s">
-        <v>462</v>
+        <v>244</v>
       </c>
       <c r="C222" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D222" s="6" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E222" s="4" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="223" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A223" s="5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B223" s="6" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C223" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D223" s="6" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E223" s="4" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="224" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A224" s="5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B224" s="6" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C224" s="6" t="s">
         <v>5</v>
@@ -6129,29 +6118,46 @@
         <v>6</v>
       </c>
       <c r="E224" s="4" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A225" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="B225" s="6" t="s">
+        <v>464</v>
+      </c>
+      <c r="C225" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D225" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E225" s="4" t="s">
         <v>689</v>
       </c>
     </row>
-    <row r="225" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A225" s="7" t="s">
+    <row r="226" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A226" s="7" t="s">
         <v>233</v>
       </c>
-      <c r="B225" s="8" t="s">
+      <c r="B226" s="8" t="s">
         <v>465</v>
       </c>
-      <c r="C225" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D225" s="8" t="s">
+      <c r="C226" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D226" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E225" s="4" t="s">
+      <c r="E226" s="4" t="s">
         <v>690</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated data models for cleaner challenge creation (#25)
* Updated data models for cleaner challenge creation

* Edited controllers to reflect new data models

* Added basic routing for controllers and added blank spec files for each
</commit_message>
<xml_diff>
--- a/models/mock-data/FakeUsers.xlsx
+++ b/models/mock-data/FakeUsers.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1180" windowWidth="28160" windowHeight="15220" tabRatio="500"/>
+    <workbookView xWindow="28800" yWindow="-4600" windowWidth="51200" windowHeight="26740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1012" uniqueCount="691">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1017" uniqueCount="694">
   <si>
     <t>Spot</t>
   </si>
@@ -2097,6 +2097,15 @@
   </si>
   <si>
     <t xml:space="preserve"> Krebsbach.938</t>
+  </si>
+  <si>
+    <t>A5</t>
+  </si>
+  <si>
+    <t>Kyle Thompson</t>
+  </si>
+  <si>
+    <t>Thompson.1234</t>
   </si>
 </sst>
 </file>
@@ -2231,27 +2240,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2535,10 +2524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E225"/>
+  <dimension ref="A1:E226"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="E6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2637,78 +2626,78 @@
     </row>
     <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>11</v>
+        <v>691</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>249</v>
+        <v>692</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>471</v>
+        <v>693</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>5</v>
@@ -2717,117 +2706,117 @@
         <v>10</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B14" s="6" t="s">
         <v>256</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="6" t="s">
+      <c r="C14" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E14" s="4" t="s">
         <v>478</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+    <row r="15" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B15" s="8" t="s">
         <v>257</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="8" t="s">
+      <c r="C15" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E15" s="4" t="s">
         <v>479</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>258</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>480</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>5</v>
@@ -2836,32 +2825,32 @@
         <v>23</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>5</v>
@@ -2870,49 +2859,49 @@
         <v>21</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>5</v>
@@ -2921,15 +2910,15 @@
         <v>21</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>5</v>
@@ -2938,32 +2927,32 @@
         <v>21</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>5</v>
@@ -2972,15 +2961,15 @@
         <v>23</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>5</v>
@@ -2989,15 +2978,15 @@
         <v>23</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>5</v>
@@ -3006,66 +2995,66 @@
         <v>23</v>
       </c>
       <c r="E27" s="4" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E28" s="4" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A28" s="7" t="s">
+    <row r="29" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="B29" s="8" t="s">
         <v>271</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D28" s="8" t="s">
+      <c r="C29" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="E29" s="4" t="s">
         <v>493</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>272</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>494</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D30" s="9" t="s">
+      <c r="D30" s="6" t="s">
         <v>37</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>5</v>
@@ -3074,15 +3063,15 @@
         <v>37</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>5</v>
@@ -3091,15 +3080,15 @@
         <v>37</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>5</v>
@@ -3108,15 +3097,15 @@
         <v>37</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>5</v>
@@ -3125,15 +3114,15 @@
         <v>37</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>5</v>
@@ -3142,15 +3131,15 @@
         <v>37</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>5</v>
@@ -3159,15 +3148,15 @@
         <v>37</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>5</v>
@@ -3176,15 +3165,15 @@
         <v>37</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>5</v>
@@ -3193,15 +3182,15 @@
         <v>37</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>5</v>
@@ -3210,15 +3199,15 @@
         <v>37</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>5</v>
@@ -3227,15 +3216,15 @@
         <v>37</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>5</v>
@@ -3244,293 +3233,293 @@
         <v>37</v>
       </c>
       <c r="E41" s="4" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E42" s="4" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A42" s="7" t="s">
+    <row r="43" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A43" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B42" s="8" t="s">
+      <c r="B43" s="8" t="s">
         <v>285</v>
       </c>
-      <c r="C42" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D42" s="10" t="s">
+      <c r="C43" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D43" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E42" s="4" t="s">
+      <c r="E43" s="4" t="s">
         <v>507</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A43" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B43" s="6" t="s">
-        <v>286</v>
-      </c>
-      <c r="C43" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D43" s="6"/>
-      <c r="E43" s="4" t="s">
-        <v>508</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C44" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D44" s="6"/>
       <c r="E44" s="4" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C45" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D45" s="6"/>
       <c r="E45" s="4" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C46" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D46" s="6"/>
       <c r="E46" s="4" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C47" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D47" s="6"/>
       <c r="E47" s="4" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C48" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D48" s="6"/>
       <c r="E48" s="4" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C49" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D49" s="6"/>
       <c r="E49" s="4" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C50" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D50" s="6"/>
       <c r="E50" s="4" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C51" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D51" s="6"/>
       <c r="E51" s="4" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C52" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D52" s="6"/>
       <c r="E52" s="4" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C53" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D53" s="6"/>
       <c r="E53" s="4" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C54" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D54" s="6"/>
       <c r="E54" s="4" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C55" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D55" s="6"/>
       <c r="E55" s="4" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A56" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="B56" s="8" t="s">
-        <v>299</v>
+      <c r="A56" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>298</v>
       </c>
       <c r="C56" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D56" s="8"/>
+      <c r="D56" s="6"/>
       <c r="E56" s="4" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A57" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B57" s="8" t="s">
+        <v>299</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D57" s="8"/>
+      <c r="E57" s="4" t="s">
         <v>521</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A57" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="B57" s="6" t="s">
-        <v>300</v>
-      </c>
-      <c r="C57" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D57" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="E57" s="4" t="s">
-        <v>522</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C58" s="6" t="s">
         <v>67</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>23</v>
+        <v>68</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C59" s="6" t="s">
         <v>67</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C60" s="6" t="s">
         <v>67</v>
@@ -3539,1596 +3528,1596 @@
         <v>21</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C61" s="6" t="s">
         <v>67</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C62" s="6" t="s">
         <v>67</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>68</v>
+        <v>23</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
-        <v>234</v>
+        <v>73</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C63" s="6" t="s">
         <v>67</v>
       </c>
       <c r="D63" s="6" t="s">
-        <v>21</v>
+        <v>68</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
-        <v>74</v>
+        <v>234</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C64" s="6" t="s">
         <v>67</v>
       </c>
       <c r="D64" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C65" s="6" t="s">
         <v>67</v>
       </c>
       <c r="D65" s="6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C66" s="6" t="s">
         <v>67</v>
       </c>
       <c r="D66" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C67" s="6" t="s">
         <v>67</v>
       </c>
       <c r="D67" s="6" t="s">
-        <v>68</v>
+        <v>23</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C68" s="6" t="s">
         <v>67</v>
       </c>
       <c r="D68" s="6" t="s">
-        <v>23</v>
+        <v>68</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C69" s="6" t="s">
         <v>67</v>
       </c>
       <c r="D69" s="6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A70" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="B70" s="8" t="s">
-        <v>313</v>
+      <c r="A70" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B70" s="6" t="s">
+        <v>312</v>
       </c>
       <c r="C70" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="D70" s="8" t="s">
+      <c r="D70" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E70" s="4" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A71" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B71" s="8" t="s">
+        <v>313</v>
+      </c>
+      <c r="C71" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D71" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E70" s="4" t="s">
+      <c r="E71" s="4" t="s">
         <v>535</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A71" s="5" t="s">
-        <v>235</v>
-      </c>
-      <c r="B71" s="6" t="s">
-        <v>314</v>
-      </c>
-      <c r="C71" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="D71" s="6"/>
-      <c r="E71" s="4" t="s">
-        <v>536</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
-        <v>81</v>
+        <v>235</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C72" s="6" t="s">
         <v>82</v>
       </c>
       <c r="D72" s="6"/>
       <c r="E72" s="4" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C73" s="6" t="s">
         <v>82</v>
       </c>
       <c r="D73" s="6"/>
       <c r="E73" s="4" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C74" s="6" t="s">
         <v>82</v>
       </c>
       <c r="D74" s="6"/>
       <c r="E74" s="4" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C75" s="6" t="s">
         <v>82</v>
       </c>
       <c r="D75" s="6"/>
       <c r="E75" s="4" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C76" s="6" t="s">
         <v>82</v>
       </c>
       <c r="D76" s="6"/>
       <c r="E76" s="4" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B77" s="6" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C77" s="6" t="s">
         <v>82</v>
       </c>
       <c r="D77" s="6"/>
       <c r="E77" s="4" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C78" s="6" t="s">
         <v>82</v>
       </c>
       <c r="D78" s="6"/>
       <c r="E78" s="4" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C79" s="6" t="s">
         <v>82</v>
       </c>
       <c r="D79" s="6"/>
       <c r="E79" s="4" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C80" s="6" t="s">
         <v>82</v>
       </c>
       <c r="D80" s="6"/>
       <c r="E80" s="4" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C81" s="6" t="s">
         <v>82</v>
       </c>
       <c r="D81" s="6"/>
       <c r="E81" s="4" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C82" s="6" t="s">
         <v>82</v>
       </c>
       <c r="D82" s="6"/>
       <c r="E82" s="4" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C83" s="6" t="s">
         <v>82</v>
       </c>
       <c r="D83" s="6"/>
       <c r="E83" s="4" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A84" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="B84" s="8" t="s">
-        <v>327</v>
+      <c r="A84" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B84" s="6" t="s">
+        <v>326</v>
       </c>
       <c r="C84" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="D84" s="8"/>
+      <c r="D84" s="6"/>
       <c r="E84" s="4" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A85" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B85" s="8" t="s">
+        <v>327</v>
+      </c>
+      <c r="C85" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D85" s="8"/>
+      <c r="E85" s="4" t="s">
         <v>549</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A85" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="B85" s="6" t="s">
-        <v>328</v>
-      </c>
-      <c r="C85" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="D85" s="6"/>
-      <c r="E85" s="4" t="s">
-        <v>550</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C86" s="6" t="s">
         <v>96</v>
       </c>
       <c r="D86" s="6"/>
       <c r="E86" s="4" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C87" s="6" t="s">
         <v>96</v>
       </c>
       <c r="D87" s="6"/>
       <c r="E87" s="4" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C88" s="6" t="s">
         <v>96</v>
       </c>
       <c r="D88" s="6"/>
       <c r="E88" s="4" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C89" s="6" t="s">
         <v>96</v>
       </c>
       <c r="D89" s="6"/>
       <c r="E89" s="4" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C90" s="6" t="s">
         <v>96</v>
       </c>
       <c r="D90" s="6"/>
       <c r="E90" s="4" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B91" s="6" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C91" s="6" t="s">
         <v>96</v>
       </c>
       <c r="D91" s="6"/>
       <c r="E91" s="4" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B92" s="6" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C92" s="6" t="s">
         <v>96</v>
       </c>
       <c r="D92" s="6"/>
       <c r="E92" s="4" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B93" s="6" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C93" s="6" t="s">
         <v>96</v>
       </c>
       <c r="D93" s="6"/>
       <c r="E93" s="4" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B94" s="6" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C94" s="6" t="s">
         <v>96</v>
       </c>
       <c r="D94" s="6"/>
       <c r="E94" s="4" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C95" s="6" t="s">
         <v>96</v>
       </c>
       <c r="D95" s="6"/>
       <c r="E95" s="4" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B96" s="6" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C96" s="6" t="s">
         <v>96</v>
       </c>
       <c r="D96" s="6"/>
       <c r="E96" s="4" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
-        <v>236</v>
+        <v>107</v>
       </c>
       <c r="B97" s="6" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C97" s="6" t="s">
         <v>96</v>
       </c>
       <c r="D97" s="6"/>
       <c r="E97" s="4" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A98" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="B98" s="8" t="s">
-        <v>341</v>
+      <c r="A98" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="B98" s="6" t="s">
+        <v>340</v>
       </c>
       <c r="C98" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="D98" s="8"/>
+      <c r="D98" s="6"/>
       <c r="E98" s="4" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A99" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="B99" s="8" t="s">
+        <v>341</v>
+      </c>
+      <c r="C99" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="D99" s="8"/>
+      <c r="E99" s="4" t="s">
         <v>563</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A99" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="B99" s="6" t="s">
-        <v>342</v>
-      </c>
-      <c r="C99" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D99" s="6"/>
-      <c r="E99" s="4" t="s">
-        <v>564</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
-        <v>237</v>
+        <v>109</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C100" s="6" t="s">
-        <v>68</v>
+        <v>110</v>
       </c>
       <c r="D100" s="6"/>
       <c r="E100" s="4" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="101" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
-        <v>111</v>
+        <v>237</v>
       </c>
       <c r="B101" s="6" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C101" s="6" t="s">
         <v>68</v>
       </c>
       <c r="D101" s="6"/>
       <c r="E101" s="4" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B102" s="6" t="s">
-        <v>242</v>
+        <v>344</v>
       </c>
       <c r="C102" s="6" t="s">
-        <v>113</v>
+        <v>68</v>
       </c>
       <c r="D102" s="6"/>
       <c r="E102" s="4" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="103" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B103" s="6" t="s">
-        <v>345</v>
+        <v>242</v>
       </c>
       <c r="C103" s="6" t="s">
         <v>113</v>
       </c>
       <c r="D103" s="6"/>
       <c r="E103" s="4" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="104" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B104" s="6" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C104" s="6" t="s">
-        <v>68</v>
+        <v>113</v>
       </c>
       <c r="D104" s="6"/>
       <c r="E104" s="4" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="105" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B105" s="6" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C105" s="6" t="s">
         <v>68</v>
       </c>
       <c r="D105" s="6"/>
       <c r="E105" s="4" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="106" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B106" s="6" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C106" s="6" t="s">
-        <v>113</v>
+        <v>68</v>
       </c>
       <c r="D106" s="6"/>
       <c r="E106" s="4" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="107" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B107" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C107" s="6" t="s">
         <v>113</v>
       </c>
       <c r="D107" s="6"/>
       <c r="E107" s="4" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="108" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B108" s="6" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C108" s="6" t="s">
-        <v>68</v>
+        <v>113</v>
       </c>
       <c r="D108" s="6"/>
       <c r="E108" s="4" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="109" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B109" s="6" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C109" s="6" t="s">
-        <v>110</v>
+        <v>68</v>
       </c>
       <c r="D109" s="6"/>
       <c r="E109" s="4" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="110" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B110" s="6" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C110" s="6" t="s">
         <v>110</v>
       </c>
       <c r="D110" s="6"/>
       <c r="E110" s="4" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="111" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B111" s="6" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C111" s="6" t="s">
         <v>110</v>
       </c>
       <c r="D111" s="6"/>
       <c r="E111" s="4" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="112" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B112" s="6" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C112" s="6" t="s">
-        <v>68</v>
+        <v>110</v>
       </c>
       <c r="D112" s="6"/>
       <c r="E112" s="4" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A113" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B113" s="6" t="s">
+        <v>354</v>
+      </c>
+      <c r="C113" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D113" s="6"/>
+      <c r="E113" s="4" t="s">
         <v>577</v>
       </c>
     </row>
-    <row r="113" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A113" s="7" t="s">
+    <row r="114" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A114" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="B113" s="8" t="s">
+      <c r="B114" s="8" t="s">
         <v>355</v>
       </c>
-      <c r="C113" s="8" t="s">
+      <c r="C114" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="D113" s="8"/>
-      <c r="E113" s="4" t="s">
+      <c r="D114" s="8"/>
+      <c r="E114" s="4" t="s">
         <v>578</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A114" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="B114" s="6" t="s">
-        <v>356</v>
-      </c>
-      <c r="C114" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="D114" s="6"/>
-      <c r="E114" s="4" t="s">
-        <v>579</v>
       </c>
     </row>
     <row r="115" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B115" s="6" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C115" s="6" t="s">
         <v>126</v>
       </c>
       <c r="D115" s="6"/>
       <c r="E115" s="4" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="116" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B116" s="6" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C116" s="6" t="s">
         <v>126</v>
       </c>
       <c r="D116" s="6"/>
       <c r="E116" s="4" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="117" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="s">
-        <v>238</v>
+        <v>128</v>
       </c>
       <c r="B117" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C117" s="6" t="s">
         <v>126</v>
       </c>
       <c r="D117" s="6"/>
       <c r="E117" s="4" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="118" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
-        <v>129</v>
+        <v>238</v>
       </c>
       <c r="B118" s="6" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C118" s="6" t="s">
         <v>126</v>
       </c>
       <c r="D118" s="6"/>
       <c r="E118" s="4" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="119" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A119" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B119" s="6" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C119" s="6" t="s">
         <v>126</v>
       </c>
       <c r="D119" s="6"/>
       <c r="E119" s="4" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="120" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A120" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B120" s="6" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C120" s="6" t="s">
         <v>126</v>
       </c>
       <c r="D120" s="6"/>
       <c r="E120" s="4" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="121" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B121" s="6" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C121" s="6" t="s">
         <v>126</v>
       </c>
       <c r="D121" s="6"/>
       <c r="E121" s="4" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="122" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A122" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B122" s="6" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C122" s="6" t="s">
         <v>126</v>
       </c>
       <c r="D122" s="6"/>
       <c r="E122" s="4" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="123" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B123" s="6" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C123" s="6" t="s">
         <v>126</v>
       </c>
       <c r="D123" s="6"/>
       <c r="E123" s="4" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="124" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B124" s="6" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C124" s="6" t="s">
         <v>126</v>
       </c>
       <c r="D124" s="6"/>
       <c r="E124" s="4" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="125" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B125" s="6" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C125" s="6" t="s">
         <v>126</v>
       </c>
       <c r="D125" s="6"/>
       <c r="E125" s="4" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="126" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B126" s="6" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C126" s="6" t="s">
         <v>126</v>
       </c>
       <c r="D126" s="6"/>
       <c r="E126" s="4" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="127" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A127" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="B127" s="8" t="s">
-        <v>369</v>
+      <c r="A127" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="B127" s="6" t="s">
+        <v>368</v>
       </c>
       <c r="C127" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="D127" s="8"/>
+      <c r="D127" s="6"/>
       <c r="E127" s="4" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="128" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A128" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="B128" s="6" t="s">
-        <v>370</v>
+      <c r="A128" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="B128" s="8" t="s">
+        <v>369</v>
       </c>
       <c r="C128" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="D128" s="6"/>
+      <c r="D128" s="8"/>
       <c r="E128" s="4" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="129" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A129" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B129" s="6" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C129" s="6" t="s">
         <v>126</v>
       </c>
       <c r="D129" s="6"/>
       <c r="E129" s="4" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="130" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B130" s="6" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C130" s="6" t="s">
         <v>126</v>
       </c>
       <c r="D130" s="6"/>
       <c r="E130" s="4" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="131" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A131" s="5" t="s">
-        <v>240</v>
+        <v>141</v>
       </c>
       <c r="B131" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C131" s="6" t="s">
         <v>126</v>
       </c>
       <c r="D131" s="6"/>
       <c r="E131" s="4" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="132" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A132" s="5" t="s">
-        <v>142</v>
+        <v>240</v>
       </c>
       <c r="B132" s="6" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C132" s="6" t="s">
         <v>126</v>
       </c>
       <c r="D132" s="6"/>
       <c r="E132" s="4" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="133" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A133" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B133" s="6" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C133" s="6" t="s">
         <v>126</v>
       </c>
       <c r="D133" s="6"/>
       <c r="E133" s="4" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="134" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A134" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B134" s="6" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C134" s="6" t="s">
         <v>126</v>
       </c>
       <c r="D134" s="6"/>
       <c r="E134" s="4" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="135" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A135" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B135" s="6" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C135" s="6" t="s">
         <v>126</v>
       </c>
       <c r="D135" s="6"/>
       <c r="E135" s="4" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="136" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A136" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B136" s="6" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C136" s="6" t="s">
         <v>126</v>
       </c>
       <c r="D136" s="6"/>
       <c r="E136" s="4" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="137" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A137" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B137" s="6" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C137" s="6" t="s">
         <v>126</v>
       </c>
       <c r="D137" s="6"/>
       <c r="E137" s="4" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="138" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A138" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B138" s="6" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C138" s="6" t="s">
         <v>126</v>
       </c>
       <c r="D138" s="6"/>
       <c r="E138" s="4" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="139" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A139" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B139" s="6" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C139" s="6" t="s">
         <v>126</v>
       </c>
       <c r="D139" s="6"/>
       <c r="E139" s="4" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="140" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A140" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B140" s="6" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C140" s="6" t="s">
         <v>126</v>
       </c>
       <c r="D140" s="6"/>
       <c r="E140" s="4" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="141" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A141" s="5" t="s">
-        <v>239</v>
+        <v>150</v>
       </c>
       <c r="B141" s="6" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C141" s="6" t="s">
         <v>126</v>
       </c>
       <c r="D141" s="6"/>
       <c r="E141" s="4" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="142" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A142" s="5" t="s">
-        <v>151</v>
+        <v>239</v>
       </c>
       <c r="B142" s="6" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C142" s="6" t="s">
-        <v>82</v>
+        <v>126</v>
       </c>
       <c r="D142" s="6"/>
       <c r="E142" s="4" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="143" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A143" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B143" s="6" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C143" s="6" t="s">
         <v>82</v>
       </c>
       <c r="D143" s="6"/>
       <c r="E143" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="144" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A144" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B144" s="6" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C144" s="6" t="s">
         <v>82</v>
       </c>
       <c r="D144" s="6"/>
       <c r="E144" s="4" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="145" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A145" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B145" s="6" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C145" s="6" t="s">
         <v>82</v>
       </c>
       <c r="D145" s="6"/>
       <c r="E145" s="4" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="146" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A146" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B146" s="6" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C146" s="6" t="s">
         <v>82</v>
       </c>
       <c r="D146" s="6"/>
       <c r="E146" s="4" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="147" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A147" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B147" s="6" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C147" s="6" t="s">
         <v>82</v>
       </c>
       <c r="D147" s="6"/>
       <c r="E147" s="4" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="148" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A148" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B148" s="6" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C148" s="6" t="s">
         <v>82</v>
       </c>
       <c r="D148" s="6"/>
       <c r="E148" s="4" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="149" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A149" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B149" s="6" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C149" s="6" t="s">
         <v>82</v>
       </c>
       <c r="D149" s="6"/>
       <c r="E149" s="4" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="150" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A150" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B150" s="6" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C150" s="6" t="s">
         <v>82</v>
       </c>
       <c r="D150" s="6"/>
       <c r="E150" s="4" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="151" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A151" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B151" s="6" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C151" s="6" t="s">
         <v>82</v>
       </c>
       <c r="D151" s="6"/>
       <c r="E151" s="4" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="152" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A152" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B152" s="6" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C152" s="6" t="s">
         <v>82</v>
       </c>
       <c r="D152" s="6"/>
       <c r="E152" s="4" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="153" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A153" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B153" s="6" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C153" s="6" t="s">
         <v>82</v>
       </c>
       <c r="D153" s="6"/>
       <c r="E153" s="4" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="154" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A154" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B154" s="6" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C154" s="6" t="s">
         <v>82</v>
       </c>
       <c r="D154" s="6"/>
       <c r="E154" s="4" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="155" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A155" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="B155" s="8" t="s">
-        <v>397</v>
+      <c r="A155" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="B155" s="6" t="s">
+        <v>396</v>
       </c>
       <c r="C155" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="D155" s="8"/>
+      <c r="D155" s="6"/>
       <c r="E155" s="4" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A156" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="B156" s="8" t="s">
+        <v>397</v>
+      </c>
+      <c r="C156" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D156" s="8"/>
+      <c r="E156" s="4" t="s">
         <v>620</v>
-      </c>
-    </row>
-    <row r="156" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A156" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="B156" s="6" t="s">
-        <v>398</v>
-      </c>
-      <c r="C156" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D156" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E156" s="4" t="s">
-        <v>621</v>
       </c>
     </row>
     <row r="157" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A157" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B157" s="6" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C157" s="6" t="s">
         <v>67</v>
       </c>
       <c r="D157" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E157" s="4" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="158" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A158" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B158" s="6" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C158" s="6" t="s">
         <v>67</v>
       </c>
       <c r="D158" s="6" t="s">
-        <v>68</v>
+        <v>23</v>
       </c>
       <c r="E158" s="4" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="159" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A159" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B159" s="6" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C159" s="6" t="s">
         <v>67</v>
       </c>
       <c r="D159" s="6" t="s">
-        <v>21</v>
+        <v>68</v>
       </c>
       <c r="E159" s="4" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="160" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A160" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B160" s="6" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C160" s="6" t="s">
         <v>67</v>
       </c>
       <c r="D160" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E160" s="4" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="161" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A161" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B161" s="6" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C161" s="6" t="s">
         <v>67</v>
       </c>
       <c r="D161" s="6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E161" s="4" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="162" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A162" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B162" s="6" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C162" s="6" t="s">
         <v>67</v>
       </c>
       <c r="D162" s="6" t="s">
-        <v>68</v>
+        <v>21</v>
       </c>
       <c r="E162" s="4" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="163" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A163" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B163" s="6" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C163" s="6" t="s">
         <v>67</v>
       </c>
       <c r="D163" s="6" t="s">
-        <v>23</v>
+        <v>68</v>
       </c>
       <c r="E163" s="4" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="164" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A164" s="5" t="s">
-        <v>241</v>
+        <v>172</v>
       </c>
       <c r="B164" s="6" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C164" s="6" t="s">
         <v>67</v>
@@ -5137,15 +5126,15 @@
         <v>23</v>
       </c>
       <c r="E164" s="4" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="165" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A165" s="5" t="s">
-        <v>173</v>
+        <v>241</v>
       </c>
       <c r="B165" s="6" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C165" s="6" t="s">
         <v>67</v>
@@ -5154,548 +5143,548 @@
         <v>23</v>
       </c>
       <c r="E165" s="4" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="166" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A166" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B166" s="6" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C166" s="6" t="s">
         <v>67</v>
       </c>
       <c r="D166" s="6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E166" s="4" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="167" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A167" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B167" s="6" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C167" s="6" t="s">
         <v>67</v>
       </c>
       <c r="D167" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E167" s="4" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="168" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A168" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B168" s="6" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C168" s="6" t="s">
         <v>67</v>
       </c>
       <c r="D168" s="6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E168" s="4" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="169" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A169" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="B169" s="8" t="s">
-        <v>411</v>
+      <c r="A169" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="B169" s="6" t="s">
+        <v>410</v>
       </c>
       <c r="C169" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="D169" s="8" t="s">
+      <c r="D169" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E169" s="4" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A170" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="B170" s="8" t="s">
+        <v>411</v>
+      </c>
+      <c r="C170" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D170" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="E169" s="4" t="s">
+      <c r="E170" s="4" t="s">
         <v>634</v>
-      </c>
-    </row>
-    <row r="170" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A170" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="B170" s="6" t="s">
-        <v>412</v>
-      </c>
-      <c r="C170" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D170" s="1"/>
-      <c r="E170" s="4" t="s">
-        <v>635</v>
       </c>
     </row>
     <row r="171" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A171" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B171" s="6" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C171" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D171" s="1"/>
       <c r="E171" s="4" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="172" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A172" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B172" s="6" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C172" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D172" s="1"/>
       <c r="E172" s="4" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="173" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A173" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B173" s="6" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C173" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D173" s="1"/>
       <c r="E173" s="4" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="174" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A174" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B174" s="6" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C174" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D174" s="1"/>
       <c r="E174" s="4" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="175" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A175" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B175" s="6" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C175" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D175" s="1"/>
       <c r="E175" s="4" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="176" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A176" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B176" s="6" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C176" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D176" s="1"/>
       <c r="E176" s="4" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="177" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A177" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B177" s="6" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C177" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D177" s="1"/>
       <c r="E177" s="4" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="178" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A178" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B178" s="6" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C178" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D178" s="1"/>
       <c r="E178" s="4" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="179" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A179" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B179" s="6" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C179" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D179" s="1"/>
       <c r="E179" s="4" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="180" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A180" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B180" s="6" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C180" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D180" s="1"/>
       <c r="E180" s="4" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="181" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A181" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B181" s="6" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C181" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D181" s="1"/>
       <c r="E181" s="4" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="182" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A182" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B182" s="6" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C182" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D182" s="1"/>
       <c r="E182" s="4" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="183" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A183" s="7" t="s">
-        <v>191</v>
-      </c>
-      <c r="B183" s="8" t="s">
-        <v>425</v>
-      </c>
-      <c r="C183" s="8" t="s">
+      <c r="A183" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="B183" s="6" t="s">
+        <v>424</v>
+      </c>
+      <c r="C183" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D183" s="1"/>
       <c r="E183" s="4" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A184" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="B184" s="8" t="s">
+        <v>425</v>
+      </c>
+      <c r="C184" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D184" s="1"/>
+      <c r="E184" s="4" t="s">
         <v>648</v>
-      </c>
-    </row>
-    <row r="184" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A184" s="5" t="s">
-        <v>192</v>
-      </c>
-      <c r="B184" s="6" t="s">
-        <v>426</v>
-      </c>
-      <c r="C184" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D184" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E184" s="4" t="s">
-        <v>649</v>
       </c>
     </row>
     <row r="185" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A185" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B185" s="6" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C185" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D185" s="6" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="E185" s="4" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="186" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A186" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B186" s="6" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C186" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D186" s="6" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="E186" s="4" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="187" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A187" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B187" s="6" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C187" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D187" s="6" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="E187" s="4" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="188" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A188" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B188" s="6" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C188" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D188" s="6" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="E188" s="4" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="189" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A189" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B189" s="6" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C189" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D189" s="6" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="E189" s="4" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="190" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A190" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B190" s="6" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C190" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D190" s="6" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="E190" s="4" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="191" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A191" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B191" s="6" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C191" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D191" s="6" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="E191" s="4" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="192" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A192" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B192" s="6" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C192" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D192" s="6" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="E192" s="4" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="193" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A193" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B193" s="6" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C193" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D193" s="6" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="E193" s="4" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="194" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A194" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B194" s="6" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C194" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D194" s="6" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="E194" s="4" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="195" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A195" s="5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B195" s="6" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C195" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D195" s="6" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="E195" s="4" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="196" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A196" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="B196" s="6" t="s">
+        <v>437</v>
+      </c>
+      <c r="C196" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D196" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E196" s="4" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A197" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="B196" s="6" t="s">
+      <c r="B197" s="6" t="s">
         <v>438</v>
       </c>
-      <c r="C196" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D196" s="6" t="s">
+      <c r="C197" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D197" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E196" s="4" t="s">
+      <c r="E197" s="4" t="s">
         <v>661</v>
       </c>
     </row>
-    <row r="197" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A197" s="7" t="s">
+    <row r="198" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A198" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="B197" s="8" t="s">
+      <c r="B198" s="8" t="s">
         <v>439</v>
       </c>
-      <c r="C197" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D197" s="8" t="s">
+      <c r="C198" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D198" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E197" s="4" t="s">
+      <c r="E198" s="4" t="s">
         <v>662</v>
-      </c>
-    </row>
-    <row r="198" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A198" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="B198" s="6" t="s">
-        <v>440</v>
-      </c>
-      <c r="C198" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D198" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E198" s="4" t="s">
-        <v>663</v>
       </c>
     </row>
     <row r="199" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A199" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B199" s="6" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C199" s="6" t="s">
         <v>5</v>
@@ -5704,32 +5693,32 @@
         <v>21</v>
       </c>
       <c r="E199" s="4" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="200" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A200" s="5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B200" s="6" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C200" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D200" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E200" s="4" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="201" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A201" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B201" s="6" t="s">
-        <v>243</v>
+        <v>442</v>
       </c>
       <c r="C201" s="6" t="s">
         <v>5</v>
@@ -5738,49 +5727,49 @@
         <v>23</v>
       </c>
       <c r="E201" s="4" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="202" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A202" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B202" s="6" t="s">
-        <v>443</v>
+        <v>243</v>
       </c>
       <c r="C202" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D202" s="6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E202" s="4" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="203" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A203" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B203" s="6" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C203" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D203" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E203" s="4" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="204" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A204" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B204" s="6" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C204" s="6" t="s">
         <v>5</v>
@@ -5789,32 +5778,32 @@
         <v>23</v>
       </c>
       <c r="E204" s="4" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="205" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A205" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B205" s="6" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C205" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D205" s="6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E205" s="4" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="206" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A206" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B206" s="6" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C206" s="6" t="s">
         <v>5</v>
@@ -5823,151 +5812,151 @@
         <v>21</v>
       </c>
       <c r="E206" s="4" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="207" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A207" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B207" s="6" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C207" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D207" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E207" s="4" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="208" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A208" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B208" s="6" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C208" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D208" s="6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E208" s="4" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="209" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A209" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B209" s="6" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C209" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D209" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E209" s="4" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="210" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A210" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="B210" s="6" t="s">
+        <v>450</v>
+      </c>
+      <c r="C210" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D210" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E210" s="4" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A211" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="B210" s="6" t="s">
+      <c r="B211" s="6" t="s">
         <v>451</v>
       </c>
-      <c r="C210" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D210" s="6" t="s">
+      <c r="C211" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D211" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E210" s="4" t="s">
+      <c r="E211" s="4" t="s">
         <v>675</v>
       </c>
     </row>
-    <row r="211" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A211" s="7" t="s">
+    <row r="212" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A212" s="7" t="s">
         <v>219</v>
       </c>
-      <c r="B211" s="8" t="s">
+      <c r="B212" s="8" t="s">
         <v>452</v>
       </c>
-      <c r="C211" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D211" s="8" t="s">
+      <c r="C212" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D212" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E211" s="4" t="s">
+      <c r="E212" s="4" t="s">
         <v>676</v>
-      </c>
-    </row>
-    <row r="212" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A212" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="B212" s="6" t="s">
-        <v>453</v>
-      </c>
-      <c r="C212" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D212" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E212" s="4" t="s">
-        <v>677</v>
       </c>
     </row>
     <row r="213" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A213" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B213" s="6" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C213" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D213" s="6" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E213" s="4" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="214" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A214" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B214" s="6" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C214" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D214" s="6" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E214" s="4" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="215" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A215" s="5" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B215" s="6" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C215" s="6" t="s">
         <v>5</v>
@@ -5976,32 +5965,32 @@
         <v>10</v>
       </c>
       <c r="E215" s="4" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="216" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A216" s="5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B216" s="6" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C216" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D216" s="6" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E216" s="4" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="217" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A217" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B217" s="6" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C217" s="6" t="s">
         <v>5</v>
@@ -6010,49 +5999,49 @@
         <v>6</v>
       </c>
       <c r="E217" s="4" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="218" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A218" s="5" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B218" s="6" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C218" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D218" s="6" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E218" s="4" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="219" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A219" s="5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B219" s="6" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C219" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D219" s="6" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E219" s="4" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="220" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A220" s="5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B220" s="6" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C220" s="6" t="s">
         <v>5</v>
@@ -6060,16 +6049,16 @@
       <c r="D220" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E220" s="11" t="s">
-        <v>685</v>
+      <c r="E220" s="4" t="s">
+        <v>684</v>
       </c>
     </row>
     <row r="221" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A221" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B221" s="6" t="s">
-        <v>244</v>
+        <v>461</v>
       </c>
       <c r="C221" s="6" t="s">
         <v>5</v>
@@ -6077,50 +6066,50 @@
       <c r="D221" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E221" s="4" t="s">
-        <v>686</v>
+      <c r="E221" s="11" t="s">
+        <v>685</v>
       </c>
     </row>
     <row r="222" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A222" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B222" s="6" t="s">
-        <v>462</v>
+        <v>244</v>
       </c>
       <c r="C222" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D222" s="6" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E222" s="4" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="223" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A223" s="5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B223" s="6" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C223" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D223" s="6" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E223" s="4" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="224" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A224" s="5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B224" s="6" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C224" s="6" t="s">
         <v>5</v>
@@ -6129,29 +6118,46 @@
         <v>6</v>
       </c>
       <c r="E224" s="4" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A225" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="B225" s="6" t="s">
+        <v>464</v>
+      </c>
+      <c r="C225" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D225" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E225" s="4" t="s">
         <v>689</v>
       </c>
     </row>
-    <row r="225" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A225" s="7" t="s">
+    <row r="226" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A226" s="7" t="s">
         <v>233</v>
       </c>
-      <c r="B225" s="8" t="s">
+      <c r="B226" s="8" t="s">
         <v>465</v>
       </c>
-      <c r="C225" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D225" s="8" t="s">
+      <c r="C226" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D226" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E225" s="4" t="s">
+      <c r="E226" s="4" t="s">
         <v>690</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Mirror old PR for User testing to keep some good stuff
</commit_message>
<xml_diff>
--- a/models/mock-data/FakeUsers.xlsx
+++ b/models/mock-data/FakeUsers.xlsx
@@ -1430,675 +1430,21 @@
     <t>Koop.960</t>
   </si>
   <si>
-    <t xml:space="preserve"> Mcbain.358</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Huot.633</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Bezanson.660</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Cavalieri.839</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Bass.111</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Isaacs.442</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Wolanski.136</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Clendening.100</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Ashbaugh.213</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Pinder.964</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Depalma.763</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Imel.715</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Shambaugh.40</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Albritton.668</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Slocum.139</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Maysonet.58</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Maag.400</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Laguardia.605</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Rosso.903</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Jeanbaptiste.831</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Siegrist.361</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Balas.71</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Costello.760</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Poulter.816</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Whitmire.337</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Politte.833</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Hartshorn.948</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Iser.962</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Tinajero.70</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Caplan.540</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Seppala.173</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Statler.8</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Dartez.850</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Backman.359</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Norgard.983</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Ingwersen.694</t>
-  </si>
-  <si>
     <t>Torgersen.942</t>
   </si>
   <si>
-    <t xml:space="preserve"> Landey.624</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Herbst.123</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Mings.349</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Gandara.979</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Caffrey.986</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Branning.888</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Beland.117</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Mariscal.729</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Medel.318</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Normandin.386</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Breuer.491</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Liberto.857</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Godfrey.949</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Mikkelson.973</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Fleagle.381</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Darlington.481</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Hosein.882</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Juarbe.11</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Deslauriers.767</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Horney.105</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Nivens.576</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Enfinger.107</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Mccraw.316</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Eggleton.598</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Wymore.153</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Dayton.843</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Petti.427</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Guercio.396</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Vasconcellos.50</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Heal.856</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Hornick.940</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Franson.807</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Mahar.143</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Denney.753</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Saffell.584</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Maze.620</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Pawlowicz.398</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Lahr.942</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Lerman.315</t>
-  </si>
-  <si>
     <t>Provencal.801</t>
   </si>
   <si>
-    <t xml:space="preserve"> Delagarza.200</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Thompkins.432</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Mccroskey.8</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Wynter.419</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Cliff.333</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Storck.591</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Meikle.556</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Lightfoot.559</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Ester.921</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Mungo.80</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Michalski.556</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Lunceford.641</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Siebert.643</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Call.939</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Robin.11</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Roddy.883</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Pangle.362</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Hastings.286</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Seller.821</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Mumaw.240</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Popham.241</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Grieve.693</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Camacho.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Ehrenberg.441</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Champine.202</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Wells.55</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Spicer.41</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Shirley.671</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Eddington.306</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Morrisette.605</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Whiting.851</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Nordahl.9</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Mullet.321</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Rand.840</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Mathisen.218</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Garten.560</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Tyree.611</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Peppler.143</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Paulson.371</t>
-  </si>
-  <si>
     <t>Mercer.633</t>
   </si>
   <si>
-    <t xml:space="preserve"> Lickteig.332</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Haddon.17</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Mauger.736</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Berge.171</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Willcutt.973</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Gaver.489</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Ruyle.883</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Heeter.44</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Fitzwater.145</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Aquilino.382</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Palomino.241</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Dunson.706</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Hager.952</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Bussell.732</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Reese.274</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Borjas.930</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Cady.595</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Okada.299</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Debow.528</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Calderone.593</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Berrier.471</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Parry.560</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Tignor.161</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Cutsforth.174</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Cripe.236</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Belmont.982</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Girard.502</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Vining.935</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Clever.468</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Dias.832</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Drake.377</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Lane.218</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Gerry.184</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Younts.552</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Mcmurtrie.820</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Dowless.286</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Scheffer.323</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Rempel.454</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Lis.287</t>
-  </si>
-  <si>
     <t>Marsch.502</t>
   </si>
   <si>
-    <t xml:space="preserve"> Lesperance.914</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Gunning.855</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Cripps.973</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Younkin.677</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Braz.539</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Zielinski.230</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Junior.195</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Veneziano.661</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Down.797</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Ogle.891</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Resnick.437</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Tindell.641</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Woltz.563</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Borjas.78</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Esquer.919</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Zdenek.728</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Astorga.32</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Dollins.210</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Standifer.77</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Stoke.982</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Grief.860</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Denis.806</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Gamblin.788</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Faddis.634</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Binns.159</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Hepfer.154</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Slade.484</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Papp.563</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Encinas.262</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Mcdonald.342</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Benigno.116</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Brinkley.866</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Certain.335</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Cypher.353</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Lautenschlage.917</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Rushford.890</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Delossantos.38</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Slee.951</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Moretti.365</t>
-  </si>
-  <si>
     <t>Alphin.603</t>
   </si>
   <si>
-    <t xml:space="preserve"> Rainer.108</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Breitenstein.677</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Coletta.344</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Hieber.798</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Closson.956</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Tully.114</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Caywood.170</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Silsby.242</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Tait.159</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Aleman.73</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Brindley.439</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Dicarlo.674</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Florez.613</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Sawyers.890</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Byrne.461</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Hagar.119</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Goldie.250</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Monfort.301</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Toll.679</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Gammage.15</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Darnell.242</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Paro.334</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Barwick.128</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Dugger.786</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Leibowitz.835</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Krebsbach.938</t>
-  </si>
-  <si>
     <t>A5</t>
   </si>
   <si>
@@ -2106,6 +1452,660 @@
   </si>
   <si>
     <t>Thompson.1234</t>
+  </si>
+  <si>
+    <t>Mcbain.358</t>
+  </si>
+  <si>
+    <t>Huot.633</t>
+  </si>
+  <si>
+    <t>Bezanson.660</t>
+  </si>
+  <si>
+    <t>Cavalieri.839</t>
+  </si>
+  <si>
+    <t>Bass.111</t>
+  </si>
+  <si>
+    <t>Isaacs.442</t>
+  </si>
+  <si>
+    <t>Wolanski.136</t>
+  </si>
+  <si>
+    <t>Clendening.100</t>
+  </si>
+  <si>
+    <t>Ashbaugh.213</t>
+  </si>
+  <si>
+    <t>Pinder.964</t>
+  </si>
+  <si>
+    <t>Depalma.763</t>
+  </si>
+  <si>
+    <t>Imel.715</t>
+  </si>
+  <si>
+    <t>Shambaugh.40</t>
+  </si>
+  <si>
+    <t>Albritton.668</t>
+  </si>
+  <si>
+    <t>Slocum.139</t>
+  </si>
+  <si>
+    <t>Maysonet.58</t>
+  </si>
+  <si>
+    <t>Maag.400</t>
+  </si>
+  <si>
+    <t>Laguardia.605</t>
+  </si>
+  <si>
+    <t>Rosso.903</t>
+  </si>
+  <si>
+    <t>Jeanbaptiste.831</t>
+  </si>
+  <si>
+    <t>Siegrist.361</t>
+  </si>
+  <si>
+    <t>Balas.71</t>
+  </si>
+  <si>
+    <t>Costello.760</t>
+  </si>
+  <si>
+    <t>Poulter.816</t>
+  </si>
+  <si>
+    <t>Whitmire.337</t>
+  </si>
+  <si>
+    <t>Politte.833</t>
+  </si>
+  <si>
+    <t>Hartshorn.948</t>
+  </si>
+  <si>
+    <t>Iser.962</t>
+  </si>
+  <si>
+    <t>Tinajero.70</t>
+  </si>
+  <si>
+    <t>Caplan.540</t>
+  </si>
+  <si>
+    <t>Seppala.173</t>
+  </si>
+  <si>
+    <t>Statler.8</t>
+  </si>
+  <si>
+    <t>Dartez.850</t>
+  </si>
+  <si>
+    <t>Backman.359</t>
+  </si>
+  <si>
+    <t>Norgard.983</t>
+  </si>
+  <si>
+    <t>Ingwersen.694</t>
+  </si>
+  <si>
+    <t>Landey.624</t>
+  </si>
+  <si>
+    <t>Herbst.123</t>
+  </si>
+  <si>
+    <t>Mings.349</t>
+  </si>
+  <si>
+    <t>Gandara.979</t>
+  </si>
+  <si>
+    <t>Caffrey.986</t>
+  </si>
+  <si>
+    <t>Branning.888</t>
+  </si>
+  <si>
+    <t>Beland.117</t>
+  </si>
+  <si>
+    <t>Mariscal.729</t>
+  </si>
+  <si>
+    <t>Medel.318</t>
+  </si>
+  <si>
+    <t>Normandin.386</t>
+  </si>
+  <si>
+    <t>Breuer.491</t>
+  </si>
+  <si>
+    <t>Liberto.857</t>
+  </si>
+  <si>
+    <t>Godfrey.949</t>
+  </si>
+  <si>
+    <t>Mikkelson.973</t>
+  </si>
+  <si>
+    <t>Fleagle.381</t>
+  </si>
+  <si>
+    <t>Darlington.481</t>
+  </si>
+  <si>
+    <t>Hosein.882</t>
+  </si>
+  <si>
+    <t>Juarbe.11</t>
+  </si>
+  <si>
+    <t>Deslauriers.767</t>
+  </si>
+  <si>
+    <t>Horney.105</t>
+  </si>
+  <si>
+    <t>Nivens.576</t>
+  </si>
+  <si>
+    <t>Enfinger.107</t>
+  </si>
+  <si>
+    <t>Mccraw.316</t>
+  </si>
+  <si>
+    <t>Eggleton.598</t>
+  </si>
+  <si>
+    <t>Wymore.153</t>
+  </si>
+  <si>
+    <t>Dayton.843</t>
+  </si>
+  <si>
+    <t>Petti.427</t>
+  </si>
+  <si>
+    <t>Guercio.396</t>
+  </si>
+  <si>
+    <t>Vasconcellos.50</t>
+  </si>
+  <si>
+    <t>Heal.856</t>
+  </si>
+  <si>
+    <t>Hornick.940</t>
+  </si>
+  <si>
+    <t>Franson.807</t>
+  </si>
+  <si>
+    <t>Mahar.143</t>
+  </si>
+  <si>
+    <t>Denney.753</t>
+  </si>
+  <si>
+    <t>Saffell.584</t>
+  </si>
+  <si>
+    <t>Maze.620</t>
+  </si>
+  <si>
+    <t>Pawlowicz.398</t>
+  </si>
+  <si>
+    <t>Lahr.942</t>
+  </si>
+  <si>
+    <t>Lerman.315</t>
+  </si>
+  <si>
+    <t>Delagarza.200</t>
+  </si>
+  <si>
+    <t>Thompkins.432</t>
+  </si>
+  <si>
+    <t>Mccroskey.8</t>
+  </si>
+  <si>
+    <t>Wynter.419</t>
+  </si>
+  <si>
+    <t>Cliff.333</t>
+  </si>
+  <si>
+    <t>Storck.591</t>
+  </si>
+  <si>
+    <t>Meikle.556</t>
+  </si>
+  <si>
+    <t>Lightfoot.559</t>
+  </si>
+  <si>
+    <t>Ester.921</t>
+  </si>
+  <si>
+    <t>Mungo.80</t>
+  </si>
+  <si>
+    <t>Michalski.556</t>
+  </si>
+  <si>
+    <t>Lunceford.641</t>
+  </si>
+  <si>
+    <t>Siebert.643</t>
+  </si>
+  <si>
+    <t>Call.939</t>
+  </si>
+  <si>
+    <t>Robin.11</t>
+  </si>
+  <si>
+    <t>Roddy.883</t>
+  </si>
+  <si>
+    <t>Pangle.362</t>
+  </si>
+  <si>
+    <t>Hastings.286</t>
+  </si>
+  <si>
+    <t>Seller.821</t>
+  </si>
+  <si>
+    <t>Mumaw.240</t>
+  </si>
+  <si>
+    <t>Popham.241</t>
+  </si>
+  <si>
+    <t>Grieve.693</t>
+  </si>
+  <si>
+    <t>Camacho.4</t>
+  </si>
+  <si>
+    <t>Ehrenberg.441</t>
+  </si>
+  <si>
+    <t>Champine.202</t>
+  </si>
+  <si>
+    <t>Wells.55</t>
+  </si>
+  <si>
+    <t>Spicer.41</t>
+  </si>
+  <si>
+    <t>Shirley.671</t>
+  </si>
+  <si>
+    <t>Eddington.306</t>
+  </si>
+  <si>
+    <t>Morrisette.605</t>
+  </si>
+  <si>
+    <t>Whiting.851</t>
+  </si>
+  <si>
+    <t>Nordahl.9</t>
+  </si>
+  <si>
+    <t>Mullet.321</t>
+  </si>
+  <si>
+    <t>Rand.840</t>
+  </si>
+  <si>
+    <t>Mathisen.218</t>
+  </si>
+  <si>
+    <t>Garten.560</t>
+  </si>
+  <si>
+    <t>Tyree.611</t>
+  </si>
+  <si>
+    <t>Peppler.143</t>
+  </si>
+  <si>
+    <t>Paulson.371</t>
+  </si>
+  <si>
+    <t>Lickteig.332</t>
+  </si>
+  <si>
+    <t>Haddon.17</t>
+  </si>
+  <si>
+    <t>Mauger.736</t>
+  </si>
+  <si>
+    <t>Berge.171</t>
+  </si>
+  <si>
+    <t>Willcutt.973</t>
+  </si>
+  <si>
+    <t>Gaver.489</t>
+  </si>
+  <si>
+    <t>Ruyle.883</t>
+  </si>
+  <si>
+    <t>Heeter.44</t>
+  </si>
+  <si>
+    <t>Fitzwater.145</t>
+  </si>
+  <si>
+    <t>Aquilino.382</t>
+  </si>
+  <si>
+    <t>Palomino.241</t>
+  </si>
+  <si>
+    <t>Dunson.706</t>
+  </si>
+  <si>
+    <t>Hager.952</t>
+  </si>
+  <si>
+    <t>Bussell.732</t>
+  </si>
+  <si>
+    <t>Reese.274</t>
+  </si>
+  <si>
+    <t>Borjas.930</t>
+  </si>
+  <si>
+    <t>Cady.595</t>
+  </si>
+  <si>
+    <t>Okada.299</t>
+  </si>
+  <si>
+    <t>Debow.528</t>
+  </si>
+  <si>
+    <t>Calderone.593</t>
+  </si>
+  <si>
+    <t>Berrier.471</t>
+  </si>
+  <si>
+    <t>Parry.560</t>
+  </si>
+  <si>
+    <t>Tignor.161</t>
+  </si>
+  <si>
+    <t>Cutsforth.174</t>
+  </si>
+  <si>
+    <t>Cripe.236</t>
+  </si>
+  <si>
+    <t>Belmont.982</t>
+  </si>
+  <si>
+    <t>Girard.502</t>
+  </si>
+  <si>
+    <t>Vining.935</t>
+  </si>
+  <si>
+    <t>Clever.468</t>
+  </si>
+  <si>
+    <t>Dias.832</t>
+  </si>
+  <si>
+    <t>Drake.377</t>
+  </si>
+  <si>
+    <t>Lane.218</t>
+  </si>
+  <si>
+    <t>Gerry.184</t>
+  </si>
+  <si>
+    <t>Younts.552</t>
+  </si>
+  <si>
+    <t>Mcmurtrie.820</t>
+  </si>
+  <si>
+    <t>Dowless.286</t>
+  </si>
+  <si>
+    <t>Scheffer.323</t>
+  </si>
+  <si>
+    <t>Rempel.454</t>
+  </si>
+  <si>
+    <t>Lis.287</t>
+  </si>
+  <si>
+    <t>Lesperance.914</t>
+  </si>
+  <si>
+    <t>Gunning.855</t>
+  </si>
+  <si>
+    <t>Cripps.973</t>
+  </si>
+  <si>
+    <t>Younkin.677</t>
+  </si>
+  <si>
+    <t>Braz.539</t>
+  </si>
+  <si>
+    <t>Zielinski.230</t>
+  </si>
+  <si>
+    <t>Junior.195</t>
+  </si>
+  <si>
+    <t>Veneziano.661</t>
+  </si>
+  <si>
+    <t>Down.797</t>
+  </si>
+  <si>
+    <t>Ogle.891</t>
+  </si>
+  <si>
+    <t>Resnick.437</t>
+  </si>
+  <si>
+    <t>Tindell.641</t>
+  </si>
+  <si>
+    <t>Woltz.563</t>
+  </si>
+  <si>
+    <t>Borjas.78</t>
+  </si>
+  <si>
+    <t>Esquer.919</t>
+  </si>
+  <si>
+    <t>Zdenek.728</t>
+  </si>
+  <si>
+    <t>Astorga.32</t>
+  </si>
+  <si>
+    <t>Dollins.210</t>
+  </si>
+  <si>
+    <t>Standifer.77</t>
+  </si>
+  <si>
+    <t>Stoke.982</t>
+  </si>
+  <si>
+    <t>Grief.860</t>
+  </si>
+  <si>
+    <t>Denis.806</t>
+  </si>
+  <si>
+    <t>Gamblin.788</t>
+  </si>
+  <si>
+    <t>Faddis.634</t>
+  </si>
+  <si>
+    <t>Binns.159</t>
+  </si>
+  <si>
+    <t>Hepfer.154</t>
+  </si>
+  <si>
+    <t>Slade.484</t>
+  </si>
+  <si>
+    <t>Papp.563</t>
+  </si>
+  <si>
+    <t>Encinas.262</t>
+  </si>
+  <si>
+    <t>Mcdonald.342</t>
+  </si>
+  <si>
+    <t>Benigno.116</t>
+  </si>
+  <si>
+    <t>Brinkley.866</t>
+  </si>
+  <si>
+    <t>Certain.335</t>
+  </si>
+  <si>
+    <t>Cypher.353</t>
+  </si>
+  <si>
+    <t>Lautenschlage.917</t>
+  </si>
+  <si>
+    <t>Rushford.890</t>
+  </si>
+  <si>
+    <t>Delossantos.38</t>
+  </si>
+  <si>
+    <t>Slee.951</t>
+  </si>
+  <si>
+    <t>Moretti.365</t>
+  </si>
+  <si>
+    <t>Rainer.108</t>
+  </si>
+  <si>
+    <t>Breitenstein.677</t>
+  </si>
+  <si>
+    <t>Coletta.344</t>
+  </si>
+  <si>
+    <t>Hieber.798</t>
+  </si>
+  <si>
+    <t>Closson.956</t>
+  </si>
+  <si>
+    <t>Tully.114</t>
+  </si>
+  <si>
+    <t>Caywood.170</t>
+  </si>
+  <si>
+    <t>Silsby.242</t>
+  </si>
+  <si>
+    <t>Tait.159</t>
+  </si>
+  <si>
+    <t>Aleman.73</t>
+  </si>
+  <si>
+    <t>Brindley.439</t>
+  </si>
+  <si>
+    <t>Dicarlo.674</t>
+  </si>
+  <si>
+    <t>Florez.613</t>
+  </si>
+  <si>
+    <t>Sawyers.890</t>
+  </si>
+  <si>
+    <t>Byrne.461</t>
+  </si>
+  <si>
+    <t>Hagar.119</t>
+  </si>
+  <si>
+    <t>Goldie.250</t>
+  </si>
+  <si>
+    <t>Monfort.301</t>
+  </si>
+  <si>
+    <t>Toll.679</t>
+  </si>
+  <si>
+    <t>Gammage.15</t>
+  </si>
+  <si>
+    <t>Darnell.242</t>
+  </si>
+  <si>
+    <t>Paro.334</t>
+  </si>
+  <si>
+    <t>Barwick.128</t>
+  </si>
+  <si>
+    <t>Dugger.786</t>
+  </si>
+  <si>
+    <t>Leibowitz.835</t>
+  </si>
+  <si>
+    <t>Krebsbach.938</t>
   </si>
 </sst>
 </file>
@@ -2527,7 +2527,7 @@
   <dimension ref="A1:E226"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="A6:XFD6"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2587,7 +2587,7 @@
         <v>6</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>468</v>
+        <v>476</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -2604,7 +2604,7 @@
         <v>6</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>469</v>
+        <v>477</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -2621,15 +2621,15 @@
         <v>10</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>470</v>
+        <v>478</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>691</v>
+        <v>473</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>692</v>
+        <v>474</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>5</v>
@@ -2638,7 +2638,7 @@
         <v>10</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>693</v>
+        <v>475</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -2655,7 +2655,7 @@
         <v>6</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>471</v>
+        <v>479</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -2672,7 +2672,7 @@
         <v>10</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>472</v>
+        <v>480</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -2689,7 +2689,7 @@
         <v>6</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>473</v>
+        <v>481</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -2706,7 +2706,7 @@
         <v>10</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>474</v>
+        <v>482</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -2723,7 +2723,7 @@
         <v>10</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>475</v>
+        <v>483</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -2740,7 +2740,7 @@
         <v>6</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>476</v>
+        <v>484</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -2757,7 +2757,7 @@
         <v>10</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>477</v>
+        <v>485</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -2774,7 +2774,7 @@
         <v>6</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>478</v>
+        <v>486</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -2791,7 +2791,7 @@
         <v>10</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>479</v>
+        <v>487</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -2808,7 +2808,7 @@
         <v>21</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>480</v>
+        <v>488</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -2825,7 +2825,7 @@
         <v>23</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>481</v>
+        <v>489</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -2842,7 +2842,7 @@
         <v>23</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>482</v>
+        <v>490</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -2859,7 +2859,7 @@
         <v>21</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>483</v>
+        <v>491</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -2876,7 +2876,7 @@
         <v>21</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>484</v>
+        <v>492</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -2893,7 +2893,7 @@
         <v>23</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>485</v>
+        <v>493</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -2910,7 +2910,7 @@
         <v>21</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>486</v>
+        <v>494</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -2927,7 +2927,7 @@
         <v>21</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>487</v>
+        <v>495</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -2944,7 +2944,7 @@
         <v>21</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>488</v>
+        <v>496</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -2961,7 +2961,7 @@
         <v>23</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>489</v>
+        <v>497</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -2978,7 +2978,7 @@
         <v>23</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>490</v>
+        <v>498</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -2995,7 +2995,7 @@
         <v>23</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>491</v>
+        <v>499</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -3012,7 +3012,7 @@
         <v>23</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>492</v>
+        <v>500</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -3029,7 +3029,7 @@
         <v>21</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>493</v>
+        <v>501</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -3046,7 +3046,7 @@
         <v>37</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>494</v>
+        <v>502</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -3063,7 +3063,7 @@
         <v>37</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>495</v>
+        <v>503</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -3080,7 +3080,7 @@
         <v>37</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>496</v>
+        <v>504</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -3097,7 +3097,7 @@
         <v>37</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>497</v>
+        <v>505</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -3114,7 +3114,7 @@
         <v>37</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>498</v>
+        <v>506</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -3131,7 +3131,7 @@
         <v>37</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>499</v>
+        <v>507</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -3148,7 +3148,7 @@
         <v>37</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>500</v>
+        <v>508</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -3165,7 +3165,7 @@
         <v>37</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>501</v>
+        <v>509</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -3182,7 +3182,7 @@
         <v>37</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>502</v>
+        <v>510</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -3199,7 +3199,7 @@
         <v>37</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>503</v>
+        <v>511</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -3216,7 +3216,7 @@
         <v>37</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>504</v>
+        <v>468</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -3233,7 +3233,7 @@
         <v>37</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>505</v>
+        <v>512</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -3250,7 +3250,7 @@
         <v>37</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>506</v>
+        <v>513</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -3267,7 +3267,7 @@
         <v>37</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>507</v>
+        <v>514</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -3282,7 +3282,7 @@
       </c>
       <c r="D44" s="6"/>
       <c r="E44" s="4" t="s">
-        <v>508</v>
+        <v>515</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -3297,7 +3297,7 @@
       </c>
       <c r="D45" s="6"/>
       <c r="E45" s="4" t="s">
-        <v>509</v>
+        <v>516</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -3312,7 +3312,7 @@
       </c>
       <c r="D46" s="6"/>
       <c r="E46" s="4" t="s">
-        <v>510</v>
+        <v>517</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -3327,7 +3327,7 @@
       </c>
       <c r="D47" s="6"/>
       <c r="E47" s="4" t="s">
-        <v>511</v>
+        <v>518</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -3342,7 +3342,7 @@
       </c>
       <c r="D48" s="6"/>
       <c r="E48" s="4" t="s">
-        <v>512</v>
+        <v>519</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -3357,7 +3357,7 @@
       </c>
       <c r="D49" s="6"/>
       <c r="E49" s="4" t="s">
-        <v>513</v>
+        <v>520</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -3372,7 +3372,7 @@
       </c>
       <c r="D50" s="6"/>
       <c r="E50" s="4" t="s">
-        <v>514</v>
+        <v>521</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -3387,7 +3387,7 @@
       </c>
       <c r="D51" s="6"/>
       <c r="E51" s="4" t="s">
-        <v>515</v>
+        <v>522</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -3402,7 +3402,7 @@
       </c>
       <c r="D52" s="6"/>
       <c r="E52" s="4" t="s">
-        <v>516</v>
+        <v>523</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -3417,7 +3417,7 @@
       </c>
       <c r="D53" s="6"/>
       <c r="E53" s="4" t="s">
-        <v>517</v>
+        <v>524</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -3432,7 +3432,7 @@
       </c>
       <c r="D54" s="6"/>
       <c r="E54" s="4" t="s">
-        <v>518</v>
+        <v>525</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -3447,7 +3447,7 @@
       </c>
       <c r="D55" s="6"/>
       <c r="E55" s="4" t="s">
-        <v>519</v>
+        <v>526</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -3462,7 +3462,7 @@
       </c>
       <c r="D56" s="6"/>
       <c r="E56" s="4" t="s">
-        <v>520</v>
+        <v>527</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -3477,7 +3477,7 @@
       </c>
       <c r="D57" s="8"/>
       <c r="E57" s="4" t="s">
-        <v>521</v>
+        <v>528</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -3494,7 +3494,7 @@
         <v>68</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>522</v>
+        <v>529</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -3511,7 +3511,7 @@
         <v>23</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>523</v>
+        <v>530</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -3528,7 +3528,7 @@
         <v>21</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>524</v>
+        <v>531</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -3545,7 +3545,7 @@
         <v>21</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>525</v>
+        <v>532</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -3562,7 +3562,7 @@
         <v>23</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>526</v>
+        <v>533</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -3579,7 +3579,7 @@
         <v>68</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>527</v>
+        <v>534</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -3596,7 +3596,7 @@
         <v>21</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>528</v>
+        <v>535</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -3613,7 +3613,7 @@
         <v>23</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>529</v>
+        <v>536</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -3630,7 +3630,7 @@
         <v>21</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>530</v>
+        <v>537</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -3647,7 +3647,7 @@
         <v>23</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>531</v>
+        <v>538</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -3664,7 +3664,7 @@
         <v>68</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>532</v>
+        <v>539</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -3681,7 +3681,7 @@
         <v>23</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>533</v>
+        <v>540</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -3698,7 +3698,7 @@
         <v>21</v>
       </c>
       <c r="E70" s="4" t="s">
-        <v>534</v>
+        <v>541</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -3715,7 +3715,7 @@
         <v>23</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>535</v>
+        <v>542</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -3730,7 +3730,7 @@
       </c>
       <c r="D72" s="6"/>
       <c r="E72" s="4" t="s">
-        <v>536</v>
+        <v>543</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -3745,7 +3745,7 @@
       </c>
       <c r="D73" s="6"/>
       <c r="E73" s="4" t="s">
-        <v>537</v>
+        <v>544</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -3760,7 +3760,7 @@
       </c>
       <c r="D74" s="6"/>
       <c r="E74" s="4" t="s">
-        <v>538</v>
+        <v>545</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -3775,7 +3775,7 @@
       </c>
       <c r="D75" s="6"/>
       <c r="E75" s="4" t="s">
-        <v>539</v>
+        <v>546</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -3790,7 +3790,7 @@
       </c>
       <c r="D76" s="6"/>
       <c r="E76" s="4" t="s">
-        <v>540</v>
+        <v>547</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -3805,7 +3805,7 @@
       </c>
       <c r="D77" s="6"/>
       <c r="E77" s="4" t="s">
-        <v>541</v>
+        <v>548</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -3820,7 +3820,7 @@
       </c>
       <c r="D78" s="6"/>
       <c r="E78" s="4" t="s">
-        <v>542</v>
+        <v>549</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -3835,7 +3835,7 @@
       </c>
       <c r="D79" s="6"/>
       <c r="E79" s="4" t="s">
-        <v>543</v>
+        <v>550</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -3850,7 +3850,7 @@
       </c>
       <c r="D80" s="6"/>
       <c r="E80" s="4" t="s">
-        <v>544</v>
+        <v>469</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -3865,7 +3865,7 @@
       </c>
       <c r="D81" s="6"/>
       <c r="E81" s="4" t="s">
-        <v>545</v>
+        <v>551</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -3880,7 +3880,7 @@
       </c>
       <c r="D82" s="6"/>
       <c r="E82" s="4" t="s">
-        <v>546</v>
+        <v>552</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -3895,7 +3895,7 @@
       </c>
       <c r="D83" s="6"/>
       <c r="E83" s="4" t="s">
-        <v>547</v>
+        <v>553</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -3910,7 +3910,7 @@
       </c>
       <c r="D84" s="6"/>
       <c r="E84" s="4" t="s">
-        <v>548</v>
+        <v>554</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -3925,7 +3925,7 @@
       </c>
       <c r="D85" s="8"/>
       <c r="E85" s="4" t="s">
-        <v>549</v>
+        <v>555</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -3940,7 +3940,7 @@
       </c>
       <c r="D86" s="6"/>
       <c r="E86" s="4" t="s">
-        <v>550</v>
+        <v>556</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -3955,7 +3955,7 @@
       </c>
       <c r="D87" s="6"/>
       <c r="E87" s="4" t="s">
-        <v>551</v>
+        <v>557</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -3970,7 +3970,7 @@
       </c>
       <c r="D88" s="6"/>
       <c r="E88" s="4" t="s">
-        <v>552</v>
+        <v>558</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -3985,7 +3985,7 @@
       </c>
       <c r="D89" s="6"/>
       <c r="E89" s="4" t="s">
-        <v>553</v>
+        <v>559</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -4000,7 +4000,7 @@
       </c>
       <c r="D90" s="6"/>
       <c r="E90" s="4" t="s">
-        <v>554</v>
+        <v>560</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -4015,7 +4015,7 @@
       </c>
       <c r="D91" s="6"/>
       <c r="E91" s="4" t="s">
-        <v>555</v>
+        <v>561</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -4030,7 +4030,7 @@
       </c>
       <c r="D92" s="6"/>
       <c r="E92" s="4" t="s">
-        <v>556</v>
+        <v>562</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -4045,7 +4045,7 @@
       </c>
       <c r="D93" s="6"/>
       <c r="E93" s="4" t="s">
-        <v>557</v>
+        <v>563</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -4060,7 +4060,7 @@
       </c>
       <c r="D94" s="6"/>
       <c r="E94" s="4" t="s">
-        <v>558</v>
+        <v>564</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -4075,7 +4075,7 @@
       </c>
       <c r="D95" s="6"/>
       <c r="E95" s="4" t="s">
-        <v>559</v>
+        <v>565</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -4090,7 +4090,7 @@
       </c>
       <c r="D96" s="6"/>
       <c r="E96" s="4" t="s">
-        <v>560</v>
+        <v>566</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -4105,7 +4105,7 @@
       </c>
       <c r="D97" s="6"/>
       <c r="E97" s="4" t="s">
-        <v>561</v>
+        <v>567</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -4120,7 +4120,7 @@
       </c>
       <c r="D98" s="6"/>
       <c r="E98" s="4" t="s">
-        <v>562</v>
+        <v>568</v>
       </c>
     </row>
     <row r="99" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -4135,7 +4135,7 @@
       </c>
       <c r="D99" s="8"/>
       <c r="E99" s="4" t="s">
-        <v>563</v>
+        <v>569</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -4150,7 +4150,7 @@
       </c>
       <c r="D100" s="6"/>
       <c r="E100" s="4" t="s">
-        <v>564</v>
+        <v>570</v>
       </c>
     </row>
     <row r="101" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -4165,7 +4165,7 @@
       </c>
       <c r="D101" s="6"/>
       <c r="E101" s="4" t="s">
-        <v>565</v>
+        <v>571</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -4180,7 +4180,7 @@
       </c>
       <c r="D102" s="6"/>
       <c r="E102" s="4" t="s">
-        <v>566</v>
+        <v>572</v>
       </c>
     </row>
     <row r="103" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -4195,7 +4195,7 @@
       </c>
       <c r="D103" s="6"/>
       <c r="E103" s="4" t="s">
-        <v>567</v>
+        <v>573</v>
       </c>
     </row>
     <row r="104" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -4210,7 +4210,7 @@
       </c>
       <c r="D104" s="6"/>
       <c r="E104" s="4" t="s">
-        <v>568</v>
+        <v>574</v>
       </c>
     </row>
     <row r="105" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -4225,7 +4225,7 @@
       </c>
       <c r="D105" s="6"/>
       <c r="E105" s="4" t="s">
-        <v>569</v>
+        <v>575</v>
       </c>
     </row>
     <row r="106" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -4240,7 +4240,7 @@
       </c>
       <c r="D106" s="6"/>
       <c r="E106" s="4" t="s">
-        <v>570</v>
+        <v>576</v>
       </c>
     </row>
     <row r="107" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -4255,7 +4255,7 @@
       </c>
       <c r="D107" s="6"/>
       <c r="E107" s="4" t="s">
-        <v>571</v>
+        <v>577</v>
       </c>
     </row>
     <row r="108" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -4270,7 +4270,7 @@
       </c>
       <c r="D108" s="6"/>
       <c r="E108" s="4" t="s">
-        <v>572</v>
+        <v>578</v>
       </c>
     </row>
     <row r="109" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -4285,7 +4285,7 @@
       </c>
       <c r="D109" s="6"/>
       <c r="E109" s="4" t="s">
-        <v>573</v>
+        <v>579</v>
       </c>
     </row>
     <row r="110" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -4300,7 +4300,7 @@
       </c>
       <c r="D110" s="6"/>
       <c r="E110" s="4" t="s">
-        <v>574</v>
+        <v>580</v>
       </c>
     </row>
     <row r="111" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -4315,7 +4315,7 @@
       </c>
       <c r="D111" s="6"/>
       <c r="E111" s="4" t="s">
-        <v>575</v>
+        <v>581</v>
       </c>
     </row>
     <row r="112" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -4330,7 +4330,7 @@
       </c>
       <c r="D112" s="6"/>
       <c r="E112" s="4" t="s">
-        <v>576</v>
+        <v>582</v>
       </c>
     </row>
     <row r="113" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -4345,7 +4345,7 @@
       </c>
       <c r="D113" s="6"/>
       <c r="E113" s="4" t="s">
-        <v>577</v>
+        <v>583</v>
       </c>
     </row>
     <row r="114" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -4360,7 +4360,7 @@
       </c>
       <c r="D114" s="8"/>
       <c r="E114" s="4" t="s">
-        <v>578</v>
+        <v>584</v>
       </c>
     </row>
     <row r="115" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -4375,7 +4375,7 @@
       </c>
       <c r="D115" s="6"/>
       <c r="E115" s="4" t="s">
-        <v>579</v>
+        <v>585</v>
       </c>
     </row>
     <row r="116" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -4390,7 +4390,7 @@
       </c>
       <c r="D116" s="6"/>
       <c r="E116" s="4" t="s">
-        <v>580</v>
+        <v>586</v>
       </c>
     </row>
     <row r="117" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -4405,7 +4405,7 @@
       </c>
       <c r="D117" s="6"/>
       <c r="E117" s="4" t="s">
-        <v>581</v>
+        <v>587</v>
       </c>
     </row>
     <row r="118" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -4420,7 +4420,7 @@
       </c>
       <c r="D118" s="6"/>
       <c r="E118" s="4" t="s">
-        <v>582</v>
+        <v>588</v>
       </c>
     </row>
     <row r="119" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -4435,7 +4435,7 @@
       </c>
       <c r="D119" s="6"/>
       <c r="E119" s="4" t="s">
-        <v>583</v>
+        <v>589</v>
       </c>
     </row>
     <row r="120" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -4450,7 +4450,7 @@
       </c>
       <c r="D120" s="6"/>
       <c r="E120" s="4" t="s">
-        <v>584</v>
+        <v>470</v>
       </c>
     </row>
     <row r="121" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -4465,7 +4465,7 @@
       </c>
       <c r="D121" s="6"/>
       <c r="E121" s="4" t="s">
-        <v>585</v>
+        <v>590</v>
       </c>
     </row>
     <row r="122" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -4480,7 +4480,7 @@
       </c>
       <c r="D122" s="6"/>
       <c r="E122" s="4" t="s">
-        <v>586</v>
+        <v>591</v>
       </c>
     </row>
     <row r="123" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -4495,7 +4495,7 @@
       </c>
       <c r="D123" s="6"/>
       <c r="E123" s="4" t="s">
-        <v>587</v>
+        <v>592</v>
       </c>
     </row>
     <row r="124" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -4510,7 +4510,7 @@
       </c>
       <c r="D124" s="6"/>
       <c r="E124" s="4" t="s">
-        <v>588</v>
+        <v>593</v>
       </c>
     </row>
     <row r="125" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -4525,7 +4525,7 @@
       </c>
       <c r="D125" s="6"/>
       <c r="E125" s="4" t="s">
-        <v>589</v>
+        <v>594</v>
       </c>
     </row>
     <row r="126" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -4540,7 +4540,7 @@
       </c>
       <c r="D126" s="6"/>
       <c r="E126" s="4" t="s">
-        <v>590</v>
+        <v>595</v>
       </c>
     </row>
     <row r="127" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -4555,7 +4555,7 @@
       </c>
       <c r="D127" s="6"/>
       <c r="E127" s="4" t="s">
-        <v>591</v>
+        <v>596</v>
       </c>
     </row>
     <row r="128" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -4570,7 +4570,7 @@
       </c>
       <c r="D128" s="8"/>
       <c r="E128" s="4" t="s">
-        <v>592</v>
+        <v>597</v>
       </c>
     </row>
     <row r="129" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -4585,7 +4585,7 @@
       </c>
       <c r="D129" s="6"/>
       <c r="E129" s="4" t="s">
-        <v>593</v>
+        <v>598</v>
       </c>
     </row>
     <row r="130" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -4600,7 +4600,7 @@
       </c>
       <c r="D130" s="6"/>
       <c r="E130" s="4" t="s">
-        <v>594</v>
+        <v>599</v>
       </c>
     </row>
     <row r="131" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -4615,7 +4615,7 @@
       </c>
       <c r="D131" s="6"/>
       <c r="E131" s="4" t="s">
-        <v>595</v>
+        <v>600</v>
       </c>
     </row>
     <row r="132" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -4630,7 +4630,7 @@
       </c>
       <c r="D132" s="6"/>
       <c r="E132" s="4" t="s">
-        <v>596</v>
+        <v>601</v>
       </c>
     </row>
     <row r="133" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -4645,7 +4645,7 @@
       </c>
       <c r="D133" s="6"/>
       <c r="E133" s="4" t="s">
-        <v>597</v>
+        <v>602</v>
       </c>
     </row>
     <row r="134" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -4660,7 +4660,7 @@
       </c>
       <c r="D134" s="6"/>
       <c r="E134" s="4" t="s">
-        <v>598</v>
+        <v>603</v>
       </c>
     </row>
     <row r="135" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -4675,7 +4675,7 @@
       </c>
       <c r="D135" s="6"/>
       <c r="E135" s="4" t="s">
-        <v>599</v>
+        <v>604</v>
       </c>
     </row>
     <row r="136" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -4690,7 +4690,7 @@
       </c>
       <c r="D136" s="6"/>
       <c r="E136" s="4" t="s">
-        <v>600</v>
+        <v>605</v>
       </c>
     </row>
     <row r="137" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -4705,7 +4705,7 @@
       </c>
       <c r="D137" s="6"/>
       <c r="E137" s="4" t="s">
-        <v>601</v>
+        <v>606</v>
       </c>
     </row>
     <row r="138" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -4720,7 +4720,7 @@
       </c>
       <c r="D138" s="6"/>
       <c r="E138" s="4" t="s">
-        <v>602</v>
+        <v>607</v>
       </c>
     </row>
     <row r="139" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -4735,7 +4735,7 @@
       </c>
       <c r="D139" s="6"/>
       <c r="E139" s="4" t="s">
-        <v>603</v>
+        <v>608</v>
       </c>
     </row>
     <row r="140" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -4750,7 +4750,7 @@
       </c>
       <c r="D140" s="6"/>
       <c r="E140" s="4" t="s">
-        <v>604</v>
+        <v>609</v>
       </c>
     </row>
     <row r="141" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -4765,7 +4765,7 @@
       </c>
       <c r="D141" s="6"/>
       <c r="E141" s="4" t="s">
-        <v>605</v>
+        <v>610</v>
       </c>
     </row>
     <row r="142" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -4780,7 +4780,7 @@
       </c>
       <c r="D142" s="6"/>
       <c r="E142" s="4" t="s">
-        <v>606</v>
+        <v>611</v>
       </c>
     </row>
     <row r="143" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -4795,7 +4795,7 @@
       </c>
       <c r="D143" s="6"/>
       <c r="E143" s="4" t="s">
-        <v>607</v>
+        <v>612</v>
       </c>
     </row>
     <row r="144" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -4810,7 +4810,7 @@
       </c>
       <c r="D144" s="6"/>
       <c r="E144" s="4" t="s">
-        <v>608</v>
+        <v>613</v>
       </c>
     </row>
     <row r="145" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -4825,7 +4825,7 @@
       </c>
       <c r="D145" s="6"/>
       <c r="E145" s="4" t="s">
-        <v>609</v>
+        <v>614</v>
       </c>
     </row>
     <row r="146" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -4840,7 +4840,7 @@
       </c>
       <c r="D146" s="6"/>
       <c r="E146" s="4" t="s">
-        <v>610</v>
+        <v>615</v>
       </c>
     </row>
     <row r="147" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -4855,7 +4855,7 @@
       </c>
       <c r="D147" s="6"/>
       <c r="E147" s="4" t="s">
-        <v>611</v>
+        <v>616</v>
       </c>
     </row>
     <row r="148" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -4870,7 +4870,7 @@
       </c>
       <c r="D148" s="6"/>
       <c r="E148" s="4" t="s">
-        <v>612</v>
+        <v>617</v>
       </c>
     </row>
     <row r="149" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -4885,7 +4885,7 @@
       </c>
       <c r="D149" s="6"/>
       <c r="E149" s="4" t="s">
-        <v>613</v>
+        <v>618</v>
       </c>
     </row>
     <row r="150" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -4900,7 +4900,7 @@
       </c>
       <c r="D150" s="6"/>
       <c r="E150" s="4" t="s">
-        <v>614</v>
+        <v>619</v>
       </c>
     </row>
     <row r="151" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -4915,7 +4915,7 @@
       </c>
       <c r="D151" s="6"/>
       <c r="E151" s="4" t="s">
-        <v>615</v>
+        <v>620</v>
       </c>
     </row>
     <row r="152" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -4930,7 +4930,7 @@
       </c>
       <c r="D152" s="6"/>
       <c r="E152" s="4" t="s">
-        <v>616</v>
+        <v>621</v>
       </c>
     </row>
     <row r="153" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -4945,7 +4945,7 @@
       </c>
       <c r="D153" s="6"/>
       <c r="E153" s="4" t="s">
-        <v>617</v>
+        <v>622</v>
       </c>
     </row>
     <row r="154" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -4960,7 +4960,7 @@
       </c>
       <c r="D154" s="6"/>
       <c r="E154" s="4" t="s">
-        <v>618</v>
+        <v>623</v>
       </c>
     </row>
     <row r="155" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -4975,7 +4975,7 @@
       </c>
       <c r="D155" s="6"/>
       <c r="E155" s="4" t="s">
-        <v>619</v>
+        <v>624</v>
       </c>
     </row>
     <row r="156" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -4990,7 +4990,7 @@
       </c>
       <c r="D156" s="8"/>
       <c r="E156" s="4" t="s">
-        <v>620</v>
+        <v>625</v>
       </c>
     </row>
     <row r="157" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -5007,7 +5007,7 @@
         <v>21</v>
       </c>
       <c r="E157" s="4" t="s">
-        <v>621</v>
+        <v>626</v>
       </c>
     </row>
     <row r="158" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -5024,7 +5024,7 @@
         <v>23</v>
       </c>
       <c r="E158" s="4" t="s">
-        <v>622</v>
+        <v>627</v>
       </c>
     </row>
     <row r="159" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -5041,7 +5041,7 @@
         <v>68</v>
       </c>
       <c r="E159" s="4" t="s">
-        <v>623</v>
+        <v>628</v>
       </c>
     </row>
     <row r="160" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -5058,7 +5058,7 @@
         <v>21</v>
       </c>
       <c r="E160" s="4" t="s">
-        <v>624</v>
+        <v>471</v>
       </c>
     </row>
     <row r="161" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -5075,7 +5075,7 @@
         <v>23</v>
       </c>
       <c r="E161" s="4" t="s">
-        <v>625</v>
+        <v>629</v>
       </c>
     </row>
     <row r="162" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -5092,7 +5092,7 @@
         <v>21</v>
       </c>
       <c r="E162" s="4" t="s">
-        <v>626</v>
+        <v>630</v>
       </c>
     </row>
     <row r="163" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -5109,7 +5109,7 @@
         <v>68</v>
       </c>
       <c r="E163" s="4" t="s">
-        <v>627</v>
+        <v>631</v>
       </c>
     </row>
     <row r="164" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -5126,7 +5126,7 @@
         <v>23</v>
       </c>
       <c r="E164" s="4" t="s">
-        <v>628</v>
+        <v>632</v>
       </c>
     </row>
     <row r="165" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -5143,7 +5143,7 @@
         <v>23</v>
       </c>
       <c r="E165" s="4" t="s">
-        <v>629</v>
+        <v>633</v>
       </c>
     </row>
     <row r="166" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -5160,7 +5160,7 @@
         <v>23</v>
       </c>
       <c r="E166" s="4" t="s">
-        <v>630</v>
+        <v>634</v>
       </c>
     </row>
     <row r="167" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -5177,7 +5177,7 @@
         <v>21</v>
       </c>
       <c r="E167" s="4" t="s">
-        <v>631</v>
+        <v>635</v>
       </c>
     </row>
     <row r="168" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -5194,7 +5194,7 @@
         <v>23</v>
       </c>
       <c r="E168" s="4" t="s">
-        <v>632</v>
+        <v>636</v>
       </c>
     </row>
     <row r="169" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -5211,7 +5211,7 @@
         <v>21</v>
       </c>
       <c r="E169" s="4" t="s">
-        <v>633</v>
+        <v>637</v>
       </c>
     </row>
     <row r="170" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -5228,7 +5228,7 @@
         <v>68</v>
       </c>
       <c r="E170" s="4" t="s">
-        <v>634</v>
+        <v>638</v>
       </c>
     </row>
     <row r="171" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -5243,7 +5243,7 @@
       </c>
       <c r="D171" s="1"/>
       <c r="E171" s="4" t="s">
-        <v>635</v>
+        <v>639</v>
       </c>
     </row>
     <row r="172" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -5258,7 +5258,7 @@
       </c>
       <c r="D172" s="1"/>
       <c r="E172" s="4" t="s">
-        <v>636</v>
+        <v>640</v>
       </c>
     </row>
     <row r="173" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -5273,7 +5273,7 @@
       </c>
       <c r="D173" s="1"/>
       <c r="E173" s="4" t="s">
-        <v>637</v>
+        <v>641</v>
       </c>
     </row>
     <row r="174" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -5288,7 +5288,7 @@
       </c>
       <c r="D174" s="1"/>
       <c r="E174" s="4" t="s">
-        <v>638</v>
+        <v>642</v>
       </c>
     </row>
     <row r="175" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -5303,7 +5303,7 @@
       </c>
       <c r="D175" s="1"/>
       <c r="E175" s="4" t="s">
-        <v>639</v>
+        <v>643</v>
       </c>
     </row>
     <row r="176" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -5318,7 +5318,7 @@
       </c>
       <c r="D176" s="1"/>
       <c r="E176" s="4" t="s">
-        <v>640</v>
+        <v>644</v>
       </c>
     </row>
     <row r="177" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -5333,7 +5333,7 @@
       </c>
       <c r="D177" s="1"/>
       <c r="E177" s="4" t="s">
-        <v>641</v>
+        <v>645</v>
       </c>
     </row>
     <row r="178" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -5348,7 +5348,7 @@
       </c>
       <c r="D178" s="1"/>
       <c r="E178" s="4" t="s">
-        <v>642</v>
+        <v>646</v>
       </c>
     </row>
     <row r="179" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -5363,7 +5363,7 @@
       </c>
       <c r="D179" s="1"/>
       <c r="E179" s="4" t="s">
-        <v>643</v>
+        <v>647</v>
       </c>
     </row>
     <row r="180" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -5378,7 +5378,7 @@
       </c>
       <c r="D180" s="1"/>
       <c r="E180" s="4" t="s">
-        <v>644</v>
+        <v>648</v>
       </c>
     </row>
     <row r="181" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -5393,7 +5393,7 @@
       </c>
       <c r="D181" s="1"/>
       <c r="E181" s="4" t="s">
-        <v>645</v>
+        <v>649</v>
       </c>
     </row>
     <row r="182" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -5408,7 +5408,7 @@
       </c>
       <c r="D182" s="1"/>
       <c r="E182" s="4" t="s">
-        <v>646</v>
+        <v>650</v>
       </c>
     </row>
     <row r="183" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -5423,7 +5423,7 @@
       </c>
       <c r="D183" s="1"/>
       <c r="E183" s="4" t="s">
-        <v>647</v>
+        <v>651</v>
       </c>
     </row>
     <row r="184" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -5438,7 +5438,7 @@
       </c>
       <c r="D184" s="1"/>
       <c r="E184" s="4" t="s">
-        <v>648</v>
+        <v>652</v>
       </c>
     </row>
     <row r="185" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -5455,7 +5455,7 @@
         <v>37</v>
       </c>
       <c r="E185" s="4" t="s">
-        <v>649</v>
+        <v>653</v>
       </c>
     </row>
     <row r="186" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -5472,7 +5472,7 @@
         <v>21</v>
       </c>
       <c r="E186" s="4" t="s">
-        <v>650</v>
+        <v>654</v>
       </c>
     </row>
     <row r="187" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -5489,7 +5489,7 @@
         <v>37</v>
       </c>
       <c r="E187" s="4" t="s">
-        <v>651</v>
+        <v>655</v>
       </c>
     </row>
     <row r="188" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -5506,7 +5506,7 @@
         <v>21</v>
       </c>
       <c r="E188" s="4" t="s">
-        <v>652</v>
+        <v>656</v>
       </c>
     </row>
     <row r="189" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -5523,7 +5523,7 @@
         <v>37</v>
       </c>
       <c r="E189" s="4" t="s">
-        <v>653</v>
+        <v>657</v>
       </c>
     </row>
     <row r="190" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -5540,7 +5540,7 @@
         <v>21</v>
       </c>
       <c r="E190" s="4" t="s">
-        <v>654</v>
+        <v>658</v>
       </c>
     </row>
     <row r="191" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -5557,7 +5557,7 @@
         <v>37</v>
       </c>
       <c r="E191" s="4" t="s">
-        <v>655</v>
+        <v>659</v>
       </c>
     </row>
     <row r="192" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -5574,7 +5574,7 @@
         <v>21</v>
       </c>
       <c r="E192" s="4" t="s">
-        <v>656</v>
+        <v>660</v>
       </c>
     </row>
     <row r="193" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -5591,7 +5591,7 @@
         <v>37</v>
       </c>
       <c r="E193" s="4" t="s">
-        <v>657</v>
+        <v>661</v>
       </c>
     </row>
     <row r="194" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -5608,7 +5608,7 @@
         <v>21</v>
       </c>
       <c r="E194" s="4" t="s">
-        <v>658</v>
+        <v>662</v>
       </c>
     </row>
     <row r="195" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -5625,7 +5625,7 @@
         <v>37</v>
       </c>
       <c r="E195" s="4" t="s">
-        <v>659</v>
+        <v>663</v>
       </c>
     </row>
     <row r="196" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -5642,7 +5642,7 @@
         <v>21</v>
       </c>
       <c r="E196" s="4" t="s">
-        <v>660</v>
+        <v>664</v>
       </c>
     </row>
     <row r="197" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -5659,7 +5659,7 @@
         <v>37</v>
       </c>
       <c r="E197" s="4" t="s">
-        <v>661</v>
+        <v>665</v>
       </c>
     </row>
     <row r="198" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -5676,7 +5676,7 @@
         <v>21</v>
       </c>
       <c r="E198" s="4" t="s">
-        <v>662</v>
+        <v>666</v>
       </c>
     </row>
     <row r="199" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -5693,7 +5693,7 @@
         <v>21</v>
       </c>
       <c r="E199" s="4" t="s">
-        <v>663</v>
+        <v>667</v>
       </c>
     </row>
     <row r="200" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -5710,7 +5710,7 @@
         <v>21</v>
       </c>
       <c r="E200" s="4" t="s">
-        <v>664</v>
+        <v>472</v>
       </c>
     </row>
     <row r="201" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -5727,7 +5727,7 @@
         <v>23</v>
       </c>
       <c r="E201" s="4" t="s">
-        <v>665</v>
+        <v>668</v>
       </c>
     </row>
     <row r="202" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -5744,7 +5744,7 @@
         <v>23</v>
       </c>
       <c r="E202" s="4" t="s">
-        <v>666</v>
+        <v>669</v>
       </c>
     </row>
     <row r="203" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -5761,7 +5761,7 @@
         <v>21</v>
       </c>
       <c r="E203" s="4" t="s">
-        <v>667</v>
+        <v>670</v>
       </c>
     </row>
     <row r="204" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -5778,7 +5778,7 @@
         <v>23</v>
       </c>
       <c r="E204" s="4" t="s">
-        <v>668</v>
+        <v>671</v>
       </c>
     </row>
     <row r="205" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -5795,7 +5795,7 @@
         <v>23</v>
       </c>
       <c r="E205" s="4" t="s">
-        <v>669</v>
+        <v>672</v>
       </c>
     </row>
     <row r="206" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -5812,7 +5812,7 @@
         <v>21</v>
       </c>
       <c r="E206" s="4" t="s">
-        <v>670</v>
+        <v>673</v>
       </c>
     </row>
     <row r="207" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -5829,7 +5829,7 @@
         <v>21</v>
       </c>
       <c r="E207" s="4" t="s">
-        <v>671</v>
+        <v>674</v>
       </c>
     </row>
     <row r="208" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -5846,7 +5846,7 @@
         <v>23</v>
       </c>
       <c r="E208" s="4" t="s">
-        <v>672</v>
+        <v>675</v>
       </c>
     </row>
     <row r="209" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -5863,7 +5863,7 @@
         <v>21</v>
       </c>
       <c r="E209" s="4" t="s">
-        <v>673</v>
+        <v>676</v>
       </c>
     </row>
     <row r="210" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -5880,7 +5880,7 @@
         <v>23</v>
       </c>
       <c r="E210" s="4" t="s">
-        <v>674</v>
+        <v>677</v>
       </c>
     </row>
     <row r="211" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -5897,7 +5897,7 @@
         <v>21</v>
       </c>
       <c r="E211" s="4" t="s">
-        <v>675</v>
+        <v>678</v>
       </c>
     </row>
     <row r="212" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -5914,7 +5914,7 @@
         <v>23</v>
       </c>
       <c r="E212" s="4" t="s">
-        <v>676</v>
+        <v>679</v>
       </c>
     </row>
     <row r="213" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -5931,7 +5931,7 @@
         <v>10</v>
       </c>
       <c r="E213" s="4" t="s">
-        <v>677</v>
+        <v>680</v>
       </c>
     </row>
     <row r="214" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -5948,7 +5948,7 @@
         <v>6</v>
       </c>
       <c r="E214" s="4" t="s">
-        <v>678</v>
+        <v>681</v>
       </c>
     </row>
     <row r="215" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -5965,7 +5965,7 @@
         <v>10</v>
       </c>
       <c r="E215" s="4" t="s">
-        <v>679</v>
+        <v>682</v>
       </c>
     </row>
     <row r="216" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -5982,7 +5982,7 @@
         <v>10</v>
       </c>
       <c r="E216" s="4" t="s">
-        <v>680</v>
+        <v>683</v>
       </c>
     </row>
     <row r="217" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -5999,7 +5999,7 @@
         <v>6</v>
       </c>
       <c r="E217" s="4" t="s">
-        <v>681</v>
+        <v>684</v>
       </c>
     </row>
     <row r="218" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -6016,7 +6016,7 @@
         <v>6</v>
       </c>
       <c r="E218" s="4" t="s">
-        <v>682</v>
+        <v>685</v>
       </c>
     </row>
     <row r="219" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -6033,7 +6033,7 @@
         <v>10</v>
       </c>
       <c r="E219" s="4" t="s">
-        <v>683</v>
+        <v>686</v>
       </c>
     </row>
     <row r="220" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -6050,7 +6050,7 @@
         <v>6</v>
       </c>
       <c r="E220" s="4" t="s">
-        <v>684</v>
+        <v>687</v>
       </c>
     </row>
     <row r="221" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -6067,7 +6067,7 @@
         <v>6</v>
       </c>
       <c r="E221" s="11" t="s">
-        <v>685</v>
+        <v>688</v>
       </c>
     </row>
     <row r="222" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -6084,7 +6084,7 @@
         <v>6</v>
       </c>
       <c r="E222" s="4" t="s">
-        <v>686</v>
+        <v>689</v>
       </c>
     </row>
     <row r="223" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -6101,7 +6101,7 @@
         <v>10</v>
       </c>
       <c r="E223" s="4" t="s">
-        <v>687</v>
+        <v>690</v>
       </c>
     </row>
     <row r="224" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -6118,7 +6118,7 @@
         <v>6</v>
       </c>
       <c r="E224" s="4" t="s">
-        <v>688</v>
+        <v>691</v>
       </c>
     </row>
     <row r="225" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -6135,7 +6135,7 @@
         <v>6</v>
       </c>
       <c r="E225" s="4" t="s">
-        <v>689</v>
+        <v>692</v>
       </c>
     </row>
     <row r="226" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -6152,7 +6152,7 @@
         <v>10</v>
       </c>
       <c r="E226" s="4" t="s">
-        <v>690</v>
+        <v>693</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added info into mock data
</commit_message>
<xml_diff>
--- a/models/mock-data/FakeUsers.xlsx
+++ b/models/mock-data/FakeUsers.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-4600" windowWidth="51200" windowHeight="26740" tabRatio="500"/>
+    <workbookView xWindow="28800" yWindow="-4600" windowWidth="15120" windowHeight="26740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1017" uniqueCount="694">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1020" uniqueCount="697">
   <si>
     <t>Spot</t>
   </si>
@@ -2106,6 +2106,15 @@
   </si>
   <si>
     <t>Krebsbach.938</t>
+  </si>
+  <si>
+    <t>Eligible</t>
+  </si>
+  <si>
+    <t>SquadLeader</t>
+  </si>
+  <si>
+    <t>Admin</t>
   </si>
 </sst>
 </file>
@@ -2219,7 +2228,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -2236,6 +2245,8 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2524,10 +2535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E226"/>
+  <dimension ref="A1:H226"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A184" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H226"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2539,7 +2550,7 @@
     <col min="5" max="5" width="16.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2555,8 +2566,17 @@
       <c r="E1" s="1" t="s">
         <v>466</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>694</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>695</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -2572,8 +2592,17 @@
       <c r="E2" s="4" t="s">
         <v>467</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F2" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
@@ -2589,8 +2618,17 @@
       <c r="E3" s="4" t="s">
         <v>476</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F3" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
@@ -2606,8 +2644,17 @@
       <c r="E4" s="4" t="s">
         <v>477</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F4" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G4" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
@@ -2623,8 +2670,17 @@
       <c r="E5" s="4" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F5" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>473</v>
       </c>
@@ -2640,8 +2696,17 @@
       <c r="E6" s="4" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F6" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G6" t="b">
+        <v>0</v>
+      </c>
+      <c r="H6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>11</v>
       </c>
@@ -2657,8 +2722,17 @@
       <c r="E7" s="4" t="s">
         <v>479</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F7" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>12</v>
       </c>
@@ -2674,8 +2748,17 @@
       <c r="E8" s="4" t="s">
         <v>480</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F8" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G8" t="b">
+        <v>0</v>
+      </c>
+      <c r="H8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>13</v>
       </c>
@@ -2691,8 +2774,17 @@
       <c r="E9" s="4" t="s">
         <v>481</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F9" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G9" t="b">
+        <v>0</v>
+      </c>
+      <c r="H9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>14</v>
       </c>
@@ -2708,8 +2800,17 @@
       <c r="E10" s="4" t="s">
         <v>482</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F10" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G10" t="b">
+        <v>0</v>
+      </c>
+      <c r="H10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>15</v>
       </c>
@@ -2725,8 +2826,17 @@
       <c r="E11" s="4" t="s">
         <v>483</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F11" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G11" t="b">
+        <v>0</v>
+      </c>
+      <c r="H11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>16</v>
       </c>
@@ -2742,8 +2852,17 @@
       <c r="E12" s="4" t="s">
         <v>484</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F12" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G12" t="b">
+        <v>0</v>
+      </c>
+      <c r="H12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>17</v>
       </c>
@@ -2759,8 +2878,17 @@
       <c r="E13" s="4" t="s">
         <v>485</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F13" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>18</v>
       </c>
@@ -2776,8 +2904,17 @@
       <c r="E14" s="4" t="s">
         <v>486</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F14" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>19</v>
       </c>
@@ -2793,8 +2930,17 @@
       <c r="E15" s="4" t="s">
         <v>487</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F15" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>20</v>
       </c>
@@ -2810,8 +2956,17 @@
       <c r="E16" s="4" t="s">
         <v>488</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F16" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G16" t="b">
+        <v>1</v>
+      </c>
+      <c r="H16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>22</v>
       </c>
@@ -2827,8 +2982,17 @@
       <c r="E17" s="4" t="s">
         <v>489</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F17" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G17" t="b">
+        <v>0</v>
+      </c>
+      <c r="H17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>24</v>
       </c>
@@ -2844,8 +3008,17 @@
       <c r="E18" s="4" t="s">
         <v>490</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F18" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G18" t="b">
+        <v>0</v>
+      </c>
+      <c r="H18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>25</v>
       </c>
@@ -2861,8 +3034,17 @@
       <c r="E19" s="4" t="s">
         <v>491</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F19" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G19" t="b">
+        <v>0</v>
+      </c>
+      <c r="H19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>26</v>
       </c>
@@ -2878,8 +3060,17 @@
       <c r="E20" s="4" t="s">
         <v>492</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F20" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G20" t="b">
+        <v>0</v>
+      </c>
+      <c r="H20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>27</v>
       </c>
@@ -2895,8 +3086,17 @@
       <c r="E21" s="4" t="s">
         <v>493</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F21" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G21" t="b">
+        <v>0</v>
+      </c>
+      <c r="H21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>28</v>
       </c>
@@ -2912,8 +3112,17 @@
       <c r="E22" s="4" t="s">
         <v>494</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F22" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G22" t="b">
+        <v>0</v>
+      </c>
+      <c r="H22" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>29</v>
       </c>
@@ -2929,8 +3138,17 @@
       <c r="E23" s="4" t="s">
         <v>495</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F23" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G23" t="b">
+        <v>0</v>
+      </c>
+      <c r="H23" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>30</v>
       </c>
@@ -2946,8 +3164,17 @@
       <c r="E24" s="4" t="s">
         <v>496</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F24" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G24" t="b">
+        <v>0</v>
+      </c>
+      <c r="H24" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>31</v>
       </c>
@@ -2963,8 +3190,17 @@
       <c r="E25" s="4" t="s">
         <v>497</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F25" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G25" t="b">
+        <v>0</v>
+      </c>
+      <c r="H25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>32</v>
       </c>
@@ -2980,8 +3216,17 @@
       <c r="E26" s="4" t="s">
         <v>498</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F26" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G26" t="b">
+        <v>0</v>
+      </c>
+      <c r="H26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>33</v>
       </c>
@@ -2997,8 +3242,17 @@
       <c r="E27" s="4" t="s">
         <v>499</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F27" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G27" t="b">
+        <v>1</v>
+      </c>
+      <c r="H27" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>34</v>
       </c>
@@ -3014,8 +3268,17 @@
       <c r="E28" s="4" t="s">
         <v>500</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F28" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G28" t="b">
+        <v>0</v>
+      </c>
+      <c r="H28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>35</v>
       </c>
@@ -3031,8 +3294,17 @@
       <c r="E29" s="4" t="s">
         <v>501</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F29" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G29" t="b">
+        <v>0</v>
+      </c>
+      <c r="H29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>36</v>
       </c>
@@ -3048,8 +3320,17 @@
       <c r="E30" s="4" t="s">
         <v>502</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F30" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G30" t="b">
+        <v>1</v>
+      </c>
+      <c r="H30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>38</v>
       </c>
@@ -3065,8 +3346,17 @@
       <c r="E31" s="4" t="s">
         <v>503</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F31" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G31" t="b">
+        <v>0</v>
+      </c>
+      <c r="H31" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>39</v>
       </c>
@@ -3082,8 +3372,17 @@
       <c r="E32" s="4" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F32" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G32" t="b">
+        <v>0</v>
+      </c>
+      <c r="H32" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>40</v>
       </c>
@@ -3099,8 +3398,17 @@
       <c r="E33" s="4" t="s">
         <v>505</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F33" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G33" t="b">
+        <v>0</v>
+      </c>
+      <c r="H33" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>41</v>
       </c>
@@ -3116,8 +3424,17 @@
       <c r="E34" s="4" t="s">
         <v>506</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F34" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G34" t="b">
+        <v>0</v>
+      </c>
+      <c r="H34" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>42</v>
       </c>
@@ -3133,8 +3450,17 @@
       <c r="E35" s="4" t="s">
         <v>507</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F35" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G35" t="b">
+        <v>0</v>
+      </c>
+      <c r="H35" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>43</v>
       </c>
@@ -3150,8 +3476,17 @@
       <c r="E36" s="4" t="s">
         <v>508</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F36" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G36" t="b">
+        <v>0</v>
+      </c>
+      <c r="H36" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>44</v>
       </c>
@@ -3167,8 +3502,17 @@
       <c r="E37" s="4" t="s">
         <v>509</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F37" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G37" t="b">
+        <v>0</v>
+      </c>
+      <c r="H37" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>45</v>
       </c>
@@ -3184,8 +3528,17 @@
       <c r="E38" s="4" t="s">
         <v>510</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F38" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G38" t="b">
+        <v>0</v>
+      </c>
+      <c r="H38" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>46</v>
       </c>
@@ -3201,8 +3554,17 @@
       <c r="E39" s="4" t="s">
         <v>511</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F39" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G39" t="b">
+        <v>0</v>
+      </c>
+      <c r="H39" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>47</v>
       </c>
@@ -3218,8 +3580,17 @@
       <c r="E40" s="4" t="s">
         <v>468</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F40" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G40" t="b">
+        <v>0</v>
+      </c>
+      <c r="H40" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
         <v>48</v>
       </c>
@@ -3235,8 +3606,17 @@
       <c r="E41" s="4" t="s">
         <v>512</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F41" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G41" t="b">
+        <v>1</v>
+      </c>
+      <c r="H41" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>49</v>
       </c>
@@ -3252,8 +3632,17 @@
       <c r="E42" s="4" t="s">
         <v>513</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F42" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G42" t="b">
+        <v>0</v>
+      </c>
+      <c r="H42" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
         <v>50</v>
       </c>
@@ -3269,8 +3658,17 @@
       <c r="E43" s="4" t="s">
         <v>514</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F43" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G43" t="b">
+        <v>0</v>
+      </c>
+      <c r="H43" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>51</v>
       </c>
@@ -3284,8 +3682,17 @@
       <c r="E44" s="4" t="s">
         <v>515</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F44" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G44" t="b">
+        <v>1</v>
+      </c>
+      <c r="H44" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
         <v>53</v>
       </c>
@@ -3299,8 +3706,17 @@
       <c r="E45" s="4" t="s">
         <v>516</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F45" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G45" t="b">
+        <v>0</v>
+      </c>
+      <c r="H45" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
         <v>54</v>
       </c>
@@ -3314,8 +3730,17 @@
       <c r="E46" s="4" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F46" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G46" t="b">
+        <v>0</v>
+      </c>
+      <c r="H46" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>55</v>
       </c>
@@ -3329,8 +3754,17 @@
       <c r="E47" s="4" t="s">
         <v>518</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F47" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G47" t="b">
+        <v>0</v>
+      </c>
+      <c r="H47" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>56</v>
       </c>
@@ -3344,8 +3778,17 @@
       <c r="E48" s="4" t="s">
         <v>519</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F48" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G48" t="b">
+        <v>0</v>
+      </c>
+      <c r="H48" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
         <v>57</v>
       </c>
@@ -3359,8 +3802,17 @@
       <c r="E49" s="4" t="s">
         <v>520</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F49" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
         <v>58</v>
       </c>
@@ -3374,8 +3826,17 @@
       <c r="E50" s="4" t="s">
         <v>521</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F50" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G50" t="b">
+        <v>0</v>
+      </c>
+      <c r="H50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
         <v>59</v>
       </c>
@@ -3389,8 +3850,17 @@
       <c r="E51" s="4" t="s">
         <v>522</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F51" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G51" t="b">
+        <v>0</v>
+      </c>
+      <c r="H51" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
         <v>60</v>
       </c>
@@ -3404,8 +3874,17 @@
       <c r="E52" s="4" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F52" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G52" t="b">
+        <v>0</v>
+      </c>
+      <c r="H52" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
         <v>61</v>
       </c>
@@ -3419,8 +3898,17 @@
       <c r="E53" s="4" t="s">
         <v>524</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F53" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G53" t="b">
+        <v>0</v>
+      </c>
+      <c r="H53" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
         <v>62</v>
       </c>
@@ -3434,8 +3922,17 @@
       <c r="E54" s="4" t="s">
         <v>525</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F54" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G54" t="b">
+        <v>0</v>
+      </c>
+      <c r="H54" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
         <v>63</v>
       </c>
@@ -3449,8 +3946,17 @@
       <c r="E55" s="4" t="s">
         <v>526</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F55" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G55" t="b">
+        <v>1</v>
+      </c>
+      <c r="H55" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
         <v>64</v>
       </c>
@@ -3464,8 +3970,17 @@
       <c r="E56" s="4" t="s">
         <v>527</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F56" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G56" t="b">
+        <v>0</v>
+      </c>
+      <c r="H56" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
         <v>65</v>
       </c>
@@ -3479,8 +3994,17 @@
       <c r="E57" s="4" t="s">
         <v>528</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F57" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G57" t="b">
+        <v>0</v>
+      </c>
+      <c r="H57" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
         <v>66</v>
       </c>
@@ -3496,8 +4020,17 @@
       <c r="E58" s="4" t="s">
         <v>529</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F58" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G58" t="b">
+        <v>1</v>
+      </c>
+      <c r="H58" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
         <v>69</v>
       </c>
@@ -3513,8 +4046,17 @@
       <c r="E59" s="4" t="s">
         <v>530</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F59" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G59" t="b">
+        <v>0</v>
+      </c>
+      <c r="H59" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
         <v>70</v>
       </c>
@@ -3530,8 +4072,17 @@
       <c r="E60" s="4" t="s">
         <v>531</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F60" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G60" t="b">
+        <v>0</v>
+      </c>
+      <c r="H60" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
         <v>71</v>
       </c>
@@ -3547,8 +4098,17 @@
       <c r="E61" s="4" t="s">
         <v>532</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F61" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G61" t="b">
+        <v>0</v>
+      </c>
+      <c r="H61" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
         <v>72</v>
       </c>
@@ -3564,8 +4124,17 @@
       <c r="E62" s="4" t="s">
         <v>533</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F62" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G62" t="b">
+        <v>0</v>
+      </c>
+      <c r="H62" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
         <v>73</v>
       </c>
@@ -3581,8 +4150,17 @@
       <c r="E63" s="4" t="s">
         <v>534</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F63" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G63" t="b">
+        <v>0</v>
+      </c>
+      <c r="H63" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
         <v>234</v>
       </c>
@@ -3598,8 +4176,17 @@
       <c r="E64" s="4" t="s">
         <v>535</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F64" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G64" t="b">
+        <v>0</v>
+      </c>
+      <c r="H64" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
         <v>74</v>
       </c>
@@ -3615,8 +4202,17 @@
       <c r="E65" s="4" t="s">
         <v>536</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F65" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G65" t="b">
+        <v>0</v>
+      </c>
+      <c r="H65" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
         <v>75</v>
       </c>
@@ -3632,8 +4228,17 @@
       <c r="E66" s="4" t="s">
         <v>537</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F66" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G66" t="b">
+        <v>0</v>
+      </c>
+      <c r="H66" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
         <v>76</v>
       </c>
@@ -3649,8 +4254,17 @@
       <c r="E67" s="4" t="s">
         <v>538</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F67" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G67" t="b">
+        <v>0</v>
+      </c>
+      <c r="H67" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
         <v>77</v>
       </c>
@@ -3666,8 +4280,17 @@
       <c r="E68" s="4" t="s">
         <v>539</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F68" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G68" t="b">
+        <v>0</v>
+      </c>
+      <c r="H68" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
         <v>78</v>
       </c>
@@ -3683,8 +4306,17 @@
       <c r="E69" s="4" t="s">
         <v>540</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F69" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G69" t="b">
+        <v>1</v>
+      </c>
+      <c r="H69" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
         <v>79</v>
       </c>
@@ -3700,8 +4332,17 @@
       <c r="E70" s="4" t="s">
         <v>541</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F70" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G70" t="b">
+        <v>0</v>
+      </c>
+      <c r="H70" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
         <v>80</v>
       </c>
@@ -3717,8 +4358,17 @@
       <c r="E71" s="4" t="s">
         <v>542</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F71" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G71" t="b">
+        <v>0</v>
+      </c>
+      <c r="H71" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
         <v>235</v>
       </c>
@@ -3732,8 +4382,17 @@
       <c r="E72" s="4" t="s">
         <v>543</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F72" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G72" t="b">
+        <v>1</v>
+      </c>
+      <c r="H72" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
         <v>81</v>
       </c>
@@ -3747,8 +4406,17 @@
       <c r="E73" s="4" t="s">
         <v>544</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F73" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G73" t="b">
+        <v>0</v>
+      </c>
+      <c r="H73" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
         <v>83</v>
       </c>
@@ -3762,8 +4430,17 @@
       <c r="E74" s="4" t="s">
         <v>545</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F74" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G74" t="b">
+        <v>0</v>
+      </c>
+      <c r="H74" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
         <v>84</v>
       </c>
@@ -3777,8 +4454,17 @@
       <c r="E75" s="4" t="s">
         <v>546</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F75" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G75" t="b">
+        <v>0</v>
+      </c>
+      <c r="H75" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
         <v>85</v>
       </c>
@@ -3792,8 +4478,17 @@
       <c r="E76" s="4" t="s">
         <v>547</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F76" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G76" t="b">
+        <v>0</v>
+      </c>
+      <c r="H76" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
         <v>86</v>
       </c>
@@ -3807,8 +4502,17 @@
       <c r="E77" s="4" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F77" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G77" t="b">
+        <v>0</v>
+      </c>
+      <c r="H77" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
         <v>87</v>
       </c>
@@ -3822,8 +4526,17 @@
       <c r="E78" s="4" t="s">
         <v>549</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F78" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G78" t="b">
+        <v>0</v>
+      </c>
+      <c r="H78" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
         <v>88</v>
       </c>
@@ -3837,8 +4550,17 @@
       <c r="E79" s="4" t="s">
         <v>550</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F79" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G79" t="b">
+        <v>0</v>
+      </c>
+      <c r="H79" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
         <v>89</v>
       </c>
@@ -3852,8 +4574,17 @@
       <c r="E80" s="4" t="s">
         <v>469</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F80" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G80" t="b">
+        <v>0</v>
+      </c>
+      <c r="H80" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
         <v>90</v>
       </c>
@@ -3867,8 +4598,17 @@
       <c r="E81" s="4" t="s">
         <v>551</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F81" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G81" t="b">
+        <v>0</v>
+      </c>
+      <c r="H81" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
         <v>91</v>
       </c>
@@ -3882,8 +4622,17 @@
       <c r="E82" s="4" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F82" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G82" t="b">
+        <v>0</v>
+      </c>
+      <c r="H82" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
         <v>92</v>
       </c>
@@ -3897,8 +4646,17 @@
       <c r="E83" s="4" t="s">
         <v>553</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F83" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G83" t="b">
+        <v>1</v>
+      </c>
+      <c r="H83" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
         <v>93</v>
       </c>
@@ -3912,8 +4670,17 @@
       <c r="E84" s="4" t="s">
         <v>554</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F84" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G84" t="b">
+        <v>0</v>
+      </c>
+      <c r="H84" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A85" s="7" t="s">
         <v>94</v>
       </c>
@@ -3927,8 +4694,17 @@
       <c r="E85" s="4" t="s">
         <v>555</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F85" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G85" t="b">
+        <v>0</v>
+      </c>
+      <c r="H85" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
         <v>95</v>
       </c>
@@ -3942,8 +4718,17 @@
       <c r="E86" s="4" t="s">
         <v>556</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F86" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G86" t="b">
+        <v>1</v>
+      </c>
+      <c r="H86" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
         <v>97</v>
       </c>
@@ -3957,8 +4742,17 @@
       <c r="E87" s="4" t="s">
         <v>557</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F87" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G87" t="b">
+        <v>0</v>
+      </c>
+      <c r="H87" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
         <v>98</v>
       </c>
@@ -3972,8 +4766,17 @@
       <c r="E88" s="4" t="s">
         <v>558</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F88" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G88" t="b">
+        <v>0</v>
+      </c>
+      <c r="H88" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
         <v>99</v>
       </c>
@@ -3987,8 +4790,17 @@
       <c r="E89" s="4" t="s">
         <v>559</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F89" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G89" t="b">
+        <v>0</v>
+      </c>
+      <c r="H89" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
         <v>100</v>
       </c>
@@ -4002,8 +4814,17 @@
       <c r="E90" s="4" t="s">
         <v>560</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F90" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G90" t="b">
+        <v>0</v>
+      </c>
+      <c r="H90" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
         <v>101</v>
       </c>
@@ -4017,8 +4838,17 @@
       <c r="E91" s="4" t="s">
         <v>561</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F91" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G91" t="b">
+        <v>1</v>
+      </c>
+      <c r="H91" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
         <v>102</v>
       </c>
@@ -4032,8 +4862,17 @@
       <c r="E92" s="4" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F92" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G92" t="b">
+        <v>0</v>
+      </c>
+      <c r="H92" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
         <v>103</v>
       </c>
@@ -4047,8 +4886,17 @@
       <c r="E93" s="4" t="s">
         <v>563</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F93" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G93" t="b">
+        <v>0</v>
+      </c>
+      <c r="H93" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
         <v>104</v>
       </c>
@@ -4062,8 +4910,17 @@
       <c r="E94" s="4" t="s">
         <v>564</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F94" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G94" t="b">
+        <v>0</v>
+      </c>
+      <c r="H94" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
         <v>105</v>
       </c>
@@ -4077,8 +4934,17 @@
       <c r="E95" s="4" t="s">
         <v>565</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F95" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G95" t="b">
+        <v>0</v>
+      </c>
+      <c r="H95" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
         <v>106</v>
       </c>
@@ -4092,8 +4958,17 @@
       <c r="E96" s="4" t="s">
         <v>566</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F96" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G96" t="b">
+        <v>0</v>
+      </c>
+      <c r="H96" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
         <v>107</v>
       </c>
@@ -4107,8 +4982,17 @@
       <c r="E97" s="4" t="s">
         <v>567</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F97" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G97" t="b">
+        <v>0</v>
+      </c>
+      <c r="H97" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
         <v>236</v>
       </c>
@@ -4122,8 +5006,17 @@
       <c r="E98" s="4" t="s">
         <v>568</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F98" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G98" t="b">
+        <v>0</v>
+      </c>
+      <c r="H98" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A99" s="7" t="s">
         <v>108</v>
       </c>
@@ -4137,8 +5030,17 @@
       <c r="E99" s="4" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F99" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G99" t="b">
+        <v>0</v>
+      </c>
+      <c r="H99" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
         <v>109</v>
       </c>
@@ -4152,8 +5054,17 @@
       <c r="E100" s="4" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F100" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G100" t="b">
+        <v>1</v>
+      </c>
+      <c r="H100" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
         <v>237</v>
       </c>
@@ -4167,8 +5078,17 @@
       <c r="E101" s="4" t="s">
         <v>571</v>
       </c>
-    </row>
-    <row r="102" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F101" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G101" t="b">
+        <v>0</v>
+      </c>
+      <c r="H101" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
         <v>111</v>
       </c>
@@ -4182,8 +5102,17 @@
       <c r="E102" s="4" t="s">
         <v>572</v>
       </c>
-    </row>
-    <row r="103" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F102" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G102" t="b">
+        <v>0</v>
+      </c>
+      <c r="H102" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
         <v>112</v>
       </c>
@@ -4197,8 +5126,17 @@
       <c r="E103" s="4" t="s">
         <v>573</v>
       </c>
-    </row>
-    <row r="104" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F103" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G103" t="b">
+        <v>0</v>
+      </c>
+      <c r="H103" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
         <v>114</v>
       </c>
@@ -4212,8 +5150,17 @@
       <c r="E104" s="4" t="s">
         <v>574</v>
       </c>
-    </row>
-    <row r="105" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F104" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G104" t="b">
+        <v>0</v>
+      </c>
+      <c r="H104" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
         <v>115</v>
       </c>
@@ -4227,8 +5174,17 @@
       <c r="E105" s="4" t="s">
         <v>575</v>
       </c>
-    </row>
-    <row r="106" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F105" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G105" t="b">
+        <v>1</v>
+      </c>
+      <c r="H105" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
         <v>116</v>
       </c>
@@ -4242,8 +5198,17 @@
       <c r="E106" s="4" t="s">
         <v>576</v>
       </c>
-    </row>
-    <row r="107" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F106" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G106" t="b">
+        <v>0</v>
+      </c>
+      <c r="H106" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
         <v>117</v>
       </c>
@@ -4257,8 +5222,17 @@
       <c r="E107" s="4" t="s">
         <v>577</v>
       </c>
-    </row>
-    <row r="108" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F107" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G107" t="b">
+        <v>0</v>
+      </c>
+      <c r="H107" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
         <v>118</v>
       </c>
@@ -4272,8 +5246,17 @@
       <c r="E108" s="4" t="s">
         <v>578</v>
       </c>
-    </row>
-    <row r="109" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F108" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G108" t="b">
+        <v>0</v>
+      </c>
+      <c r="H108" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
         <v>119</v>
       </c>
@@ -4287,8 +5270,17 @@
       <c r="E109" s="4" t="s">
         <v>579</v>
       </c>
-    </row>
-    <row r="110" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F109" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G109" t="b">
+        <v>0</v>
+      </c>
+      <c r="H109" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
         <v>120</v>
       </c>
@@ -4302,8 +5294,17 @@
       <c r="E110" s="4" t="s">
         <v>580</v>
       </c>
-    </row>
-    <row r="111" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F110" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G110" t="b">
+        <v>0</v>
+      </c>
+      <c r="H110" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
         <v>121</v>
       </c>
@@ -4317,8 +5318,17 @@
       <c r="E111" s="4" t="s">
         <v>581</v>
       </c>
-    </row>
-    <row r="112" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F111" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G111" t="b">
+        <v>1</v>
+      </c>
+      <c r="H111" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
         <v>122</v>
       </c>
@@ -4332,8 +5342,17 @@
       <c r="E112" s="4" t="s">
         <v>582</v>
       </c>
-    </row>
-    <row r="113" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F112" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="G112" t="b">
+        <v>0</v>
+      </c>
+      <c r="H112" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A113" s="5" t="s">
         <v>123</v>
       </c>
@@ -4347,8 +5366,17 @@
       <c r="E113" s="4" t="s">
         <v>583</v>
       </c>
-    </row>
-    <row r="114" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F113" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G113" t="b">
+        <v>0</v>
+      </c>
+      <c r="H113" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A114" s="7" t="s">
         <v>124</v>
       </c>
@@ -4362,8 +5390,17 @@
       <c r="E114" s="4" t="s">
         <v>584</v>
       </c>
-    </row>
-    <row r="115" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F114" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G114" t="b">
+        <v>0</v>
+      </c>
+      <c r="H114" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
         <v>125</v>
       </c>
@@ -4377,8 +5414,17 @@
       <c r="E115" s="4" t="s">
         <v>585</v>
       </c>
-    </row>
-    <row r="116" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F115" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G115" t="b">
+        <v>1</v>
+      </c>
+      <c r="H115" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
         <v>127</v>
       </c>
@@ -4392,8 +5438,17 @@
       <c r="E116" s="4" t="s">
         <v>586</v>
       </c>
-    </row>
-    <row r="117" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F116" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G116" t="b">
+        <v>0</v>
+      </c>
+      <c r="H116" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="s">
         <v>128</v>
       </c>
@@ -4407,8 +5462,17 @@
       <c r="E117" s="4" t="s">
         <v>587</v>
       </c>
-    </row>
-    <row r="118" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F117" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G117" t="b">
+        <v>0</v>
+      </c>
+      <c r="H117" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
         <v>238</v>
       </c>
@@ -4422,8 +5486,17 @@
       <c r="E118" s="4" t="s">
         <v>588</v>
       </c>
-    </row>
-    <row r="119" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F118" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G118" t="b">
+        <v>0</v>
+      </c>
+      <c r="H118" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A119" s="5" t="s">
         <v>129</v>
       </c>
@@ -4437,8 +5510,17 @@
       <c r="E119" s="4" t="s">
         <v>589</v>
       </c>
-    </row>
-    <row r="120" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F119" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G119" t="b">
+        <v>0</v>
+      </c>
+      <c r="H119" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A120" s="5" t="s">
         <v>130</v>
       </c>
@@ -4452,8 +5534,17 @@
       <c r="E120" s="4" t="s">
         <v>470</v>
       </c>
-    </row>
-    <row r="121" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F120" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G120" t="b">
+        <v>0</v>
+      </c>
+      <c r="H120" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="s">
         <v>131</v>
       </c>
@@ -4467,8 +5558,17 @@
       <c r="E121" s="4" t="s">
         <v>590</v>
       </c>
-    </row>
-    <row r="122" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F121" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G121" t="b">
+        <v>0</v>
+      </c>
+      <c r="H121" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A122" s="5" t="s">
         <v>132</v>
       </c>
@@ -4482,8 +5582,17 @@
       <c r="E122" s="4" t="s">
         <v>591</v>
       </c>
-    </row>
-    <row r="123" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F122" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G122" t="b">
+        <v>0</v>
+      </c>
+      <c r="H122" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
         <v>133</v>
       </c>
@@ -4497,8 +5606,17 @@
       <c r="E123" s="4" t="s">
         <v>592</v>
       </c>
-    </row>
-    <row r="124" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F123" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G123" t="b">
+        <v>0</v>
+      </c>
+      <c r="H123" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
         <v>134</v>
       </c>
@@ -4512,8 +5630,17 @@
       <c r="E124" s="4" t="s">
         <v>593</v>
       </c>
-    </row>
-    <row r="125" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F124" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G124" t="b">
+        <v>0</v>
+      </c>
+      <c r="H124" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
         <v>135</v>
       </c>
@@ -4527,8 +5654,17 @@
       <c r="E125" s="4" t="s">
         <v>594</v>
       </c>
-    </row>
-    <row r="126" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F125" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G125" t="b">
+        <v>0</v>
+      </c>
+      <c r="H125" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
         <v>136</v>
       </c>
@@ -4542,8 +5678,17 @@
       <c r="E126" s="4" t="s">
         <v>595</v>
       </c>
-    </row>
-    <row r="127" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F126" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G126" t="b">
+        <v>1</v>
+      </c>
+      <c r="H126" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A127" s="5" t="s">
         <v>137</v>
       </c>
@@ -4557,8 +5702,17 @@
       <c r="E127" s="4" t="s">
         <v>596</v>
       </c>
-    </row>
-    <row r="128" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F127" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G127" t="b">
+        <v>0</v>
+      </c>
+      <c r="H127" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A128" s="7" t="s">
         <v>138</v>
       </c>
@@ -4572,8 +5726,17 @@
       <c r="E128" s="4" t="s">
         <v>597</v>
       </c>
-    </row>
-    <row r="129" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F128" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G128" t="b">
+        <v>0</v>
+      </c>
+      <c r="H128" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A129" s="5" t="s">
         <v>139</v>
       </c>
@@ -4587,8 +5750,17 @@
       <c r="E129" s="4" t="s">
         <v>598</v>
       </c>
-    </row>
-    <row r="130" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F129" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G129" t="b">
+        <v>1</v>
+      </c>
+      <c r="H129" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
         <v>140</v>
       </c>
@@ -4602,8 +5774,17 @@
       <c r="E130" s="4" t="s">
         <v>599</v>
       </c>
-    </row>
-    <row r="131" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F130" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G130" t="b">
+        <v>0</v>
+      </c>
+      <c r="H130" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A131" s="5" t="s">
         <v>141</v>
       </c>
@@ -4617,8 +5798,17 @@
       <c r="E131" s="4" t="s">
         <v>600</v>
       </c>
-    </row>
-    <row r="132" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F131" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G131" t="b">
+        <v>0</v>
+      </c>
+      <c r="H131" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A132" s="5" t="s">
         <v>240</v>
       </c>
@@ -4632,8 +5822,17 @@
       <c r="E132" s="4" t="s">
         <v>601</v>
       </c>
-    </row>
-    <row r="133" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F132" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G132" t="b">
+        <v>0</v>
+      </c>
+      <c r="H132" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A133" s="5" t="s">
         <v>142</v>
       </c>
@@ -4647,8 +5846,17 @@
       <c r="E133" s="4" t="s">
         <v>602</v>
       </c>
-    </row>
-    <row r="134" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F133" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G133" t="b">
+        <v>0</v>
+      </c>
+      <c r="H133" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A134" s="5" t="s">
         <v>143</v>
       </c>
@@ -4662,8 +5870,17 @@
       <c r="E134" s="4" t="s">
         <v>603</v>
       </c>
-    </row>
-    <row r="135" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F134" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G134" t="b">
+        <v>0</v>
+      </c>
+      <c r="H134" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A135" s="5" t="s">
         <v>144</v>
       </c>
@@ -4677,8 +5894,17 @@
       <c r="E135" s="4" t="s">
         <v>604</v>
       </c>
-    </row>
-    <row r="136" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F135" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G135" t="b">
+        <v>0</v>
+      </c>
+      <c r="H135" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A136" s="5" t="s">
         <v>145</v>
       </c>
@@ -4692,8 +5918,17 @@
       <c r="E136" s="4" t="s">
         <v>605</v>
       </c>
-    </row>
-    <row r="137" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F136" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G136" t="b">
+        <v>0</v>
+      </c>
+      <c r="H136" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A137" s="5" t="s">
         <v>146</v>
       </c>
@@ -4707,8 +5942,17 @@
       <c r="E137" s="4" t="s">
         <v>606</v>
       </c>
-    </row>
-    <row r="138" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F137" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G137" t="b">
+        <v>0</v>
+      </c>
+      <c r="H137" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A138" s="5" t="s">
         <v>147</v>
       </c>
@@ -4722,8 +5966,17 @@
       <c r="E138" s="4" t="s">
         <v>607</v>
       </c>
-    </row>
-    <row r="139" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F138" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G138" t="b">
+        <v>0</v>
+      </c>
+      <c r="H138" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A139" s="5" t="s">
         <v>148</v>
       </c>
@@ -4737,8 +5990,17 @@
       <c r="E139" s="4" t="s">
         <v>608</v>
       </c>
-    </row>
-    <row r="140" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F139" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G139" t="b">
+        <v>0</v>
+      </c>
+      <c r="H139" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A140" s="5" t="s">
         <v>149</v>
       </c>
@@ -4752,8 +6014,17 @@
       <c r="E140" s="4" t="s">
         <v>609</v>
       </c>
-    </row>
-    <row r="141" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F140" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G140" t="b">
+        <v>1</v>
+      </c>
+      <c r="H140" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A141" s="5" t="s">
         <v>150</v>
       </c>
@@ -4767,8 +6038,17 @@
       <c r="E141" s="4" t="s">
         <v>610</v>
       </c>
-    </row>
-    <row r="142" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F141" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="G141" t="b">
+        <v>0</v>
+      </c>
+      <c r="H141" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A142" s="5" t="s">
         <v>239</v>
       </c>
@@ -4782,8 +6062,17 @@
       <c r="E142" s="4" t="s">
         <v>611</v>
       </c>
-    </row>
-    <row r="143" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F142" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G142" t="b">
+        <v>0</v>
+      </c>
+      <c r="H142" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A143" s="5" t="s">
         <v>151</v>
       </c>
@@ -4797,8 +6086,17 @@
       <c r="E143" s="4" t="s">
         <v>612</v>
       </c>
-    </row>
-    <row r="144" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F143" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G143" t="b">
+        <v>1</v>
+      </c>
+      <c r="H143" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A144" s="5" t="s">
         <v>152</v>
       </c>
@@ -4812,8 +6110,17 @@
       <c r="E144" s="4" t="s">
         <v>613</v>
       </c>
-    </row>
-    <row r="145" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F144" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G144" t="b">
+        <v>0</v>
+      </c>
+      <c r="H144" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A145" s="5" t="s">
         <v>153</v>
       </c>
@@ -4827,8 +6134,17 @@
       <c r="E145" s="4" t="s">
         <v>614</v>
       </c>
-    </row>
-    <row r="146" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F145" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G145" t="b">
+        <v>0</v>
+      </c>
+      <c r="H145" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A146" s="5" t="s">
         <v>154</v>
       </c>
@@ -4842,8 +6158,17 @@
       <c r="E146" s="4" t="s">
         <v>615</v>
       </c>
-    </row>
-    <row r="147" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F146" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G146" t="b">
+        <v>0</v>
+      </c>
+      <c r="H146" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A147" s="5" t="s">
         <v>155</v>
       </c>
@@ -4857,8 +6182,17 @@
       <c r="E147" s="4" t="s">
         <v>616</v>
       </c>
-    </row>
-    <row r="148" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F147" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G147" t="b">
+        <v>0</v>
+      </c>
+      <c r="H147" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A148" s="5" t="s">
         <v>156</v>
       </c>
@@ -4872,8 +6206,17 @@
       <c r="E148" s="4" t="s">
         <v>617</v>
       </c>
-    </row>
-    <row r="149" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F148" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G148" t="b">
+        <v>0</v>
+      </c>
+      <c r="H148" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A149" s="5" t="s">
         <v>157</v>
       </c>
@@ -4887,8 +6230,17 @@
       <c r="E149" s="4" t="s">
         <v>618</v>
       </c>
-    </row>
-    <row r="150" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F149" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G149" t="b">
+        <v>0</v>
+      </c>
+      <c r="H149" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A150" s="5" t="s">
         <v>158</v>
       </c>
@@ -4902,8 +6254,17 @@
       <c r="E150" s="4" t="s">
         <v>619</v>
       </c>
-    </row>
-    <row r="151" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F150" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G150" t="b">
+        <v>0</v>
+      </c>
+      <c r="H150" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A151" s="5" t="s">
         <v>159</v>
       </c>
@@ -4917,8 +6278,17 @@
       <c r="E151" s="4" t="s">
         <v>620</v>
       </c>
-    </row>
-    <row r="152" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F151" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G151" t="b">
+        <v>0</v>
+      </c>
+      <c r="H151" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A152" s="5" t="s">
         <v>160</v>
       </c>
@@ -4932,8 +6302,17 @@
       <c r="E152" s="4" t="s">
         <v>621</v>
       </c>
-    </row>
-    <row r="153" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F152" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G152" t="b">
+        <v>0</v>
+      </c>
+      <c r="H152" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A153" s="5" t="s">
         <v>161</v>
       </c>
@@ -4947,8 +6326,17 @@
       <c r="E153" s="4" t="s">
         <v>622</v>
       </c>
-    </row>
-    <row r="154" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F153" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G153" t="b">
+        <v>0</v>
+      </c>
+      <c r="H153" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A154" s="5" t="s">
         <v>162</v>
       </c>
@@ -4962,8 +6350,17 @@
       <c r="E154" s="4" t="s">
         <v>623</v>
       </c>
-    </row>
-    <row r="155" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F154" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G154" t="b">
+        <v>1</v>
+      </c>
+      <c r="H154" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A155" s="5" t="s">
         <v>163</v>
       </c>
@@ -4977,8 +6374,17 @@
       <c r="E155" s="4" t="s">
         <v>624</v>
       </c>
-    </row>
-    <row r="156" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F155" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G155" t="b">
+        <v>0</v>
+      </c>
+      <c r="H155" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A156" s="7" t="s">
         <v>164</v>
       </c>
@@ -4992,8 +6398,17 @@
       <c r="E156" s="4" t="s">
         <v>625</v>
       </c>
-    </row>
-    <row r="157" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F156" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="G156" t="b">
+        <v>0</v>
+      </c>
+      <c r="H156" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A157" s="5" t="s">
         <v>165</v>
       </c>
@@ -5009,8 +6424,17 @@
       <c r="E157" s="4" t="s">
         <v>626</v>
       </c>
-    </row>
-    <row r="158" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F157" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G157" t="b">
+        <v>1</v>
+      </c>
+      <c r="H157" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A158" s="5" t="s">
         <v>166</v>
       </c>
@@ -5026,8 +6450,17 @@
       <c r="E158" s="4" t="s">
         <v>627</v>
       </c>
-    </row>
-    <row r="159" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F158" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G158" t="b">
+        <v>0</v>
+      </c>
+      <c r="H158" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A159" s="5" t="s">
         <v>167</v>
       </c>
@@ -5043,8 +6476,17 @@
       <c r="E159" s="4" t="s">
         <v>628</v>
       </c>
-    </row>
-    <row r="160" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F159" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G159" t="b">
+        <v>0</v>
+      </c>
+      <c r="H159" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A160" s="5" t="s">
         <v>168</v>
       </c>
@@ -5060,8 +6502,17 @@
       <c r="E160" s="4" t="s">
         <v>471</v>
       </c>
-    </row>
-    <row r="161" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F160" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G160" t="b">
+        <v>0</v>
+      </c>
+      <c r="H160" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A161" s="5" t="s">
         <v>169</v>
       </c>
@@ -5077,8 +6528,17 @@
       <c r="E161" s="4" t="s">
         <v>629</v>
       </c>
-    </row>
-    <row r="162" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F161" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G161" t="b">
+        <v>0</v>
+      </c>
+      <c r="H161" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A162" s="5" t="s">
         <v>170</v>
       </c>
@@ -5094,8 +6554,17 @@
       <c r="E162" s="4" t="s">
         <v>630</v>
       </c>
-    </row>
-    <row r="163" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F162" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G162" t="b">
+        <v>0</v>
+      </c>
+      <c r="H162" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A163" s="5" t="s">
         <v>171</v>
       </c>
@@ -5111,8 +6580,17 @@
       <c r="E163" s="4" t="s">
         <v>631</v>
       </c>
-    </row>
-    <row r="164" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F163" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G163" t="b">
+        <v>0</v>
+      </c>
+      <c r="H163" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A164" s="5" t="s">
         <v>172</v>
       </c>
@@ -5128,8 +6606,17 @@
       <c r="E164" s="4" t="s">
         <v>632</v>
       </c>
-    </row>
-    <row r="165" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F164" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G164" t="b">
+        <v>0</v>
+      </c>
+      <c r="H164" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A165" s="5" t="s">
         <v>241</v>
       </c>
@@ -5145,8 +6632,17 @@
       <c r="E165" s="4" t="s">
         <v>633</v>
       </c>
-    </row>
-    <row r="166" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F165" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G165" t="b">
+        <v>0</v>
+      </c>
+      <c r="H165" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A166" s="5" t="s">
         <v>173</v>
       </c>
@@ -5162,8 +6658,17 @@
       <c r="E166" s="4" t="s">
         <v>634</v>
       </c>
-    </row>
-    <row r="167" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F166" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G166" t="b">
+        <v>0</v>
+      </c>
+      <c r="H166" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A167" s="5" t="s">
         <v>174</v>
       </c>
@@ -5179,8 +6684,17 @@
       <c r="E167" s="4" t="s">
         <v>635</v>
       </c>
-    </row>
-    <row r="168" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F167" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G167" t="b">
+        <v>0</v>
+      </c>
+      <c r="H167" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A168" s="5" t="s">
         <v>175</v>
       </c>
@@ -5196,8 +6710,17 @@
       <c r="E168" s="4" t="s">
         <v>636</v>
       </c>
-    </row>
-    <row r="169" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F168" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G168" t="b">
+        <v>1</v>
+      </c>
+      <c r="H168" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A169" s="5" t="s">
         <v>176</v>
       </c>
@@ -5213,8 +6736,17 @@
       <c r="E169" s="4" t="s">
         <v>637</v>
       </c>
-    </row>
-    <row r="170" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F169" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G169" t="b">
+        <v>0</v>
+      </c>
+      <c r="H169" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A170" s="7" t="s">
         <v>177</v>
       </c>
@@ -5230,8 +6762,17 @@
       <c r="E170" s="4" t="s">
         <v>638</v>
       </c>
-    </row>
-    <row r="171" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F170" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G170" t="b">
+        <v>0</v>
+      </c>
+      <c r="H170" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A171" s="5" t="s">
         <v>178</v>
       </c>
@@ -5245,8 +6786,17 @@
       <c r="E171" s="4" t="s">
         <v>639</v>
       </c>
-    </row>
-    <row r="172" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F171" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G171" t="b">
+        <v>1</v>
+      </c>
+      <c r="H171" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A172" s="5" t="s">
         <v>179</v>
       </c>
@@ -5260,8 +6810,17 @@
       <c r="E172" s="4" t="s">
         <v>640</v>
       </c>
-    </row>
-    <row r="173" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F172" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G172" t="b">
+        <v>0</v>
+      </c>
+      <c r="H172" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A173" s="5" t="s">
         <v>180</v>
       </c>
@@ -5275,8 +6834,17 @@
       <c r="E173" s="4" t="s">
         <v>641</v>
       </c>
-    </row>
-    <row r="174" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F173" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G173" t="b">
+        <v>0</v>
+      </c>
+      <c r="H173" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A174" s="5" t="s">
         <v>181</v>
       </c>
@@ -5290,8 +6858,17 @@
       <c r="E174" s="4" t="s">
         <v>642</v>
       </c>
-    </row>
-    <row r="175" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F174" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G174" t="b">
+        <v>0</v>
+      </c>
+      <c r="H174" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A175" s="5" t="s">
         <v>182</v>
       </c>
@@ -5305,8 +6882,17 @@
       <c r="E175" s="4" t="s">
         <v>643</v>
       </c>
-    </row>
-    <row r="176" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F175" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="G175" t="b">
+        <v>0</v>
+      </c>
+      <c r="H175" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A176" s="5" t="s">
         <v>183</v>
       </c>
@@ -5320,8 +6906,17 @@
       <c r="E176" s="4" t="s">
         <v>644</v>
       </c>
-    </row>
-    <row r="177" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F176" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G176" t="b">
+        <v>0</v>
+      </c>
+      <c r="H176" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A177" s="5" t="s">
         <v>184</v>
       </c>
@@ -5335,8 +6930,17 @@
       <c r="E177" s="4" t="s">
         <v>645</v>
       </c>
-    </row>
-    <row r="178" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F177" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G177" t="b">
+        <v>0</v>
+      </c>
+      <c r="H177" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A178" s="5" t="s">
         <v>185</v>
       </c>
@@ -5350,8 +6954,17 @@
       <c r="E178" s="4" t="s">
         <v>646</v>
       </c>
-    </row>
-    <row r="179" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F178" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G178" t="b">
+        <v>0</v>
+      </c>
+      <c r="H178" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A179" s="5" t="s">
         <v>186</v>
       </c>
@@ -5365,8 +6978,17 @@
       <c r="E179" s="4" t="s">
         <v>647</v>
       </c>
-    </row>
-    <row r="180" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F179" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G179" t="b">
+        <v>0</v>
+      </c>
+      <c r="H179" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A180" s="5" t="s">
         <v>187</v>
       </c>
@@ -5380,8 +7002,17 @@
       <c r="E180" s="4" t="s">
         <v>648</v>
       </c>
-    </row>
-    <row r="181" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F180" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G180" t="b">
+        <v>0</v>
+      </c>
+      <c r="H180" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A181" s="5" t="s">
         <v>188</v>
       </c>
@@ -5395,8 +7026,17 @@
       <c r="E181" s="4" t="s">
         <v>649</v>
       </c>
-    </row>
-    <row r="182" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F181" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G181" t="b">
+        <v>0</v>
+      </c>
+      <c r="H181" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A182" s="5" t="s">
         <v>189</v>
       </c>
@@ -5410,8 +7050,17 @@
       <c r="E182" s="4" t="s">
         <v>650</v>
       </c>
-    </row>
-    <row r="183" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F182" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G182" t="b">
+        <v>1</v>
+      </c>
+      <c r="H182" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A183" s="5" t="s">
         <v>190</v>
       </c>
@@ -5425,8 +7074,17 @@
       <c r="E183" s="4" t="s">
         <v>651</v>
       </c>
-    </row>
-    <row r="184" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F183" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G183" t="b">
+        <v>0</v>
+      </c>
+      <c r="H183" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A184" s="7" t="s">
         <v>191</v>
       </c>
@@ -5440,8 +7098,17 @@
       <c r="E184" s="4" t="s">
         <v>652</v>
       </c>
-    </row>
-    <row r="185" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F184" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G184" t="b">
+        <v>0</v>
+      </c>
+      <c r="H184" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A185" s="5" t="s">
         <v>192</v>
       </c>
@@ -5457,8 +7124,17 @@
       <c r="E185" s="4" t="s">
         <v>653</v>
       </c>
-    </row>
-    <row r="186" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F185" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G185" t="b">
+        <v>1</v>
+      </c>
+      <c r="H185" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A186" s="5" t="s">
         <v>193</v>
       </c>
@@ -5474,8 +7150,17 @@
       <c r="E186" s="4" t="s">
         <v>654</v>
       </c>
-    </row>
-    <row r="187" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F186" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G186" t="b">
+        <v>0</v>
+      </c>
+      <c r="H186" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A187" s="5" t="s">
         <v>194</v>
       </c>
@@ -5491,8 +7176,17 @@
       <c r="E187" s="4" t="s">
         <v>655</v>
       </c>
-    </row>
-    <row r="188" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F187" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G187" t="b">
+        <v>0</v>
+      </c>
+      <c r="H187" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A188" s="5" t="s">
         <v>195</v>
       </c>
@@ -5508,8 +7202,17 @@
       <c r="E188" s="4" t="s">
         <v>656</v>
       </c>
-    </row>
-    <row r="189" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F188" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G188" t="b">
+        <v>0</v>
+      </c>
+      <c r="H188" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="189" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A189" s="5" t="s">
         <v>196</v>
       </c>
@@ -5525,8 +7228,17 @@
       <c r="E189" s="4" t="s">
         <v>657</v>
       </c>
-    </row>
-    <row r="190" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F189" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G189" t="b">
+        <v>0</v>
+      </c>
+      <c r="H189" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A190" s="5" t="s">
         <v>197</v>
       </c>
@@ -5542,8 +7254,17 @@
       <c r="E190" s="4" t="s">
         <v>658</v>
       </c>
-    </row>
-    <row r="191" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F190" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G190" t="b">
+        <v>0</v>
+      </c>
+      <c r="H190" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A191" s="5" t="s">
         <v>198</v>
       </c>
@@ -5559,8 +7280,17 @@
       <c r="E191" s="4" t="s">
         <v>659</v>
       </c>
-    </row>
-    <row r="192" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F191" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G191" t="b">
+        <v>0</v>
+      </c>
+      <c r="H191" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A192" s="5" t="s">
         <v>199</v>
       </c>
@@ -5576,8 +7306,17 @@
       <c r="E192" s="4" t="s">
         <v>660</v>
       </c>
-    </row>
-    <row r="193" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F192" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G192" t="b">
+        <v>0</v>
+      </c>
+      <c r="H192" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A193" s="5" t="s">
         <v>200</v>
       </c>
@@ -5593,8 +7332,17 @@
       <c r="E193" s="4" t="s">
         <v>661</v>
       </c>
-    </row>
-    <row r="194" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F193" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G193" t="b">
+        <v>0</v>
+      </c>
+      <c r="H193" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A194" s="5" t="s">
         <v>201</v>
       </c>
@@ -5610,8 +7358,17 @@
       <c r="E194" s="4" t="s">
         <v>662</v>
       </c>
-    </row>
-    <row r="195" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F194" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G194" t="b">
+        <v>0</v>
+      </c>
+      <c r="H194" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A195" s="5" t="s">
         <v>202</v>
       </c>
@@ -5627,8 +7384,17 @@
       <c r="E195" s="4" t="s">
         <v>663</v>
       </c>
-    </row>
-    <row r="196" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F195" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G195" t="b">
+        <v>0</v>
+      </c>
+      <c r="H195" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A196" s="5" t="s">
         <v>203</v>
       </c>
@@ -5644,8 +7410,17 @@
       <c r="E196" s="4" t="s">
         <v>664</v>
       </c>
-    </row>
-    <row r="197" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F196" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G196" t="b">
+        <v>1</v>
+      </c>
+      <c r="H196" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A197" s="5" t="s">
         <v>204</v>
       </c>
@@ -5661,8 +7436,17 @@
       <c r="E197" s="4" t="s">
         <v>665</v>
       </c>
-    </row>
-    <row r="198" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F197" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G197" t="b">
+        <v>0</v>
+      </c>
+      <c r="H197" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A198" s="7" t="s">
         <v>205</v>
       </c>
@@ -5678,8 +7462,17 @@
       <c r="E198" s="4" t="s">
         <v>666</v>
       </c>
-    </row>
-    <row r="199" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F198" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G198" t="b">
+        <v>0</v>
+      </c>
+      <c r="H198" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A199" s="5" t="s">
         <v>206</v>
       </c>
@@ -5695,8 +7488,17 @@
       <c r="E199" s="4" t="s">
         <v>667</v>
       </c>
-    </row>
-    <row r="200" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F199" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G199" t="b">
+        <v>1</v>
+      </c>
+      <c r="H199" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A200" s="5" t="s">
         <v>207</v>
       </c>
@@ -5712,8 +7514,17 @@
       <c r="E200" s="4" t="s">
         <v>472</v>
       </c>
-    </row>
-    <row r="201" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F200" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G200" t="b">
+        <v>0</v>
+      </c>
+      <c r="H200" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A201" s="5" t="s">
         <v>208</v>
       </c>
@@ -5729,8 +7540,17 @@
       <c r="E201" s="4" t="s">
         <v>668</v>
       </c>
-    </row>
-    <row r="202" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F201" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G201" t="b">
+        <v>0</v>
+      </c>
+      <c r="H201" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A202" s="5" t="s">
         <v>209</v>
       </c>
@@ -5746,8 +7566,17 @@
       <c r="E202" s="4" t="s">
         <v>669</v>
       </c>
-    </row>
-    <row r="203" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F202" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G202" t="b">
+        <v>0</v>
+      </c>
+      <c r="H202" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="203" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A203" s="5" t="s">
         <v>210</v>
       </c>
@@ -5763,8 +7592,17 @@
       <c r="E203" s="4" t="s">
         <v>670</v>
       </c>
-    </row>
-    <row r="204" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F203" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G203" t="b">
+        <v>0</v>
+      </c>
+      <c r="H203" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="204" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A204" s="5" t="s">
         <v>211</v>
       </c>
@@ -5780,8 +7618,17 @@
       <c r="E204" s="4" t="s">
         <v>671</v>
       </c>
-    </row>
-    <row r="205" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F204" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G204" t="b">
+        <v>0</v>
+      </c>
+      <c r="H204" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A205" s="5" t="s">
         <v>212</v>
       </c>
@@ -5797,8 +7644,17 @@
       <c r="E205" s="4" t="s">
         <v>672</v>
       </c>
-    </row>
-    <row r="206" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F205" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G205" t="b">
+        <v>0</v>
+      </c>
+      <c r="H205" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A206" s="5" t="s">
         <v>213</v>
       </c>
@@ -5814,8 +7670,17 @@
       <c r="E206" s="4" t="s">
         <v>673</v>
       </c>
-    </row>
-    <row r="207" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F206" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G206" t="b">
+        <v>0</v>
+      </c>
+      <c r="H206" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="207" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A207" s="5" t="s">
         <v>214</v>
       </c>
@@ -5831,8 +7696,17 @@
       <c r="E207" s="4" t="s">
         <v>674</v>
       </c>
-    </row>
-    <row r="208" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F207" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G207" t="b">
+        <v>0</v>
+      </c>
+      <c r="H207" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A208" s="5" t="s">
         <v>215</v>
       </c>
@@ -5848,8 +7722,17 @@
       <c r="E208" s="4" t="s">
         <v>675</v>
       </c>
-    </row>
-    <row r="209" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F208" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G208" t="b">
+        <v>0</v>
+      </c>
+      <c r="H208" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A209" s="5" t="s">
         <v>216</v>
       </c>
@@ -5865,8 +7748,17 @@
       <c r="E209" s="4" t="s">
         <v>676</v>
       </c>
-    </row>
-    <row r="210" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F209" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G209" t="b">
+        <v>0</v>
+      </c>
+      <c r="H209" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="210" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A210" s="5" t="s">
         <v>217</v>
       </c>
@@ -5882,8 +7774,17 @@
       <c r="E210" s="4" t="s">
         <v>677</v>
       </c>
-    </row>
-    <row r="211" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F210" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G210" t="b">
+        <v>1</v>
+      </c>
+      <c r="H210" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="211" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A211" s="5" t="s">
         <v>218</v>
       </c>
@@ -5899,8 +7800,17 @@
       <c r="E211" s="4" t="s">
         <v>678</v>
       </c>
-    </row>
-    <row r="212" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F211" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G211" t="b">
+        <v>0</v>
+      </c>
+      <c r="H211" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="212" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A212" s="7" t="s">
         <v>219</v>
       </c>
@@ -5916,8 +7826,17 @@
       <c r="E212" s="4" t="s">
         <v>679</v>
       </c>
-    </row>
-    <row r="213" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F212" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G212" t="b">
+        <v>0</v>
+      </c>
+      <c r="H212" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="213" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A213" s="5" t="s">
         <v>220</v>
       </c>
@@ -5933,8 +7852,17 @@
       <c r="E213" s="4" t="s">
         <v>680</v>
       </c>
-    </row>
-    <row r="214" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F213" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G213" t="b">
+        <v>1</v>
+      </c>
+      <c r="H213" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="214" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A214" s="5" t="s">
         <v>221</v>
       </c>
@@ -5950,8 +7878,17 @@
       <c r="E214" s="4" t="s">
         <v>681</v>
       </c>
-    </row>
-    <row r="215" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F214" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G214" t="b">
+        <v>0</v>
+      </c>
+      <c r="H214" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="215" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A215" s="5" t="s">
         <v>222</v>
       </c>
@@ -5967,8 +7904,17 @@
       <c r="E215" s="4" t="s">
         <v>682</v>
       </c>
-    </row>
-    <row r="216" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F215" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="G215" t="b">
+        <v>0</v>
+      </c>
+      <c r="H215" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="216" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A216" s="5" t="s">
         <v>223</v>
       </c>
@@ -5984,8 +7930,17 @@
       <c r="E216" s="4" t="s">
         <v>683</v>
       </c>
-    </row>
-    <row r="217" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F216" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G216" t="b">
+        <v>0</v>
+      </c>
+      <c r="H216" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="217" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A217" s="5" t="s">
         <v>224</v>
       </c>
@@ -6001,8 +7956,17 @@
       <c r="E217" s="4" t="s">
         <v>684</v>
       </c>
-    </row>
-    <row r="218" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F217" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G217" t="b">
+        <v>0</v>
+      </c>
+      <c r="H217" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="218" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A218" s="5" t="s">
         <v>225</v>
       </c>
@@ -6018,8 +7982,17 @@
       <c r="E218" s="4" t="s">
         <v>685</v>
       </c>
-    </row>
-    <row r="219" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F218" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G218" t="b">
+        <v>0</v>
+      </c>
+      <c r="H218" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="219" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A219" s="5" t="s">
         <v>226</v>
       </c>
@@ -6035,8 +8008,17 @@
       <c r="E219" s="4" t="s">
         <v>686</v>
       </c>
-    </row>
-    <row r="220" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F219" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G219" t="b">
+        <v>0</v>
+      </c>
+      <c r="H219" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="220" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A220" s="5" t="s">
         <v>227</v>
       </c>
@@ -6052,8 +8034,17 @@
       <c r="E220" s="4" t="s">
         <v>687</v>
       </c>
-    </row>
-    <row r="221" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F220" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G220" t="b">
+        <v>0</v>
+      </c>
+      <c r="H220" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="221" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A221" s="5" t="s">
         <v>228</v>
       </c>
@@ -6069,8 +8060,17 @@
       <c r="E221" s="11" t="s">
         <v>688</v>
       </c>
-    </row>
-    <row r="222" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F221" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G221" t="b">
+        <v>0</v>
+      </c>
+      <c r="H221" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="222" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A222" s="5" t="s">
         <v>229</v>
       </c>
@@ -6086,8 +8086,17 @@
       <c r="E222" s="4" t="s">
         <v>689</v>
       </c>
-    </row>
-    <row r="223" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F222" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G222" t="b">
+        <v>0</v>
+      </c>
+      <c r="H222" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="223" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A223" s="5" t="s">
         <v>230</v>
       </c>
@@ -6103,8 +8112,17 @@
       <c r="E223" s="4" t="s">
         <v>690</v>
       </c>
-    </row>
-    <row r="224" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F223" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G223" t="b">
+        <v>0</v>
+      </c>
+      <c r="H223" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="224" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A224" s="5" t="s">
         <v>231</v>
       </c>
@@ -6120,8 +8138,17 @@
       <c r="E224" s="4" t="s">
         <v>691</v>
       </c>
-    </row>
-    <row r="225" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F224" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G224" t="b">
+        <v>1</v>
+      </c>
+      <c r="H224" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="225" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A225" s="5" t="s">
         <v>232</v>
       </c>
@@ -6137,8 +8164,17 @@
       <c r="E225" s="4" t="s">
         <v>692</v>
       </c>
-    </row>
-    <row r="226" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F225" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G225" t="b">
+        <v>0</v>
+      </c>
+      <c r="H225" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="226" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A226" s="7" t="s">
         <v>233</v>
       </c>
@@ -6153,6 +8189,15 @@
       </c>
       <c r="E226" s="4" t="s">
         <v>693</v>
+      </c>
+      <c r="F226" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G226" t="b">
+        <v>0</v>
+      </c>
+      <c r="H226" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated auth, fixed noAuth view, added mock data for challenges
</commit_message>
<xml_diff>
--- a/models/mock-data/FakeUsers.xlsx
+++ b/models/mock-data/FakeUsers.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-4600" windowWidth="15120" windowHeight="26740" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="11560" windowHeight="15940" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2537,8 +2537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H226"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A184" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H226"/>
+    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="F152" sqref="F152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6279,7 +6279,7 @@
         <v>620</v>
       </c>
       <c r="F151" s="12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G151" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Added password to mock data
</commit_message>
<xml_diff>
--- a/models/mock-data/FakeUsers.xlsx
+++ b/models/mock-data/FakeUsers.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-4600" windowWidth="15120" windowHeight="26740" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1020" uniqueCount="697">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1246" uniqueCount="698">
   <si>
     <t>Spot</t>
   </si>
@@ -2115,6 +2115,9 @@
   </si>
   <si>
     <t>Admin</t>
+  </si>
+  <si>
+    <t>Password</t>
   </si>
 </sst>
 </file>
@@ -2251,7 +2254,27 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2535,10 +2558,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H226"/>
+  <dimension ref="A1:I226"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A184" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H226"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2548,9 +2571,10 @@
     <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2575,8 +2599,11 @@
       <c r="H1" s="1" t="s">
         <v>696</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I1" s="1" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -2601,8 +2628,11 @@
       <c r="H2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I2" s="4" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
@@ -2627,8 +2657,11 @@
       <c r="H3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I3" s="4" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
@@ -2653,8 +2686,11 @@
       <c r="H4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I4" s="4" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
@@ -2679,8 +2715,11 @@
       <c r="H5" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I5" s="4" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>473</v>
       </c>
@@ -2705,8 +2744,11 @@
       <c r="H6" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I6" s="4" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>11</v>
       </c>
@@ -2731,8 +2773,11 @@
       <c r="H7" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I7" s="4" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>12</v>
       </c>
@@ -2757,8 +2802,11 @@
       <c r="H8" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I8" s="4" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>13</v>
       </c>
@@ -2783,8 +2831,11 @@
       <c r="H9" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I9" s="4" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>14</v>
       </c>
@@ -2809,8 +2860,11 @@
       <c r="H10" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I10" s="4" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>15</v>
       </c>
@@ -2835,8 +2889,11 @@
       <c r="H11" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I11" s="4" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>16</v>
       </c>
@@ -2861,8 +2918,11 @@
       <c r="H12" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I12" s="4" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>17</v>
       </c>
@@ -2887,8 +2947,11 @@
       <c r="H13" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I13" s="4" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>18</v>
       </c>
@@ -2913,8 +2976,11 @@
       <c r="H14" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I14" s="4" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>19</v>
       </c>
@@ -2939,8 +3005,11 @@
       <c r="H15" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I15" s="4" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>20</v>
       </c>
@@ -2965,8 +3034,11 @@
       <c r="H16" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I16" s="4" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>22</v>
       </c>
@@ -2991,8 +3063,11 @@
       <c r="H17" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I17" s="4" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>24</v>
       </c>
@@ -3017,8 +3092,11 @@
       <c r="H18" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I18" s="4" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>25</v>
       </c>
@@ -3043,8 +3121,11 @@
       <c r="H19" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I19" s="4" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>26</v>
       </c>
@@ -3069,8 +3150,11 @@
       <c r="H20" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I20" s="4" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>27</v>
       </c>
@@ -3095,8 +3179,11 @@
       <c r="H21" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I21" s="4" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>28</v>
       </c>
@@ -3121,8 +3208,11 @@
       <c r="H22" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I22" s="4" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>29</v>
       </c>
@@ -3147,8 +3237,11 @@
       <c r="H23" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I23" s="4" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>30</v>
       </c>
@@ -3173,8 +3266,11 @@
       <c r="H24" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I24" s="4" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>31</v>
       </c>
@@ -3199,8 +3295,11 @@
       <c r="H25" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I25" s="4" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>32</v>
       </c>
@@ -3225,8 +3324,11 @@
       <c r="H26" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I26" s="4" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>33</v>
       </c>
@@ -3251,8 +3353,11 @@
       <c r="H27" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I27" s="4" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>34</v>
       </c>
@@ -3277,8 +3382,11 @@
       <c r="H28" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I28" s="4" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>35</v>
       </c>
@@ -3303,8 +3411,11 @@
       <c r="H29" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I29" s="4" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>36</v>
       </c>
@@ -3329,8 +3440,11 @@
       <c r="H30" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I30" s="4" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>38</v>
       </c>
@@ -3355,8 +3469,11 @@
       <c r="H31" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I31" s="4" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>39</v>
       </c>
@@ -3381,8 +3498,11 @@
       <c r="H32" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I32" s="4" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>40</v>
       </c>
@@ -3407,8 +3527,11 @@
       <c r="H33" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I33" s="4" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>41</v>
       </c>
@@ -3433,8 +3556,11 @@
       <c r="H34" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I34" s="4" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>42</v>
       </c>
@@ -3459,8 +3585,11 @@
       <c r="H35" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I35" s="4" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>43</v>
       </c>
@@ -3485,8 +3614,11 @@
       <c r="H36" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I36" s="4" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>44</v>
       </c>
@@ -3511,8 +3643,11 @@
       <c r="H37" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I37" s="4" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>45</v>
       </c>
@@ -3537,8 +3672,11 @@
       <c r="H38" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I38" s="4" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>46</v>
       </c>
@@ -3563,8 +3701,11 @@
       <c r="H39" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I39" s="4" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>47</v>
       </c>
@@ -3589,8 +3730,11 @@
       <c r="H40" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I40" s="4" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
         <v>48</v>
       </c>
@@ -3615,8 +3759,11 @@
       <c r="H41" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I41" s="4" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>49</v>
       </c>
@@ -3641,8 +3788,11 @@
       <c r="H42" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I42" s="4" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
         <v>50</v>
       </c>
@@ -3667,8 +3817,11 @@
       <c r="H43" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I43" s="4" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>51</v>
       </c>
@@ -3691,8 +3844,11 @@
       <c r="H44" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I44" s="4" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
         <v>53</v>
       </c>
@@ -3715,8 +3871,11 @@
       <c r="H45" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I45" s="4" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
         <v>54</v>
       </c>
@@ -3739,8 +3898,11 @@
       <c r="H46" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I46" s="4" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>55</v>
       </c>
@@ -3763,8 +3925,11 @@
       <c r="H47" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I47" s="4" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>56</v>
       </c>
@@ -3787,8 +3952,11 @@
       <c r="H48" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I48" s="4" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
         <v>57</v>
       </c>
@@ -3811,8 +3979,11 @@
       <c r="H49" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I49" s="4" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
         <v>58</v>
       </c>
@@ -3835,8 +4006,11 @@
       <c r="H50" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I50" s="4" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
         <v>59</v>
       </c>
@@ -3859,8 +4033,11 @@
       <c r="H51" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I51" s="4" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
         <v>60</v>
       </c>
@@ -3883,8 +4060,11 @@
       <c r="H52" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I52" s="4" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
         <v>61</v>
       </c>
@@ -3907,8 +4087,11 @@
       <c r="H53" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I53" s="4" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
         <v>62</v>
       </c>
@@ -3931,8 +4114,11 @@
       <c r="H54" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I54" s="4" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
         <v>63</v>
       </c>
@@ -3955,8 +4141,11 @@
       <c r="H55" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I55" s="4" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
         <v>64</v>
       </c>
@@ -3979,8 +4168,11 @@
       <c r="H56" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I56" s="4" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
         <v>65</v>
       </c>
@@ -4003,8 +4195,11 @@
       <c r="H57" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I57" s="4" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
         <v>66</v>
       </c>
@@ -4029,8 +4224,11 @@
       <c r="H58" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I58" s="4" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
         <v>69</v>
       </c>
@@ -4055,8 +4253,11 @@
       <c r="H59" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I59" s="4" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
         <v>70</v>
       </c>
@@ -4081,8 +4282,11 @@
       <c r="H60" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I60" s="4" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
         <v>71</v>
       </c>
@@ -4107,8 +4311,11 @@
       <c r="H61" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I61" s="4" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
         <v>72</v>
       </c>
@@ -4133,8 +4340,11 @@
       <c r="H62" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I62" s="4" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
         <v>73</v>
       </c>
@@ -4159,8 +4369,11 @@
       <c r="H63" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I63" s="4" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
         <v>234</v>
       </c>
@@ -4185,8 +4398,11 @@
       <c r="H64" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I64" s="4" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
         <v>74</v>
       </c>
@@ -4211,8 +4427,11 @@
       <c r="H65" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I65" s="4" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
         <v>75</v>
       </c>
@@ -4237,8 +4456,11 @@
       <c r="H66" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I66" s="4" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
         <v>76</v>
       </c>
@@ -4263,8 +4485,11 @@
       <c r="H67" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I67" s="4" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
         <v>77</v>
       </c>
@@ -4289,8 +4514,11 @@
       <c r="H68" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I68" s="4" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
         <v>78</v>
       </c>
@@ -4315,8 +4543,11 @@
       <c r="H69" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I69" s="4" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
         <v>79</v>
       </c>
@@ -4341,8 +4572,11 @@
       <c r="H70" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I70" s="4" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
         <v>80</v>
       </c>
@@ -4367,8 +4601,11 @@
       <c r="H71" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I71" s="4" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
         <v>235</v>
       </c>
@@ -4391,8 +4628,11 @@
       <c r="H72" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I72" s="4" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
         <v>81</v>
       </c>
@@ -4415,8 +4655,11 @@
       <c r="H73" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="74" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I73" s="4" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
         <v>83</v>
       </c>
@@ -4439,8 +4682,11 @@
       <c r="H74" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I74" s="4" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
         <v>84</v>
       </c>
@@ -4463,8 +4709,11 @@
       <c r="H75" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I75" s="4" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
         <v>85</v>
       </c>
@@ -4487,8 +4736,11 @@
       <c r="H76" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I76" s="4" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
         <v>86</v>
       </c>
@@ -4511,8 +4763,11 @@
       <c r="H77" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="78" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I77" s="4" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
         <v>87</v>
       </c>
@@ -4535,8 +4790,11 @@
       <c r="H78" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="79" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I78" s="4" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
         <v>88</v>
       </c>
@@ -4559,8 +4817,11 @@
       <c r="H79" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="80" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I79" s="4" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
         <v>89</v>
       </c>
@@ -4583,8 +4844,11 @@
       <c r="H80" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="81" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I80" s="4" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
         <v>90</v>
       </c>
@@ -4607,8 +4871,11 @@
       <c r="H81" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="82" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I81" s="4" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
         <v>91</v>
       </c>
@@ -4631,8 +4898,11 @@
       <c r="H82" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="83" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I82" s="4" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
         <v>92</v>
       </c>
@@ -4655,8 +4925,11 @@
       <c r="H83" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="84" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I83" s="4" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
         <v>93</v>
       </c>
@@ -4679,8 +4952,11 @@
       <c r="H84" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="85" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I84" s="4" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A85" s="7" t="s">
         <v>94</v>
       </c>
@@ -4703,8 +4979,11 @@
       <c r="H85" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="86" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I85" s="4" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
         <v>95</v>
       </c>
@@ -4727,8 +5006,11 @@
       <c r="H86" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="87" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I86" s="4" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
         <v>97</v>
       </c>
@@ -4751,8 +5033,11 @@
       <c r="H87" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="88" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I87" s="4" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
         <v>98</v>
       </c>
@@ -4775,8 +5060,11 @@
       <c r="H88" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="89" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I88" s="4" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
         <v>99</v>
       </c>
@@ -4799,8 +5087,11 @@
       <c r="H89" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="90" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I89" s="4" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
         <v>100</v>
       </c>
@@ -4823,8 +5114,11 @@
       <c r="H90" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="91" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I90" s="4" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
         <v>101</v>
       </c>
@@ -4847,8 +5141,11 @@
       <c r="H91" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="92" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I91" s="4" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
         <v>102</v>
       </c>
@@ -4871,8 +5168,11 @@
       <c r="H92" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="93" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I92" s="4" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
         <v>103</v>
       </c>
@@ -4895,8 +5195,11 @@
       <c r="H93" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="94" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I93" s="4" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
         <v>104</v>
       </c>
@@ -4919,8 +5222,11 @@
       <c r="H94" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="95" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I94" s="4" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
         <v>105</v>
       </c>
@@ -4943,8 +5249,11 @@
       <c r="H95" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="96" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I95" s="4" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
         <v>106</v>
       </c>
@@ -4967,8 +5276,11 @@
       <c r="H96" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="97" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I96" s="4" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
         <v>107</v>
       </c>
@@ -4991,8 +5303,11 @@
       <c r="H97" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="98" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I97" s="4" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
         <v>236</v>
       </c>
@@ -5015,8 +5330,11 @@
       <c r="H98" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="99" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I98" s="4" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A99" s="7" t="s">
         <v>108</v>
       </c>
@@ -5039,8 +5357,11 @@
       <c r="H99" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="100" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I99" s="4" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
         <v>109</v>
       </c>
@@ -5063,8 +5384,11 @@
       <c r="H100" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="101" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I100" s="4" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
         <v>237</v>
       </c>
@@ -5087,8 +5411,11 @@
       <c r="H101" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="102" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I101" s="4" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
         <v>111</v>
       </c>
@@ -5111,8 +5438,11 @@
       <c r="H102" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="103" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I102" s="4" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
         <v>112</v>
       </c>
@@ -5135,8 +5465,11 @@
       <c r="H103" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="104" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I103" s="4" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
         <v>114</v>
       </c>
@@ -5159,8 +5492,11 @@
       <c r="H104" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="105" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I104" s="4" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
         <v>115</v>
       </c>
@@ -5183,8 +5519,11 @@
       <c r="H105" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="106" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I105" s="4" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
         <v>116</v>
       </c>
@@ -5207,8 +5546,11 @@
       <c r="H106" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="107" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I106" s="4" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
         <v>117</v>
       </c>
@@ -5231,8 +5573,11 @@
       <c r="H107" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="108" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I107" s="4" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
         <v>118</v>
       </c>
@@ -5255,8 +5600,11 @@
       <c r="H108" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="109" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I108" s="4" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
         <v>119</v>
       </c>
@@ -5279,8 +5627,11 @@
       <c r="H109" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="110" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I109" s="4" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
         <v>120</v>
       </c>
@@ -5303,8 +5654,11 @@
       <c r="H110" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="111" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I110" s="4" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
         <v>121</v>
       </c>
@@ -5327,8 +5681,11 @@
       <c r="H111" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="112" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I111" s="4" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
         <v>122</v>
       </c>
@@ -5351,8 +5708,11 @@
       <c r="H112" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="113" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I112" s="4" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A113" s="5" t="s">
         <v>123</v>
       </c>
@@ -5375,8 +5735,11 @@
       <c r="H113" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="114" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I113" s="4" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A114" s="7" t="s">
         <v>124</v>
       </c>
@@ -5399,8 +5762,11 @@
       <c r="H114" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="115" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I114" s="4" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
         <v>125</v>
       </c>
@@ -5423,8 +5789,11 @@
       <c r="H115" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="116" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I115" s="4" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
         <v>127</v>
       </c>
@@ -5447,8 +5816,11 @@
       <c r="H116" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="117" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I116" s="4" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="s">
         <v>128</v>
       </c>
@@ -5471,8 +5843,11 @@
       <c r="H117" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="118" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I117" s="4" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
         <v>238</v>
       </c>
@@ -5495,8 +5870,11 @@
       <c r="H118" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="119" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I118" s="4" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A119" s="5" t="s">
         <v>129</v>
       </c>
@@ -5519,8 +5897,11 @@
       <c r="H119" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="120" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I119" s="4" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A120" s="5" t="s">
         <v>130</v>
       </c>
@@ -5543,8 +5924,11 @@
       <c r="H120" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="121" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I120" s="4" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="s">
         <v>131</v>
       </c>
@@ -5567,8 +5951,11 @@
       <c r="H121" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="122" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I121" s="4" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A122" s="5" t="s">
         <v>132</v>
       </c>
@@ -5591,8 +5978,11 @@
       <c r="H122" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="123" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I122" s="4" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
         <v>133</v>
       </c>
@@ -5615,8 +6005,11 @@
       <c r="H123" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="124" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I123" s="4" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
         <v>134</v>
       </c>
@@ -5639,8 +6032,11 @@
       <c r="H124" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="125" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I124" s="4" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
         <v>135</v>
       </c>
@@ -5663,8 +6059,11 @@
       <c r="H125" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="126" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I125" s="4" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
         <v>136</v>
       </c>
@@ -5687,8 +6086,11 @@
       <c r="H126" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="127" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I126" s="4" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A127" s="5" t="s">
         <v>137</v>
       </c>
@@ -5711,8 +6113,11 @@
       <c r="H127" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="128" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I127" s="4" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A128" s="7" t="s">
         <v>138</v>
       </c>
@@ -5735,8 +6140,11 @@
       <c r="H128" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="129" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I128" s="4" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A129" s="5" t="s">
         <v>139</v>
       </c>
@@ -5759,8 +6167,11 @@
       <c r="H129" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="130" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I129" s="4" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
         <v>140</v>
       </c>
@@ -5783,8 +6194,11 @@
       <c r="H130" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="131" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I130" s="4" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A131" s="5" t="s">
         <v>141</v>
       </c>
@@ -5807,8 +6221,11 @@
       <c r="H131" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="132" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I131" s="4" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A132" s="5" t="s">
         <v>240</v>
       </c>
@@ -5831,8 +6248,11 @@
       <c r="H132" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="133" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I132" s="4" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A133" s="5" t="s">
         <v>142</v>
       </c>
@@ -5855,8 +6275,11 @@
       <c r="H133" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="134" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I133" s="4" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A134" s="5" t="s">
         <v>143</v>
       </c>
@@ -5879,8 +6302,11 @@
       <c r="H134" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="135" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I134" s="4" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A135" s="5" t="s">
         <v>144</v>
       </c>
@@ -5903,8 +6329,11 @@
       <c r="H135" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="136" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I135" s="4" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A136" s="5" t="s">
         <v>145</v>
       </c>
@@ -5927,8 +6356,11 @@
       <c r="H136" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="137" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I136" s="4" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A137" s="5" t="s">
         <v>146</v>
       </c>
@@ -5951,8 +6383,11 @@
       <c r="H137" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="138" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I137" s="4" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A138" s="5" t="s">
         <v>147</v>
       </c>
@@ -5975,8 +6410,11 @@
       <c r="H138" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="139" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I138" s="4" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A139" s="5" t="s">
         <v>148</v>
       </c>
@@ -5999,8 +6437,11 @@
       <c r="H139" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="140" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I139" s="4" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A140" s="5" t="s">
         <v>149</v>
       </c>
@@ -6023,8 +6464,11 @@
       <c r="H140" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="141" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I140" s="4" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A141" s="5" t="s">
         <v>150</v>
       </c>
@@ -6047,8 +6491,11 @@
       <c r="H141" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="142" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I141" s="4" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A142" s="5" t="s">
         <v>239</v>
       </c>
@@ -6071,8 +6518,11 @@
       <c r="H142" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="143" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I142" s="4" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A143" s="5" t="s">
         <v>151</v>
       </c>
@@ -6095,8 +6545,11 @@
       <c r="H143" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="144" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I143" s="4" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A144" s="5" t="s">
         <v>152</v>
       </c>
@@ -6119,8 +6572,11 @@
       <c r="H144" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="145" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I144" s="4" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A145" s="5" t="s">
         <v>153</v>
       </c>
@@ -6143,8 +6599,11 @@
       <c r="H145" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="146" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I145" s="4" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A146" s="5" t="s">
         <v>154</v>
       </c>
@@ -6167,8 +6626,11 @@
       <c r="H146" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="147" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I146" s="4" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="147" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A147" s="5" t="s">
         <v>155</v>
       </c>
@@ -6191,8 +6653,11 @@
       <c r="H147" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="148" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I147" s="4" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="148" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A148" s="5" t="s">
         <v>156</v>
       </c>
@@ -6215,8 +6680,11 @@
       <c r="H148" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="149" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I148" s="4" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="149" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A149" s="5" t="s">
         <v>157</v>
       </c>
@@ -6239,8 +6707,11 @@
       <c r="H149" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="150" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I149" s="4" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="150" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A150" s="5" t="s">
         <v>158</v>
       </c>
@@ -6263,8 +6734,11 @@
       <c r="H150" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="151" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I150" s="4" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="151" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A151" s="5" t="s">
         <v>159</v>
       </c>
@@ -6287,8 +6761,11 @@
       <c r="H151" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="152" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I151" s="4" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="152" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A152" s="5" t="s">
         <v>160</v>
       </c>
@@ -6311,8 +6788,11 @@
       <c r="H152" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="153" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I152" s="4" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="153" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A153" s="5" t="s">
         <v>161</v>
       </c>
@@ -6335,8 +6815,11 @@
       <c r="H153" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="154" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I153" s="4" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="154" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A154" s="5" t="s">
         <v>162</v>
       </c>
@@ -6359,8 +6842,11 @@
       <c r="H154" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="155" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I154" s="4" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="155" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A155" s="5" t="s">
         <v>163</v>
       </c>
@@ -6383,8 +6869,11 @@
       <c r="H155" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="156" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I155" s="4" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="156" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A156" s="7" t="s">
         <v>164</v>
       </c>
@@ -6407,8 +6896,11 @@
       <c r="H156" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="157" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I156" s="4" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="157" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A157" s="5" t="s">
         <v>165</v>
       </c>
@@ -6433,8 +6925,11 @@
       <c r="H157" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="158" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I157" s="4" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="158" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A158" s="5" t="s">
         <v>166</v>
       </c>
@@ -6459,8 +6954,11 @@
       <c r="H158" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="159" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I158" s="4" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A159" s="5" t="s">
         <v>167</v>
       </c>
@@ -6485,8 +6983,11 @@
       <c r="H159" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="160" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I159" s="4" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A160" s="5" t="s">
         <v>168</v>
       </c>
@@ -6511,8 +7012,11 @@
       <c r="H160" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="161" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I160" s="4" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="161" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A161" s="5" t="s">
         <v>169</v>
       </c>
@@ -6537,8 +7041,11 @@
       <c r="H161" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="162" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I161" s="4" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="162" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A162" s="5" t="s">
         <v>170</v>
       </c>
@@ -6563,8 +7070,11 @@
       <c r="H162" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="163" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I162" s="4" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="163" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A163" s="5" t="s">
         <v>171</v>
       </c>
@@ -6589,8 +7099,11 @@
       <c r="H163" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="164" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I163" s="4" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="164" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A164" s="5" t="s">
         <v>172</v>
       </c>
@@ -6615,8 +7128,11 @@
       <c r="H164" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="165" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I164" s="4" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="165" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A165" s="5" t="s">
         <v>241</v>
       </c>
@@ -6641,8 +7157,11 @@
       <c r="H165" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="166" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I165" s="4" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="166" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A166" s="5" t="s">
         <v>173</v>
       </c>
@@ -6667,8 +7186,11 @@
       <c r="H166" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="167" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I166" s="4" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="167" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A167" s="5" t="s">
         <v>174</v>
       </c>
@@ -6693,8 +7215,11 @@
       <c r="H167" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="168" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I167" s="4" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="168" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A168" s="5" t="s">
         <v>175</v>
       </c>
@@ -6719,8 +7244,11 @@
       <c r="H168" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="169" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I168" s="4" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="169" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A169" s="5" t="s">
         <v>176</v>
       </c>
@@ -6745,8 +7273,11 @@
       <c r="H169" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="170" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I169" s="4" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="170" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A170" s="7" t="s">
         <v>177</v>
       </c>
@@ -6771,8 +7302,11 @@
       <c r="H170" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="171" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I170" s="4" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="171" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A171" s="5" t="s">
         <v>178</v>
       </c>
@@ -6795,8 +7329,11 @@
       <c r="H171" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="172" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I171" s="4" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="172" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A172" s="5" t="s">
         <v>179</v>
       </c>
@@ -6819,8 +7356,11 @@
       <c r="H172" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="173" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I172" s="4" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="173" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A173" s="5" t="s">
         <v>180</v>
       </c>
@@ -6843,8 +7383,11 @@
       <c r="H173" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="174" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I173" s="4" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="174" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A174" s="5" t="s">
         <v>181</v>
       </c>
@@ -6867,8 +7410,11 @@
       <c r="H174" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="175" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I174" s="4" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="175" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A175" s="5" t="s">
         <v>182</v>
       </c>
@@ -6891,8 +7437,11 @@
       <c r="H175" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="176" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I175" s="4" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="176" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A176" s="5" t="s">
         <v>183</v>
       </c>
@@ -6915,8 +7464,11 @@
       <c r="H176" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="177" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I176" s="4" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="177" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A177" s="5" t="s">
         <v>184</v>
       </c>
@@ -6939,8 +7491,11 @@
       <c r="H177" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="178" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I177" s="4" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="178" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A178" s="5" t="s">
         <v>185</v>
       </c>
@@ -6963,8 +7518,11 @@
       <c r="H178" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="179" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I178" s="4" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="179" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A179" s="5" t="s">
         <v>186</v>
       </c>
@@ -6987,8 +7545,11 @@
       <c r="H179" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="180" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I179" s="4" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="180" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A180" s="5" t="s">
         <v>187</v>
       </c>
@@ -7011,8 +7572,11 @@
       <c r="H180" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="181" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I180" s="4" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="181" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A181" s="5" t="s">
         <v>188</v>
       </c>
@@ -7035,8 +7599,11 @@
       <c r="H181" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="182" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I181" s="4" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="182" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A182" s="5" t="s">
         <v>189</v>
       </c>
@@ -7059,8 +7626,11 @@
       <c r="H182" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="183" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I182" s="4" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="183" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A183" s="5" t="s">
         <v>190</v>
       </c>
@@ -7083,8 +7653,11 @@
       <c r="H183" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="184" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I183" s="4" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="184" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A184" s="7" t="s">
         <v>191</v>
       </c>
@@ -7107,8 +7680,11 @@
       <c r="H184" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="185" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I184" s="4" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="185" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A185" s="5" t="s">
         <v>192</v>
       </c>
@@ -7133,8 +7709,11 @@
       <c r="H185" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="186" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I185" s="4" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="186" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A186" s="5" t="s">
         <v>193</v>
       </c>
@@ -7159,8 +7738,11 @@
       <c r="H186" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="187" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I186" s="4" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="187" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A187" s="5" t="s">
         <v>194</v>
       </c>
@@ -7185,8 +7767,11 @@
       <c r="H187" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="188" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I187" s="4" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="188" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A188" s="5" t="s">
         <v>195</v>
       </c>
@@ -7211,8 +7796,11 @@
       <c r="H188" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="189" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I188" s="4" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="189" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A189" s="5" t="s">
         <v>196</v>
       </c>
@@ -7237,8 +7825,11 @@
       <c r="H189" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="190" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I189" s="4" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="190" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A190" s="5" t="s">
         <v>197</v>
       </c>
@@ -7263,8 +7854,11 @@
       <c r="H190" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="191" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I190" s="4" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="191" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A191" s="5" t="s">
         <v>198</v>
       </c>
@@ -7289,8 +7883,11 @@
       <c r="H191" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="192" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I191" s="4" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="192" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A192" s="5" t="s">
         <v>199</v>
       </c>
@@ -7315,8 +7912,11 @@
       <c r="H192" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="193" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I192" s="4" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="193" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A193" s="5" t="s">
         <v>200</v>
       </c>
@@ -7341,8 +7941,11 @@
       <c r="H193" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="194" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I193" s="4" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="194" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A194" s="5" t="s">
         <v>201</v>
       </c>
@@ -7367,8 +7970,11 @@
       <c r="H194" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="195" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I194" s="4" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="195" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A195" s="5" t="s">
         <v>202</v>
       </c>
@@ -7393,8 +7999,11 @@
       <c r="H195" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="196" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I195" s="4" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="196" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A196" s="5" t="s">
         <v>203</v>
       </c>
@@ -7419,8 +8028,11 @@
       <c r="H196" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="197" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I196" s="4" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="197" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A197" s="5" t="s">
         <v>204</v>
       </c>
@@ -7445,8 +8057,11 @@
       <c r="H197" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="198" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I197" s="4" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="198" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A198" s="7" t="s">
         <v>205</v>
       </c>
@@ -7471,8 +8086,11 @@
       <c r="H198" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="199" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I198" s="4" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="199" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A199" s="5" t="s">
         <v>206</v>
       </c>
@@ -7497,8 +8115,11 @@
       <c r="H199" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="200" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I199" s="4" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="200" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A200" s="5" t="s">
         <v>207</v>
       </c>
@@ -7523,8 +8144,11 @@
       <c r="H200" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="201" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I200" s="4" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="201" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A201" s="5" t="s">
         <v>208</v>
       </c>
@@ -7549,8 +8173,11 @@
       <c r="H201" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="202" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I201" s="4" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="202" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A202" s="5" t="s">
         <v>209</v>
       </c>
@@ -7575,8 +8202,11 @@
       <c r="H202" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="203" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I202" s="4" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="203" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A203" s="5" t="s">
         <v>210</v>
       </c>
@@ -7601,8 +8231,11 @@
       <c r="H203" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="204" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I203" s="4" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="204" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A204" s="5" t="s">
         <v>211</v>
       </c>
@@ -7627,8 +8260,11 @@
       <c r="H204" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="205" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I204" s="4" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="205" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A205" s="5" t="s">
         <v>212</v>
       </c>
@@ -7653,8 +8289,11 @@
       <c r="H205" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="206" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I205" s="4" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="206" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A206" s="5" t="s">
         <v>213</v>
       </c>
@@ -7679,8 +8318,11 @@
       <c r="H206" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="207" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I206" s="4" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="207" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A207" s="5" t="s">
         <v>214</v>
       </c>
@@ -7705,8 +8347,11 @@
       <c r="H207" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="208" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I207" s="4" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="208" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A208" s="5" t="s">
         <v>215</v>
       </c>
@@ -7731,8 +8376,11 @@
       <c r="H208" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="209" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I208" s="4" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="209" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A209" s="5" t="s">
         <v>216</v>
       </c>
@@ -7757,8 +8405,11 @@
       <c r="H209" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="210" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I209" s="4" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="210" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A210" s="5" t="s">
         <v>217</v>
       </c>
@@ -7783,8 +8434,11 @@
       <c r="H210" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="211" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I210" s="4" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="211" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A211" s="5" t="s">
         <v>218</v>
       </c>
@@ -7809,8 +8463,11 @@
       <c r="H211" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="212" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I211" s="4" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="212" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A212" s="7" t="s">
         <v>219</v>
       </c>
@@ -7835,8 +8492,11 @@
       <c r="H212" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="213" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I212" s="4" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="213" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A213" s="5" t="s">
         <v>220</v>
       </c>
@@ -7861,8 +8521,11 @@
       <c r="H213" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="214" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I213" s="4" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="214" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A214" s="5" t="s">
         <v>221</v>
       </c>
@@ -7887,8 +8550,11 @@
       <c r="H214" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="215" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I214" s="4" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="215" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A215" s="5" t="s">
         <v>222</v>
       </c>
@@ -7913,8 +8579,11 @@
       <c r="H215" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="216" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I215" s="4" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="216" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A216" s="5" t="s">
         <v>223</v>
       </c>
@@ -7939,8 +8608,11 @@
       <c r="H216" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="217" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I216" s="4" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="217" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A217" s="5" t="s">
         <v>224</v>
       </c>
@@ -7965,8 +8637,11 @@
       <c r="H217" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="218" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I217" s="4" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="218" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A218" s="5" t="s">
         <v>225</v>
       </c>
@@ -7991,8 +8666,11 @@
       <c r="H218" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="219" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I218" s="4" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="219" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A219" s="5" t="s">
         <v>226</v>
       </c>
@@ -8017,8 +8695,11 @@
       <c r="H219" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="220" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I219" s="4" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="220" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A220" s="5" t="s">
         <v>227</v>
       </c>
@@ -8043,8 +8724,11 @@
       <c r="H220" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="221" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I220" s="4" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="221" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A221" s="5" t="s">
         <v>228</v>
       </c>
@@ -8069,8 +8753,11 @@
       <c r="H221" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="222" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I221" s="11" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="222" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A222" s="5" t="s">
         <v>229</v>
       </c>
@@ -8095,8 +8782,11 @@
       <c r="H222" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="223" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I222" s="4" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="223" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A223" s="5" t="s">
         <v>230</v>
       </c>
@@ -8121,8 +8811,11 @@
       <c r="H223" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="224" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I223" s="4" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="224" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A224" s="5" t="s">
         <v>231</v>
       </c>
@@ -8147,8 +8840,11 @@
       <c r="H224" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="225" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I224" s="4" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="225" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A225" s="5" t="s">
         <v>232</v>
       </c>
@@ -8173,8 +8869,11 @@
       <c r="H225" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="226" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="I225" s="4" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="226" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A226" s="7" t="s">
         <v>233</v>
       </c>
@@ -8199,10 +8898,16 @@
       <c r="H226" t="b">
         <v>0</v>
       </c>
+      <c r="I226" s="4" t="s">
+        <v>693</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added mock data. Fixed query. Changed order of spec runner
</commit_message>
<xml_diff>
--- a/models/mock-data/FakeUsers.xlsx
+++ b/models/mock-data/FakeUsers.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="28800" yWindow="-1440" windowWidth="38400" windowHeight="21140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2143,12 +2143,18 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="7">
@@ -2231,7 +2237,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -2250,21 +2256,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2558,10 +2555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I226"/>
+  <dimension ref="A1:J226"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="J82" sqref="J82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2574,7 +2571,7 @@
     <col min="9" max="9" width="18.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2603,7 +2600,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -2632,7 +2629,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
@@ -2661,7 +2658,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
@@ -2689,8 +2686,9 @@
       <c r="I4" s="4" t="s">
         <v>477</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J4" s="14"/>
+    </row>
+    <row r="5" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
@@ -2718,8 +2716,9 @@
       <c r="I5" s="4" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J5" s="14"/>
+    </row>
+    <row r="6" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>473</v>
       </c>
@@ -2748,7 +2747,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>11</v>
       </c>
@@ -2777,7 +2776,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>12</v>
       </c>
@@ -2806,7 +2805,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>13</v>
       </c>
@@ -2835,7 +2834,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>14</v>
       </c>
@@ -2864,7 +2863,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>15</v>
       </c>
@@ -2893,7 +2892,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>16</v>
       </c>
@@ -2922,7 +2921,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>17</v>
       </c>
@@ -2951,7 +2950,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>18</v>
       </c>
@@ -2980,7 +2979,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>19</v>
       </c>
@@ -2997,7 +2996,7 @@
         <v>487</v>
       </c>
       <c r="F15" s="13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G15" t="b">
         <v>0</v>
@@ -3009,7 +3008,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>20</v>
       </c>
@@ -3956,7 +3955,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
         <v>57</v>
       </c>
@@ -3983,7 +3982,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
         <v>58</v>
       </c>
@@ -4010,7 +4009,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
         <v>59</v>
       </c>
@@ -4037,7 +4036,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
         <v>60</v>
       </c>
@@ -4064,7 +4063,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
         <v>61</v>
       </c>
@@ -4091,7 +4090,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
         <v>62</v>
       </c>
@@ -4118,7 +4117,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
         <v>63</v>
       </c>
@@ -4145,7 +4144,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
         <v>64</v>
       </c>
@@ -4172,7 +4171,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
         <v>65</v>
       </c>
@@ -4187,7 +4186,7 @@
         <v>528</v>
       </c>
       <c r="F57" s="13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G57" t="b">
         <v>0</v>
@@ -4199,7 +4198,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
         <v>66</v>
       </c>
@@ -4228,7 +4227,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
         <v>69</v>
       </c>
@@ -4257,7 +4256,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
         <v>70</v>
       </c>
@@ -4285,8 +4284,9 @@
       <c r="I60" s="4" t="s">
         <v>531</v>
       </c>
-    </row>
-    <row r="61" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J60" s="14"/>
+    </row>
+    <row r="61" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
         <v>71</v>
       </c>
@@ -4315,7 +4315,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
         <v>72</v>
       </c>
@@ -4344,7 +4344,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
         <v>73</v>
       </c>
@@ -4373,7 +4373,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
         <v>234</v>
       </c>
@@ -4564,7 +4564,7 @@
         <v>541</v>
       </c>
       <c r="F70" s="13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G70" t="b">
         <v>0</v>
@@ -4848,7 +4848,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="81" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
         <v>90</v>
       </c>
@@ -4874,8 +4874,9 @@
       <c r="I81" s="4" t="s">
         <v>551</v>
       </c>
-    </row>
-    <row r="82" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J81" s="14"/>
+    </row>
+    <row r="82" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
         <v>91</v>
       </c>
@@ -4901,8 +4902,9 @@
       <c r="I82" s="4" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="83" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J82" s="14"/>
+    </row>
+    <row r="83" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
         <v>92</v>
       </c>
@@ -4929,7 +4931,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="84" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
         <v>93</v>
       </c>
@@ -4944,7 +4946,7 @@
         <v>554</v>
       </c>
       <c r="F84" s="13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G84" t="b">
         <v>0</v>
@@ -4956,7 +4958,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="85" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A85" s="7" t="s">
         <v>94</v>
       </c>
@@ -4983,7 +4985,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="86" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
         <v>95</v>
       </c>
@@ -5010,7 +5012,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="87" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
         <v>97</v>
       </c>
@@ -5037,7 +5039,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="88" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
         <v>98</v>
       </c>
@@ -5063,8 +5065,9 @@
       <c r="I88" s="4" t="s">
         <v>558</v>
       </c>
-    </row>
-    <row r="89" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J88" s="14"/>
+    </row>
+    <row r="89" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
         <v>99</v>
       </c>
@@ -5091,7 +5094,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="90" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
         <v>100</v>
       </c>
@@ -5118,7 +5121,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="91" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
         <v>101</v>
       </c>
@@ -5145,7 +5148,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="92" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
         <v>102</v>
       </c>
@@ -5172,7 +5175,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="93" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
         <v>103</v>
       </c>
@@ -5199,7 +5202,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="94" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
         <v>104</v>
       </c>
@@ -5226,7 +5229,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="95" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
         <v>105</v>
       </c>
@@ -5253,7 +5256,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="96" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
         <v>106</v>
       </c>
@@ -5280,7 +5283,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="97" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
         <v>107</v>
       </c>
@@ -5307,7 +5310,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="98" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
         <v>236</v>
       </c>
@@ -5322,7 +5325,7 @@
         <v>568</v>
       </c>
       <c r="F98" s="13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G98" t="b">
         <v>0</v>
@@ -5334,7 +5337,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="99" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A99" s="7" t="s">
         <v>108</v>
       </c>
@@ -5361,7 +5364,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="100" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
         <v>109</v>
       </c>
@@ -5388,7 +5391,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="101" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
         <v>237</v>
       </c>
@@ -5415,7 +5418,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="102" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
         <v>111</v>
       </c>
@@ -5442,7 +5445,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="103" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
         <v>112</v>
       </c>
@@ -5469,7 +5472,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="104" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
         <v>114</v>
       </c>
@@ -5496,7 +5499,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="105" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
         <v>115</v>
       </c>
@@ -5523,7 +5526,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="106" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
         <v>116</v>
       </c>
@@ -5550,7 +5553,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="107" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
         <v>117</v>
       </c>
@@ -5577,7 +5580,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="108" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
         <v>118</v>
       </c>
@@ -5604,7 +5607,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="109" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
         <v>119</v>
       </c>
@@ -5631,7 +5634,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="110" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
         <v>120</v>
       </c>
@@ -5657,8 +5660,9 @@
       <c r="I110" s="4" t="s">
         <v>580</v>
       </c>
-    </row>
-    <row r="111" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J110" s="14"/>
+    </row>
+    <row r="111" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
         <v>121</v>
       </c>
@@ -5685,7 +5689,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="112" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
         <v>122</v>
       </c>
@@ -5700,7 +5704,7 @@
         <v>582</v>
       </c>
       <c r="F112" s="12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G112" t="b">
         <v>0</v>
@@ -5712,7 +5716,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="113" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A113" s="5" t="s">
         <v>123</v>
       </c>
@@ -5739,7 +5743,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="114" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A114" s="7" t="s">
         <v>124</v>
       </c>
@@ -5766,7 +5770,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="115" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
         <v>125</v>
       </c>
@@ -5793,7 +5797,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="116" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
         <v>127</v>
       </c>
@@ -5820,7 +5824,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="117" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="s">
         <v>128</v>
       </c>
@@ -5846,8 +5850,9 @@
       <c r="I117" s="4" t="s">
         <v>587</v>
       </c>
-    </row>
-    <row r="118" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J117" s="14"/>
+    </row>
+    <row r="118" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
         <v>238</v>
       </c>
@@ -5874,7 +5879,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="119" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A119" s="5" t="s">
         <v>129</v>
       </c>
@@ -5901,7 +5906,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="120" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A120" s="5" t="s">
         <v>130</v>
       </c>
@@ -5928,7 +5933,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="121" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="s">
         <v>131</v>
       </c>
@@ -5955,7 +5960,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="122" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A122" s="5" t="s">
         <v>132</v>
       </c>
@@ -5982,7 +5987,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="123" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
         <v>133</v>
       </c>
@@ -6009,7 +6014,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="124" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
         <v>134</v>
       </c>
@@ -6036,7 +6041,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="125" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
         <v>135</v>
       </c>
@@ -6063,7 +6068,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="126" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
         <v>136</v>
       </c>
@@ -6090,7 +6095,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="127" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A127" s="5" t="s">
         <v>137</v>
       </c>
@@ -6117,7 +6122,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="128" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A128" s="7" t="s">
         <v>138</v>
       </c>
@@ -6144,7 +6149,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="129" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A129" s="5" t="s">
         <v>139</v>
       </c>
@@ -6171,7 +6176,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="130" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
         <v>140</v>
       </c>
@@ -6197,8 +6202,9 @@
       <c r="I130" s="4" t="s">
         <v>599</v>
       </c>
-    </row>
-    <row r="131" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J130" s="14"/>
+    </row>
+    <row r="131" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A131" s="5" t="s">
         <v>141</v>
       </c>
@@ -6225,7 +6231,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="132" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A132" s="5" t="s">
         <v>240</v>
       </c>
@@ -6252,7 +6258,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="133" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A133" s="5" t="s">
         <v>142</v>
       </c>
@@ -6279,7 +6285,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="134" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A134" s="5" t="s">
         <v>143</v>
       </c>
@@ -6306,7 +6312,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="135" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A135" s="5" t="s">
         <v>144</v>
       </c>
@@ -6333,7 +6339,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="136" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A136" s="5" t="s">
         <v>145</v>
       </c>
@@ -6360,7 +6366,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="137" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A137" s="5" t="s">
         <v>146</v>
       </c>
@@ -6387,7 +6393,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="138" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A138" s="5" t="s">
         <v>147</v>
       </c>
@@ -6414,7 +6420,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="139" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A139" s="5" t="s">
         <v>148</v>
       </c>
@@ -6441,7 +6447,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="140" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A140" s="5" t="s">
         <v>149</v>
       </c>
@@ -6468,7 +6474,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="141" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A141" s="5" t="s">
         <v>150</v>
       </c>
@@ -6495,7 +6501,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="142" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A142" s="5" t="s">
         <v>239</v>
       </c>
@@ -6522,7 +6528,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="143" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A143" s="5" t="s">
         <v>151</v>
       </c>
@@ -6549,7 +6555,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="144" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A144" s="5" t="s">
         <v>152</v>
       </c>
@@ -6576,7 +6582,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="145" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A145" s="5" t="s">
         <v>153</v>
       </c>
@@ -6603,7 +6609,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="146" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A146" s="5" t="s">
         <v>154</v>
       </c>
@@ -6630,7 +6636,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="147" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A147" s="5" t="s">
         <v>155</v>
       </c>
@@ -6657,7 +6663,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="148" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A148" s="5" t="s">
         <v>156</v>
       </c>
@@ -6684,7 +6690,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="149" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A149" s="5" t="s">
         <v>157</v>
       </c>
@@ -6711,7 +6717,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="150" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A150" s="5" t="s">
         <v>158</v>
       </c>
@@ -6737,8 +6743,9 @@
       <c r="I150" s="4" t="s">
         <v>619</v>
       </c>
-    </row>
-    <row r="151" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J150" s="14"/>
+    </row>
+    <row r="151" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A151" s="5" t="s">
         <v>159</v>
       </c>
@@ -6765,7 +6772,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="152" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A152" s="5" t="s">
         <v>160</v>
       </c>
@@ -6792,7 +6799,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="153" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A153" s="5" t="s">
         <v>161</v>
       </c>
@@ -6819,7 +6826,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="154" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A154" s="5" t="s">
         <v>162</v>
       </c>
@@ -6846,7 +6853,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="155" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A155" s="5" t="s">
         <v>163</v>
       </c>
@@ -6873,7 +6880,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="156" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A156" s="7" t="s">
         <v>164</v>
       </c>
@@ -6900,7 +6907,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="157" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A157" s="5" t="s">
         <v>165</v>
       </c>
@@ -6929,7 +6936,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="158" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A158" s="5" t="s">
         <v>166</v>
       </c>
@@ -6958,7 +6965,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="159" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A159" s="5" t="s">
         <v>167</v>
       </c>
@@ -6986,8 +6993,9 @@
       <c r="I159" s="4" t="s">
         <v>628</v>
       </c>
-    </row>
-    <row r="160" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J159" s="14"/>
+    </row>
+    <row r="160" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A160" s="5" t="s">
         <v>168</v>
       </c>
@@ -7016,7 +7024,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="161" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A161" s="5" t="s">
         <v>169</v>
       </c>
@@ -7045,7 +7053,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="162" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A162" s="5" t="s">
         <v>170</v>
       </c>
@@ -7074,7 +7082,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="163" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A163" s="5" t="s">
         <v>171</v>
       </c>
@@ -7103,7 +7111,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="164" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A164" s="5" t="s">
         <v>172</v>
       </c>
@@ -7132,7 +7140,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="165" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A165" s="5" t="s">
         <v>241</v>
       </c>
@@ -7161,7 +7169,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="166" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A166" s="5" t="s">
         <v>173</v>
       </c>
@@ -7190,7 +7198,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="167" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A167" s="5" t="s">
         <v>174</v>
       </c>
@@ -7219,7 +7227,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="168" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A168" s="5" t="s">
         <v>175</v>
       </c>
@@ -7248,7 +7256,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="169" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A169" s="5" t="s">
         <v>176</v>
       </c>
@@ -7277,7 +7285,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="170" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A170" s="7" t="s">
         <v>177</v>
       </c>
@@ -7306,7 +7314,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="171" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A171" s="5" t="s">
         <v>178</v>
       </c>
@@ -7333,7 +7341,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="172" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A172" s="5" t="s">
         <v>179</v>
       </c>
@@ -7359,8 +7367,9 @@
       <c r="I172" s="4" t="s">
         <v>640</v>
       </c>
-    </row>
-    <row r="173" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J172" s="14"/>
+    </row>
+    <row r="173" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A173" s="5" t="s">
         <v>180</v>
       </c>
@@ -7387,7 +7396,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="174" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A174" s="5" t="s">
         <v>181</v>
       </c>
@@ -7413,8 +7422,9 @@
       <c r="I174" s="4" t="s">
         <v>642</v>
       </c>
-    </row>
-    <row r="175" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J174" s="14"/>
+    </row>
+    <row r="175" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A175" s="5" t="s">
         <v>182</v>
       </c>
@@ -7441,7 +7451,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="176" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A176" s="5" t="s">
         <v>183</v>
       </c>
@@ -7672,7 +7682,7 @@
         <v>652</v>
       </c>
       <c r="F184" s="13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G184" t="b">
         <v>0</v>
@@ -7916,7 +7926,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="193" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A193" s="5" t="s">
         <v>200</v>
       </c>
@@ -7945,7 +7955,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="194" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A194" s="5" t="s">
         <v>201</v>
       </c>
@@ -7973,8 +7983,9 @@
       <c r="I194" s="4" t="s">
         <v>662</v>
       </c>
-    </row>
-    <row r="195" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J194" s="14"/>
+    </row>
+    <row r="195" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A195" s="5" t="s">
         <v>202</v>
       </c>
@@ -8003,7 +8014,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="196" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A196" s="5" t="s">
         <v>203</v>
       </c>
@@ -8032,7 +8043,7 @@
         <v>664</v>
       </c>
     </row>
-    <row r="197" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A197" s="5" t="s">
         <v>204</v>
       </c>
@@ -8061,7 +8072,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="198" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A198" s="7" t="s">
         <v>205</v>
       </c>
@@ -8078,7 +8089,7 @@
         <v>666</v>
       </c>
       <c r="F198" s="13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G198" t="b">
         <v>0</v>
@@ -8090,7 +8101,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="199" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A199" s="5" t="s">
         <v>206</v>
       </c>
@@ -8119,7 +8130,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="200" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A200" s="5" t="s">
         <v>207</v>
       </c>
@@ -8148,7 +8159,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="201" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A201" s="5" t="s">
         <v>208</v>
       </c>
@@ -8177,7 +8188,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="202" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A202" s="5" t="s">
         <v>209</v>
       </c>
@@ -8206,7 +8217,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="203" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A203" s="5" t="s">
         <v>210</v>
       </c>
@@ -8235,7 +8246,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="204" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A204" s="5" t="s">
         <v>211</v>
       </c>
@@ -8264,7 +8275,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="205" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A205" s="5" t="s">
         <v>212</v>
       </c>
@@ -8293,7 +8304,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="206" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A206" s="5" t="s">
         <v>213</v>
       </c>
@@ -8322,7 +8333,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="207" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A207" s="5" t="s">
         <v>214</v>
       </c>
@@ -8351,7 +8362,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="208" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A208" s="5" t="s">
         <v>215</v>
       </c>
@@ -8380,7 +8391,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="209" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A209" s="5" t="s">
         <v>216</v>
       </c>
@@ -8409,7 +8420,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="210" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A210" s="5" t="s">
         <v>217</v>
       </c>
@@ -8438,7 +8449,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="211" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A211" s="5" t="s">
         <v>218</v>
       </c>
@@ -8467,7 +8478,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="212" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A212" s="7" t="s">
         <v>219</v>
       </c>
@@ -8496,7 +8507,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="213" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A213" s="5" t="s">
         <v>220</v>
       </c>
@@ -8525,7 +8536,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="214" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A214" s="5" t="s">
         <v>221</v>
       </c>
@@ -8554,7 +8565,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="215" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A215" s="5" t="s">
         <v>222</v>
       </c>
@@ -8583,7 +8594,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="216" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A216" s="5" t="s">
         <v>223</v>
       </c>
@@ -8611,8 +8622,9 @@
       <c r="I216" s="4" t="s">
         <v>683</v>
       </c>
-    </row>
-    <row r="217" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="J216" s="14"/>
+    </row>
+    <row r="217" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A217" s="5" t="s">
         <v>224</v>
       </c>
@@ -8641,7 +8653,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="218" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A218" s="5" t="s">
         <v>225</v>
       </c>
@@ -8670,7 +8682,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="219" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A219" s="5" t="s">
         <v>226</v>
       </c>
@@ -8699,7 +8711,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="220" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A220" s="5" t="s">
         <v>227</v>
       </c>
@@ -8728,7 +8740,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="221" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A221" s="5" t="s">
         <v>228</v>
       </c>
@@ -8757,7 +8769,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="222" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A222" s="5" t="s">
         <v>229</v>
       </c>
@@ -8786,7 +8798,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="223" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A223" s="5" t="s">
         <v>230</v>
       </c>
@@ -8815,7 +8827,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="224" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A224" s="5" t="s">
         <v>231</v>
       </c>
@@ -8890,7 +8902,7 @@
         <v>693</v>
       </c>
       <c r="F226" s="13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G226" t="b">
         <v>0</v>
@@ -8904,10 +8916,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>